<commit_message>
Added display for productions of transformers
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Total Cost</t>
   </si>
@@ -31,13 +31,25 @@
     <t>RefineryProduction</t>
   </si>
   <si>
+    <t>Refinery-gasoline</t>
+  </si>
+  <si>
     <t>MtGProduction</t>
   </si>
   <si>
+    <t>MtG-gasoline</t>
+  </si>
+  <si>
     <t>GtkmProduction</t>
   </si>
   <si>
+    <t>Gtkm-km</t>
+  </si>
+  <si>
     <t>B2gasProduction</t>
+  </si>
+  <si>
+    <t>B2gas-gasoline</t>
   </si>
   <si>
     <t>GasHubUsage</t>
@@ -404,13 +416,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:16">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -444,8 +456,20 @@
       <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:16">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -465,21 +489,33 @@
         <v>508.1967213114755</v>
       </c>
       <c r="G2">
+        <v>508.1967213114755</v>
+      </c>
+      <c r="H2">
         <v>1991.803278688524</v>
       </c>
-      <c r="H2">
+      <c r="I2">
+        <v>1991.803278688524</v>
+      </c>
+      <c r="J2">
         <v>1000</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>2500</v>
       </c>
       <c r="K2">
         <v>1000</v>
       </c>
       <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>2500</v>
+      </c>
+      <c r="O2">
+        <v>1000</v>
+      </c>
+      <c r="P2">
         <v>1000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added CO2 location based cost equations
Added the first version of our capex, direct and indirect opex equations
based on potential CO2 locations for H2 fuel plants
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -103,19 +103,19 @@
     <t>DieselHubUsage</t>
   </si>
   <si>
+    <t>tkm-N1Usage</t>
+  </si>
+  <si>
+    <t>tkm-N3Usage</t>
+  </si>
+  <si>
+    <t>tkm-N2Usage</t>
+  </si>
+  <si>
+    <t>pkmUsage</t>
+  </si>
+  <si>
     <t>tkm-SZMUsage</t>
-  </si>
-  <si>
-    <t>tkm-N3Usage</t>
-  </si>
-  <si>
-    <t>tkm-N2Usage</t>
-  </si>
-  <si>
-    <t>pkmUsage</t>
-  </si>
-  <si>
-    <t>tkm-N1Usage</t>
   </si>
 </sst>
 </file>
@@ -675,7 +675,7 @@
         <v>1255.909646477429</v>
       </c>
       <c r="AE2">
-        <v>414.5</v>
+        <v>7.5</v>
       </c>
       <c r="AF2">
         <v>130.3</v>
@@ -687,7 +687,7 @@
         <v>858</v>
       </c>
       <c r="AI2">
-        <v>7.5</v>
+        <v>414.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Have to commit to pull, ignore this
See title
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -103,19 +103,19 @@
     <t>DieselHubUsage</t>
   </si>
   <si>
+    <t>tkm-N3Usage</t>
+  </si>
+  <si>
+    <t>pkmUsage</t>
+  </si>
+  <si>
+    <t>tkm-SZMUsage</t>
+  </si>
+  <si>
+    <t>tkm-N2Usage</t>
+  </si>
+  <si>
     <t>tkm-N1Usage</t>
-  </si>
-  <si>
-    <t>tkm-N3Usage</t>
-  </si>
-  <si>
-    <t>tkm-N2Usage</t>
-  </si>
-  <si>
-    <t>pkmUsage</t>
-  </si>
-  <si>
-    <t>tkm-SZMUsage</t>
   </si>
 </sst>
 </file>
@@ -675,19 +675,19 @@
         <v>1255.909646477429</v>
       </c>
       <c r="AE2">
+        <v>130.3</v>
+      </c>
+      <c r="AF2">
+        <v>858</v>
+      </c>
+      <c r="AG2">
+        <v>414.5</v>
+      </c>
+      <c r="AH2">
+        <v>24.2</v>
+      </c>
+      <c r="AI2">
         <v>7.5</v>
-      </c>
-      <c r="AF2">
-        <v>130.3</v>
-      </c>
-      <c r="AG2">
-        <v>24.2</v>
-      </c>
-      <c r="AH2">
-        <v>858</v>
-      </c>
-      <c r="AI2">
-        <v>414.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Required to commit to pull
Ignore this.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -103,19 +103,19 @@
     <t>DieselHubUsage</t>
   </si>
   <si>
+    <t>pkmUsage</t>
+  </si>
+  <si>
     <t>tkm-SZMUsage</t>
   </si>
   <si>
+    <t>tkm-N1Usage</t>
+  </si>
+  <si>
+    <t>tkm-N2Usage</t>
+  </si>
+  <si>
     <t>tkm-N3Usage</t>
-  </si>
-  <si>
-    <t>tkm-N2Usage</t>
-  </si>
-  <si>
-    <t>pkmUsage</t>
-  </si>
-  <si>
-    <t>tkm-N1Usage</t>
   </si>
 </sst>
 </file>
@@ -588,16 +588,16 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>37.65025520601402</v>
+        <v>42.50739806315688</v>
       </c>
       <c r="C2">
         <v>1190.475409836065</v>
       </c>
       <c r="D2">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>354.9100221530673</v>
+        <v>612.0528792959246</v>
       </c>
       <c r="F2">
         <v>1107.142131147541</v>
@@ -606,13 +606,13 @@
         <v>365.3569032786885</v>
       </c>
       <c r="H2">
-        <v>741.7852278688525</v>
+        <v>741.7852278688524</v>
       </c>
       <c r="I2">
-        <v>216</v>
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>216</v>
+        <v>0</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -621,10 +621,10 @@
         <v>0</v>
       </c>
       <c r="M2">
-        <v>298.1244186085765</v>
+        <v>514.1244186085767</v>
       </c>
       <c r="N2">
-        <v>298.1244186085765</v>
+        <v>514.1244186085767</v>
       </c>
       <c r="O2">
         <v>0</v>
@@ -636,7 +636,7 @@
         <v>288.4396604831751</v>
       </c>
       <c r="R2">
-        <v>288.4396604831752</v>
+        <v>288.4396604831751</v>
       </c>
       <c r="S2">
         <v>569.5603395168248</v>
@@ -675,19 +675,19 @@
         <v>1255.909646477429</v>
       </c>
       <c r="AE2">
+        <v>858</v>
+      </c>
+      <c r="AF2">
         <v>414.5</v>
       </c>
-      <c r="AF2">
+      <c r="AG2">
+        <v>7.5</v>
+      </c>
+      <c r="AH2">
+        <v>24.2</v>
+      </c>
+      <c r="AI2">
         <v>130.3</v>
-      </c>
-      <c r="AG2">
-        <v>24.2</v>
-      </c>
-      <c r="AH2">
-        <v>858</v>
-      </c>
-      <c r="AI2">
-        <v>7.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added co2 output and fixed max
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -14,11 +14,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Total Cost</t>
   </si>
   <si>
+    <t>CO2</t>
+  </si>
+  <si>
     <t>crudeoil</t>
   </si>
   <si>
@@ -103,19 +106,19 @@
     <t>DieselHubUsage</t>
   </si>
   <si>
+    <t>tkm-SZMUsage</t>
+  </si>
+  <si>
     <t>tkm-N2Usage</t>
   </si>
   <si>
+    <t>tkm-N1Usage</t>
+  </si>
+  <si>
+    <t>pkmUsage</t>
+  </si>
+  <si>
     <t>tkm-N3Usage</t>
-  </si>
-  <si>
-    <t>tkm-N1Usage</t>
-  </si>
-  <si>
-    <t>pkmUsage</t>
-  </si>
-  <si>
-    <t>tkm-SZMUsage</t>
   </si>
 </sst>
 </file>
@@ -473,13 +476,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AI2"/>
+  <dimension ref="A1:AJ2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:36">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -582,8 +585,11 @@
       <c r="AI1" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="AJ1" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="2" spans="1:35">
+    <row r="2" spans="1:36">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -591,26 +597,26 @@
         <v>42.50739806315688</v>
       </c>
       <c r="C2">
+        <v>87.14279999999999</v>
+      </c>
+      <c r="D2">
         <v>1190.475409836065</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
       <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
         <v>612.0528792959244</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>1107.142131147541</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>365.3569032786885</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>741.7852278688525</v>
       </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
       <c r="J2">
         <v>0</v>
       </c>
@@ -621,73 +627,76 @@
         <v>0</v>
       </c>
       <c r="M2">
-        <v>514.1244186085765</v>
+        <v>0</v>
       </c>
       <c r="N2">
         <v>514.1244186085765</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>514.1244186085765</v>
       </c>
       <c r="P2">
         <v>0</v>
       </c>
       <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
         <v>288.4396604831751</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>288.4396604831752</v>
-      </c>
-      <c r="S2">
-        <v>569.5603395168248</v>
       </c>
       <c r="T2">
         <v>569.5603395168248</v>
       </c>
       <c r="U2">
-        <v>7.5</v>
+        <v>569.5603395168248</v>
       </c>
       <c r="V2">
         <v>7.5</v>
       </c>
       <c r="W2">
-        <v>24.2</v>
+        <v>7.5</v>
       </c>
       <c r="X2">
         <v>24.2</v>
       </c>
       <c r="Y2">
-        <v>130.3</v>
+        <v>24.2</v>
       </c>
       <c r="Z2">
         <v>130.3</v>
       </c>
       <c r="AA2">
-        <v>414.5</v>
+        <v>130.3</v>
       </c>
       <c r="AB2">
         <v>414.5</v>
       </c>
       <c r="AC2">
+        <v>414.5</v>
+      </c>
+      <c r="AD2">
         <v>365.3569032786885</v>
       </c>
-      <c r="AD2">
+      <c r="AE2">
         <v>1255.909646477429</v>
       </c>
-      <c r="AE2">
+      <c r="AF2">
+        <v>414.5</v>
+      </c>
+      <c r="AG2">
         <v>24.2</v>
       </c>
-      <c r="AF2">
+      <c r="AH2">
+        <v>7.5</v>
+      </c>
+      <c r="AI2">
+        <v>858</v>
+      </c>
+      <c r="AJ2">
         <v>130.3</v>
-      </c>
-      <c r="AG2">
-        <v>7.5</v>
-      </c>
-      <c r="AH2">
-        <v>858</v>
-      </c>
-      <c r="AI2">
-        <v>414.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Direct Opex Function
Direct opex function for CO2 locations should now use MJ of fuel, not
kgs
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -106,16 +106,16 @@
     <t>DieselHubUsage</t>
   </si>
   <si>
+    <t>tkm-N1Usage</t>
+  </si>
+  <si>
+    <t>pkmUsage</t>
+  </si>
+  <si>
     <t>tkm-SZMUsage</t>
   </si>
   <si>
     <t>tkm-N2Usage</t>
-  </si>
-  <si>
-    <t>tkm-N1Usage</t>
-  </si>
-  <si>
-    <t>pkmUsage</t>
   </si>
   <si>
     <t>tkm-N3Usage</t>
@@ -684,16 +684,16 @@
         <v>1255.909646477429</v>
       </c>
       <c r="AF2">
+        <v>7.5</v>
+      </c>
+      <c r="AG2">
+        <v>858</v>
+      </c>
+      <c r="AH2">
         <v>414.5</v>
       </c>
-      <c r="AG2">
+      <c r="AI2">
         <v>24.2</v>
-      </c>
-      <c r="AH2">
-        <v>7.5</v>
-      </c>
-      <c r="AI2">
-        <v>858</v>
       </c>
       <c r="AJ2">
         <v>130.3</v>

</xml_diff>

<commit_message>
Changed CO2 Plant Scale to GW
Testing an idea to fix range issues, converting CO2 location capacities
from MW to GW. Cost isn't swapped yet, so the values aren't right, but
it is at least sort of working.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -106,19 +106,19 @@
     <t>DieselHubUsage</t>
   </si>
   <si>
+    <t>pkmUsage</t>
+  </si>
+  <si>
+    <t>tkm-N1Usage</t>
+  </si>
+  <si>
+    <t>tkm-N2Usage</t>
+  </si>
+  <si>
+    <t>tkm-SZMUsage</t>
+  </si>
+  <si>
     <t>tkm-N3Usage</t>
-  </si>
-  <si>
-    <t>tkm-N2Usage</t>
-  </si>
-  <si>
-    <t>tkm-SZMUsage</t>
-  </si>
-  <si>
-    <t>pkmUsage</t>
-  </si>
-  <si>
-    <t>tkm-N1Usage</t>
   </si>
 </sst>
 </file>
@@ -594,7 +594,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>42.50739806315688</v>
+        <v>42.5073980631569</v>
       </c>
       <c r="C2">
         <v>87.14279999999999</v>
@@ -606,7 +606,7 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>612.0528792959244</v>
+        <v>612.0528792959249</v>
       </c>
       <c r="G2">
         <v>1107.142131147541</v>
@@ -630,10 +630,10 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>514.1244186085765</v>
+        <v>514.1244186085769</v>
       </c>
       <c r="O2">
-        <v>514.1244186085765</v>
+        <v>514.1244186085769</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -648,7 +648,7 @@
         <v>288.4396604831752</v>
       </c>
       <c r="T2">
-        <v>569.5603395168248</v>
+        <v>569.5603395168249</v>
       </c>
       <c r="U2">
         <v>569.5603395168248</v>
@@ -684,19 +684,19 @@
         <v>1255.909646477429</v>
       </c>
       <c r="AF2">
+        <v>858</v>
+      </c>
+      <c r="AG2">
+        <v>7.5</v>
+      </c>
+      <c r="AH2">
+        <v>24.2</v>
+      </c>
+      <c r="AI2">
+        <v>414.5</v>
+      </c>
+      <c r="AJ2">
         <v>130.3</v>
-      </c>
-      <c r="AG2">
-        <v>24.2</v>
-      </c>
-      <c r="AH2">
-        <v>414.5</v>
-      </c>
-      <c r="AI2">
-        <v>858</v>
-      </c>
-      <c r="AJ2">
-        <v>7.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added CO2 Location to Output
The output spreadsheet now contains a second sheet which displays
information pertaining to those CO2 locations which are in use. This
includes name, postal code, amount, and process.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -7,14 +7,15 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="FacilityInfo" sheetId="1" r:id="rId1"/>
+    <sheet name="CO2LocationInfo" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Total Cost</t>
   </si>
@@ -106,22 +107,37 @@
     <t>DieselHubUsage</t>
   </si>
   <si>
+    <t>tkm-N3Usage</t>
+  </si>
+  <si>
+    <t>tkm-N1Usage</t>
+  </si>
+  <si>
+    <t>tkm-N2Usage</t>
+  </si>
+  <si>
     <t>pkmUsage</t>
   </si>
   <si>
-    <t>tkm-N1Usage</t>
-  </si>
-  <si>
-    <t>tkm-N2Usage</t>
-  </si>
-  <si>
-    <t>tkm-N3Usage</t>
-  </si>
-  <si>
     <t>tkm-SZMUsage</t>
   </si>
   <si>
-    <t>BASF Schwarzheide GmbH</t>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Postal Code</t>
+  </si>
+  <si>
+    <t>Amount Used</t>
+  </si>
+  <si>
+    <t>Process Used</t>
+  </si>
+  <si>
+    <t>VERA Klärschlammverbrennung GmbH</t>
+  </si>
+  <si>
+    <t>MtD</t>
   </si>
 </sst>
 </file>
@@ -479,13 +495,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK3"/>
+  <dimension ref="A1:AJ2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:36">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -591,16 +607,13 @@
       <c r="AJ1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:37">
+    </row>
+    <row r="2" spans="1:36">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>60754.97540209295</v>
+        <v>63544.75555102103</v>
       </c>
       <c r="C2">
         <v>87.14279999999999</v>
@@ -612,7 +625,7 @@
         <v>400</v>
       </c>
       <c r="F2">
-        <v>1214701.412959892</v>
+        <v>1213426.338593582</v>
       </c>
       <c r="G2">
         <v>1107.142131147541</v>
@@ -636,28 +649,28 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>999999</v>
+        <v>1019278.124418609</v>
       </c>
       <c r="O2">
-        <v>999999</v>
+        <v>1019278.124418609</v>
       </c>
       <c r="P2">
-        <v>20350.18688630918</v>
+        <v>0</v>
       </c>
       <c r="Q2">
-        <v>20350.18688630918</v>
+        <v>0</v>
       </c>
       <c r="R2">
-        <v>16354.37667599064</v>
+        <v>288.4396604831751</v>
       </c>
       <c r="S2">
-        <v>16354.37667599064</v>
+        <v>288.4396604831563</v>
       </c>
       <c r="T2">
-        <v>833653.6233240096</v>
+        <v>849719.5603395168</v>
       </c>
       <c r="U2">
-        <v>833653.6233240094</v>
+        <v>849719.5603395168</v>
       </c>
       <c r="V2">
         <v>7.5</v>
@@ -684,13 +697,13 @@
         <v>414.5</v>
       </c>
       <c r="AD2">
-        <v>20715.54378958815</v>
+        <v>365.3569032786885</v>
       </c>
       <c r="AE2">
-        <v>1000956.785227869</v>
+        <v>1020235.909646478</v>
       </c>
       <c r="AF2">
-        <v>850008</v>
+        <v>130.3</v>
       </c>
       <c r="AG2">
         <v>7.5</v>
@@ -699,18 +712,1770 @@
         <v>24.2</v>
       </c>
       <c r="AI2">
-        <v>130.3</v>
+        <v>850008</v>
       </c>
       <c r="AJ2">
         <v>414.5</v>
       </c>
     </row>
-    <row r="3" spans="1:37">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E158"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2">
+        <v>20457</v>
+      </c>
+      <c r="D2">
+        <v>1213747.422680412</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="AK3" t="s">
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="1">
         <v>35</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="1">
+        <v>38</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="1">
+        <v>39</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="1">
+        <v>40</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="1">
+        <v>41</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="1">
+        <v>43</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="1">
+        <v>44</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="1">
+        <v>45</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="1">
+        <v>49</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="1">
+        <v>51</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="1">
+        <v>52</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="1">
+        <v>53</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="1">
+        <v>54</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="1">
+        <v>55</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="1">
+        <v>56</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="1">
+        <v>57</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="1">
+        <v>58</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="1">
+        <v>59</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="1">
+        <v>60</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="1">
+        <v>61</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="1">
+        <v>62</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="1">
+        <v>63</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="1">
+        <v>64</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="1">
+        <v>65</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="1">
+        <v>66</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="1">
+        <v>67</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="1">
+        <v>68</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="1">
+        <v>69</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="1">
+        <v>70</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="1">
+        <v>71</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="1">
+        <v>72</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="1">
+        <v>73</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="1">
+        <v>74</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="1">
+        <v>75</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="1">
+        <v>76</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="1">
+        <v>77</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+      <c r="D79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="1">
+        <v>78</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="1">
+        <v>79</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="D81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="1">
+        <v>80</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="1">
+        <v>81</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="1">
+        <v>82</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="D84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="1">
+        <v>83</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" s="1">
+        <v>84</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
+      </c>
+      <c r="D86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" s="1">
+        <v>85</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" s="1">
+        <v>86</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" s="1">
+        <v>87</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+      <c r="D89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" s="1">
+        <v>88</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
+      </c>
+      <c r="D90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" s="1">
+        <v>89</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
+      </c>
+      <c r="D91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" s="1">
+        <v>90</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
+      </c>
+      <c r="D92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" s="1">
+        <v>91</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" s="1">
+        <v>92</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
+      </c>
+      <c r="D94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" s="1">
+        <v>93</v>
+      </c>
+      <c r="C95">
+        <v>0</v>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" s="1">
+        <v>94</v>
+      </c>
+      <c r="C96">
+        <v>0</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" s="1">
+        <v>95</v>
+      </c>
+      <c r="C97">
+        <v>0</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" s="1">
+        <v>96</v>
+      </c>
+      <c r="C98">
+        <v>0</v>
+      </c>
+      <c r="D98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" s="1">
+        <v>97</v>
+      </c>
+      <c r="C99">
+        <v>0</v>
+      </c>
+      <c r="D99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" s="1">
+        <v>98</v>
+      </c>
+      <c r="C100">
+        <v>0</v>
+      </c>
+      <c r="D100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" s="1">
+        <v>99</v>
+      </c>
+      <c r="C101">
+        <v>0</v>
+      </c>
+      <c r="D101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" s="1">
+        <v>100</v>
+      </c>
+      <c r="C102">
+        <v>0</v>
+      </c>
+      <c r="D102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" s="1">
+        <v>101</v>
+      </c>
+      <c r="C103">
+        <v>0</v>
+      </c>
+      <c r="D103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" s="1">
+        <v>102</v>
+      </c>
+      <c r="C104">
+        <v>0</v>
+      </c>
+      <c r="D104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" s="1">
+        <v>103</v>
+      </c>
+      <c r="C105">
+        <v>0</v>
+      </c>
+      <c r="D105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" s="1">
+        <v>104</v>
+      </c>
+      <c r="C106">
+        <v>0</v>
+      </c>
+      <c r="D106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" s="1">
+        <v>105</v>
+      </c>
+      <c r="C107">
+        <v>0</v>
+      </c>
+      <c r="D107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" s="1">
+        <v>106</v>
+      </c>
+      <c r="C108">
+        <v>0</v>
+      </c>
+      <c r="D108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109" s="1">
+        <v>107</v>
+      </c>
+      <c r="C109">
+        <v>0</v>
+      </c>
+      <c r="D109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110" s="1">
+        <v>108</v>
+      </c>
+      <c r="C110">
+        <v>0</v>
+      </c>
+      <c r="D110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" s="1">
+        <v>109</v>
+      </c>
+      <c r="C111">
+        <v>0</v>
+      </c>
+      <c r="D111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="A112" s="1">
+        <v>110</v>
+      </c>
+      <c r="C112">
+        <v>0</v>
+      </c>
+      <c r="D112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113" s="1">
+        <v>111</v>
+      </c>
+      <c r="C113">
+        <v>0</v>
+      </c>
+      <c r="D113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114" s="1">
+        <v>112</v>
+      </c>
+      <c r="C114">
+        <v>0</v>
+      </c>
+      <c r="D114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="A115" s="1">
+        <v>113</v>
+      </c>
+      <c r="C115">
+        <v>0</v>
+      </c>
+      <c r="D115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="A116" s="1">
+        <v>114</v>
+      </c>
+      <c r="C116">
+        <v>0</v>
+      </c>
+      <c r="D116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117" s="1">
+        <v>115</v>
+      </c>
+      <c r="C117">
+        <v>0</v>
+      </c>
+      <c r="D117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" s="1">
+        <v>116</v>
+      </c>
+      <c r="C118">
+        <v>0</v>
+      </c>
+      <c r="D118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119" s="1">
+        <v>117</v>
+      </c>
+      <c r="C119">
+        <v>0</v>
+      </c>
+      <c r="D119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120" s="1">
+        <v>118</v>
+      </c>
+      <c r="C120">
+        <v>0</v>
+      </c>
+      <c r="D120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121" s="1">
+        <v>119</v>
+      </c>
+      <c r="C121">
+        <v>0</v>
+      </c>
+      <c r="D121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122" s="1">
+        <v>120</v>
+      </c>
+      <c r="C122">
+        <v>0</v>
+      </c>
+      <c r="D122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="A123" s="1">
+        <v>121</v>
+      </c>
+      <c r="C123">
+        <v>0</v>
+      </c>
+      <c r="D123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="A124" s="1">
+        <v>122</v>
+      </c>
+      <c r="C124">
+        <v>0</v>
+      </c>
+      <c r="D124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125" s="1">
+        <v>123</v>
+      </c>
+      <c r="C125">
+        <v>0</v>
+      </c>
+      <c r="D125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="A126" s="1">
+        <v>124</v>
+      </c>
+      <c r="C126">
+        <v>0</v>
+      </c>
+      <c r="D126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="A127" s="1">
+        <v>125</v>
+      </c>
+      <c r="C127">
+        <v>0</v>
+      </c>
+      <c r="D127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="A128" s="1">
+        <v>126</v>
+      </c>
+      <c r="C128">
+        <v>0</v>
+      </c>
+      <c r="D128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" s="1">
+        <v>127</v>
+      </c>
+      <c r="C129">
+        <v>0</v>
+      </c>
+      <c r="D129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" s="1">
+        <v>128</v>
+      </c>
+      <c r="C130">
+        <v>0</v>
+      </c>
+      <c r="D130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131" s="1">
+        <v>129</v>
+      </c>
+      <c r="C131">
+        <v>0</v>
+      </c>
+      <c r="D131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132" s="1">
+        <v>130</v>
+      </c>
+      <c r="C132">
+        <v>0</v>
+      </c>
+      <c r="D132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="A133" s="1">
+        <v>131</v>
+      </c>
+      <c r="C133">
+        <v>0</v>
+      </c>
+      <c r="D133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134" s="1">
+        <v>132</v>
+      </c>
+      <c r="C134">
+        <v>0</v>
+      </c>
+      <c r="D134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135" s="1">
+        <v>133</v>
+      </c>
+      <c r="C135">
+        <v>0</v>
+      </c>
+      <c r="D135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136" s="1">
+        <v>134</v>
+      </c>
+      <c r="C136">
+        <v>0</v>
+      </c>
+      <c r="D136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="A137" s="1">
+        <v>135</v>
+      </c>
+      <c r="C137">
+        <v>0</v>
+      </c>
+      <c r="D137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138" s="1">
+        <v>136</v>
+      </c>
+      <c r="C138">
+        <v>0</v>
+      </c>
+      <c r="D138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="A139" s="1">
+        <v>137</v>
+      </c>
+      <c r="C139">
+        <v>0</v>
+      </c>
+      <c r="D139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
+      <c r="A140" s="1">
+        <v>138</v>
+      </c>
+      <c r="C140">
+        <v>0</v>
+      </c>
+      <c r="D140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
+      <c r="A141" s="1">
+        <v>139</v>
+      </c>
+      <c r="C141">
+        <v>0</v>
+      </c>
+      <c r="D141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
+      <c r="A142" s="1">
+        <v>140</v>
+      </c>
+      <c r="C142">
+        <v>0</v>
+      </c>
+      <c r="D142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4">
+      <c r="A143" s="1">
+        <v>141</v>
+      </c>
+      <c r="C143">
+        <v>0</v>
+      </c>
+      <c r="D143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
+      <c r="A144" s="1">
+        <v>142</v>
+      </c>
+      <c r="C144">
+        <v>0</v>
+      </c>
+      <c r="D144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
+      <c r="A145" s="1">
+        <v>143</v>
+      </c>
+      <c r="C145">
+        <v>0</v>
+      </c>
+      <c r="D145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
+      <c r="A146" s="1">
+        <v>144</v>
+      </c>
+      <c r="C146">
+        <v>0</v>
+      </c>
+      <c r="D146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
+      <c r="A147" s="1">
+        <v>145</v>
+      </c>
+      <c r="C147">
+        <v>0</v>
+      </c>
+      <c r="D147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4">
+      <c r="A148" s="1">
+        <v>146</v>
+      </c>
+      <c r="C148">
+        <v>0</v>
+      </c>
+      <c r="D148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
+      <c r="A149" s="1">
+        <v>147</v>
+      </c>
+      <c r="C149">
+        <v>0</v>
+      </c>
+      <c r="D149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
+      <c r="A150" s="1">
+        <v>148</v>
+      </c>
+      <c r="C150">
+        <v>0</v>
+      </c>
+      <c r="D150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4">
+      <c r="A151" s="1">
+        <v>149</v>
+      </c>
+      <c r="C151">
+        <v>0</v>
+      </c>
+      <c r="D151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4">
+      <c r="A152" s="1">
+        <v>150</v>
+      </c>
+      <c r="C152">
+        <v>0</v>
+      </c>
+      <c r="D152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4">
+      <c r="A153" s="1">
+        <v>151</v>
+      </c>
+      <c r="C153">
+        <v>0</v>
+      </c>
+      <c r="D153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4">
+      <c r="A154" s="1">
+        <v>152</v>
+      </c>
+      <c r="C154">
+        <v>0</v>
+      </c>
+      <c r="D154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4">
+      <c r="A155" s="1">
+        <v>153</v>
+      </c>
+      <c r="C155">
+        <v>0</v>
+      </c>
+      <c r="D155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4">
+      <c r="A156" s="1">
+        <v>154</v>
+      </c>
+      <c r="C156">
+        <v>0</v>
+      </c>
+      <c r="D156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4">
+      <c r="A157" s="1">
+        <v>155</v>
+      </c>
+      <c r="C157">
+        <v>0</v>
+      </c>
+      <c r="D157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4">
+      <c r="A158" s="1">
+        <v>156</v>
+      </c>
+      <c r="C158">
+        <v>0</v>
+      </c>
+      <c r="D158">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added some unit changes
But not all of them. Missing a MW->GW change. Leaving it till later.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -107,21 +107,21 @@
     <t>DieselHubUsage</t>
   </si>
   <si>
+    <t>tkm-N1Usage</t>
+  </si>
+  <si>
+    <t>tkm-N2Usage</t>
+  </si>
+  <si>
+    <t>tkm-N3Usage</t>
+  </si>
+  <si>
     <t>tkm-SZMUsage</t>
   </si>
   <si>
     <t>pkmUsage</t>
   </si>
   <si>
-    <t>tkm-N1Usage</t>
-  </si>
-  <si>
-    <t>tkm-N2Usage</t>
-  </si>
-  <si>
-    <t>tkm-N3Usage</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -134,7 +134,7 @@
     <t>Process Used</t>
   </si>
   <si>
-    <t>VERA Klärschlammverbrennung GmbH</t>
+    <t>Wacker Chemie AG</t>
   </si>
   <si>
     <t>MtD</t>
@@ -613,7 +613,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>779658.4169504924</v>
+        <v>4650550.598448258</v>
       </c>
       <c r="C2">
         <v>87.14279999999999</v>
@@ -625,7 +625,7 @@
         <v>400</v>
       </c>
       <c r="F2">
-        <v>1213426.338593783</v>
+        <v>343.481450724496</v>
       </c>
       <c r="G2">
         <v>1107.142131147541</v>
@@ -649,28 +649,28 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>1019278.124415571</v>
+        <v>288.5244186085766</v>
       </c>
       <c r="O2">
-        <v>1019278.124415571</v>
+        <v>288.5244186085766</v>
       </c>
       <c r="P2">
-        <v>3.206105902791025e-06</v>
+        <v>0</v>
       </c>
       <c r="Q2">
-        <v>3.206105902791025e-06</v>
+        <v>0</v>
       </c>
       <c r="R2">
-        <v>288.4396630143114</v>
+        <v>288.4396604831751</v>
       </c>
       <c r="S2">
-        <v>288.4396630142583</v>
+        <v>288.4396604831752</v>
       </c>
       <c r="T2">
-        <v>849719.5603369857</v>
+        <v>561.5603395168249</v>
       </c>
       <c r="U2">
-        <v>849719.5603369857</v>
+        <v>561.5603395168248</v>
       </c>
       <c r="V2">
         <v>7.5</v>
@@ -697,25 +697,25 @@
         <v>414.5</v>
       </c>
       <c r="AD2">
-        <v>365.3569064847944</v>
+        <v>365.3569032786885</v>
       </c>
       <c r="AE2">
-        <v>1020235.90964344</v>
+        <v>1246.309646477429</v>
       </c>
       <c r="AF2">
+        <v>7.5</v>
+      </c>
+      <c r="AG2">
+        <v>24.2</v>
+      </c>
+      <c r="AH2">
+        <v>130.3</v>
+      </c>
+      <c r="AI2">
         <v>414.5</v>
       </c>
-      <c r="AG2">
-        <v>850008</v>
-      </c>
-      <c r="AH2">
-        <v>7.5</v>
-      </c>
-      <c r="AI2">
-        <v>24.2</v>
-      </c>
       <c r="AJ2">
-        <v>130.3</v>
+        <v>850</v>
       </c>
     </row>
   </sheetData>
@@ -753,10 +753,10 @@
         <v>39</v>
       </c>
       <c r="C2">
-        <v>20457</v>
+        <v>1612</v>
       </c>
       <c r="D2">
-        <v>1213426.338589966</v>
+        <v>343.481450724496</v>
       </c>
       <c r="E2" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
Added one more conversion
For cost, from MJ to MW
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -107,19 +107,19 @@
     <t>DieselHubUsage</t>
   </si>
   <si>
+    <t>tkm-N2Usage</t>
+  </si>
+  <si>
     <t>tkm-N1Usage</t>
   </si>
   <si>
-    <t>tkm-N2Usage</t>
+    <t>pkmUsage</t>
   </si>
   <si>
     <t>tkm-N3Usage</t>
   </si>
   <si>
     <t>tkm-SZMUsage</t>
-  </si>
-  <si>
-    <t>pkmUsage</t>
   </si>
   <si>
     <t>Name</t>
@@ -613,7 +613,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>4650550.598448258</v>
+        <v>1960969.618549671</v>
       </c>
       <c r="C2">
         <v>87.14279999999999</v>
@@ -625,7 +625,7 @@
         <v>400</v>
       </c>
       <c r="F2">
-        <v>343.481450724496</v>
+        <v>343.4814507244959</v>
       </c>
       <c r="G2">
         <v>1107.142131147541</v>
@@ -649,10 +649,10 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>288.5244186085766</v>
+        <v>288.5244186085765</v>
       </c>
       <c r="O2">
-        <v>288.5244186085766</v>
+        <v>288.5244186085765</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -667,7 +667,7 @@
         <v>288.4396604831752</v>
       </c>
       <c r="T2">
-        <v>561.5603395168249</v>
+        <v>561.5603395168248</v>
       </c>
       <c r="U2">
         <v>561.5603395168248</v>
@@ -703,19 +703,19 @@
         <v>1246.309646477429</v>
       </c>
       <c r="AF2">
+        <v>24.2</v>
+      </c>
+      <c r="AG2">
         <v>7.5</v>
       </c>
-      <c r="AG2">
-        <v>24.2</v>
-      </c>
       <c r="AH2">
+        <v>850</v>
+      </c>
+      <c r="AI2">
         <v>130.3</v>
       </c>
-      <c r="AI2">
+      <c r="AJ2">
         <v>414.5</v>
-      </c>
-      <c r="AJ2">
-        <v>850</v>
       </c>
     </row>
   </sheetData>
@@ -756,7 +756,7 @@
         <v>1612</v>
       </c>
       <c r="D2">
-        <v>343.481450724496</v>
+        <v>343.4814507244959</v>
       </c>
       <c r="E2" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
Ratio Matrix Construction "Done"
Will probably be redone shortly, but whatever.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -107,19 +107,19 @@
     <t>DieselHubUsage</t>
   </si>
   <si>
+    <t>tkm-N1Usage</t>
+  </si>
+  <si>
+    <t>pkmUsage</t>
+  </si>
+  <si>
+    <t>tkm-SZMUsage</t>
+  </si>
+  <si>
+    <t>tkm-N2Usage</t>
+  </si>
+  <si>
     <t>tkm-N3Usage</t>
-  </si>
-  <si>
-    <t>tkm-N2Usage</t>
-  </si>
-  <si>
-    <t>tkm-N1Usage</t>
-  </si>
-  <si>
-    <t>tkm-SZMUsage</t>
-  </si>
-  <si>
-    <t>pkmUsage</t>
   </si>
   <si>
     <t>Name</t>
@@ -1003,7 +1003,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>60374617795.99579</v>
+        <v>60374617778.56241</v>
       </c>
       <c r="C2">
         <v>87.14279999999999</v>
@@ -1015,7 +1015,7 @@
         <v>400</v>
       </c>
       <c r="F2">
-        <v>343.4814507244959</v>
+        <v>343.4814507244961</v>
       </c>
       <c r="G2">
         <v>1107.142131147541</v>
@@ -1039,16 +1039,16 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>288.5244186085765</v>
+        <v>288.5244186085768</v>
       </c>
       <c r="O2">
-        <v>288.5244186085765</v>
+        <v>288.5244186085768</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>-7.553957459549564e-15</v>
       </c>
       <c r="Q2">
-        <v>0</v>
+        <v>-7.553957459549564e-15</v>
       </c>
       <c r="R2">
         <v>288.4396604831751</v>
@@ -1093,19 +1093,19 @@
         <v>1246.309646477429</v>
       </c>
       <c r="AF2">
+        <v>7.5</v>
+      </c>
+      <c r="AG2">
+        <v>850</v>
+      </c>
+      <c r="AH2">
+        <v>414.5</v>
+      </c>
+      <c r="AI2">
+        <v>24.2</v>
+      </c>
+      <c r="AJ2">
         <v>130.3</v>
-      </c>
-      <c r="AG2">
-        <v>24.2</v>
-      </c>
-      <c r="AH2">
-        <v>7.5</v>
-      </c>
-      <c r="AI2">
-        <v>414.5</v>
-      </c>
-      <c r="AJ2">
-        <v>850</v>
       </c>
     </row>
   </sheetData>
@@ -1146,7 +1146,7 @@
         <v>25541</v>
       </c>
       <c r="D2">
-        <v>1.483469072164949</v>
+        <v>1.483469072164948</v>
       </c>
       <c r="E2" t="s">
         <v>170</v>
@@ -1180,7 +1180,7 @@
         <v>25572</v>
       </c>
       <c r="D4">
-        <v>6.790639175257733</v>
+        <v>6.790639175257732</v>
       </c>
       <c r="E4" t="s">
         <v>170</v>
@@ -1197,7 +1197,7 @@
         <v>25734</v>
       </c>
       <c r="D5">
-        <v>7.718798969072167</v>
+        <v>7.718798969072166</v>
       </c>
       <c r="E5" t="s">
         <v>170</v>
@@ -1401,7 +1401,7 @@
         <v>21107</v>
       </c>
       <c r="D17">
-        <v>1.769056701030927</v>
+        <v>1.769056701030928</v>
       </c>
       <c r="E17" t="s">
         <v>170</v>
@@ -1435,7 +1435,7 @@
         <v>21129</v>
       </c>
       <c r="D19">
-        <v>1.784922680412371</v>
+        <v>1.784922680412372</v>
       </c>
       <c r="E19" t="s">
         <v>170</v>
@@ -1486,7 +1486,7 @@
         <v>22113</v>
       </c>
       <c r="D22">
-        <v>3.879231958762888</v>
+        <v>3.879231958762886</v>
       </c>
       <c r="E22" t="s">
         <v>170</v>
@@ -1605,7 +1605,7 @@
         <v>49086</v>
       </c>
       <c r="D29">
-        <v>0.8726288659793812</v>
+        <v>0.8726288659793813</v>
       </c>
       <c r="E29" t="s">
         <v>170</v>
@@ -1707,7 +1707,7 @@
         <v>31171</v>
       </c>
       <c r="D35">
-        <v>0.9598917525773197</v>
+        <v>0.9598917525773195</v>
       </c>
       <c r="E35" t="s">
         <v>170</v>
@@ -1724,7 +1724,7 @@
         <v>31226</v>
       </c>
       <c r="D36">
-        <v>1.30101030927835</v>
+        <v>1.301010309278351</v>
       </c>
       <c r="E36" t="s">
         <v>170</v>
@@ -1877,7 +1877,7 @@
         <v>39164</v>
       </c>
       <c r="D45">
-        <v>0.9598917525773197</v>
+        <v>0.9598917525773195</v>
       </c>
       <c r="E45" t="s">
         <v>170</v>
@@ -1962,7 +1962,7 @@
         <v>58710</v>
       </c>
       <c r="D50">
-        <v>6.393989690721649</v>
+        <v>6.39398969072165</v>
       </c>
       <c r="E50" t="s">
         <v>170</v>
@@ -2064,7 +2064,7 @@
         <v>45329</v>
       </c>
       <c r="D56">
-        <v>4.910520618556701</v>
+        <v>4.910520618556702</v>
       </c>
       <c r="E56" t="s">
         <v>170</v>
@@ -2132,7 +2132,7 @@
         <v>46049</v>
       </c>
       <c r="D60">
-        <v>5.545159793814433</v>
+        <v>5.545159793814434</v>
       </c>
       <c r="E60" t="s">
         <v>170</v>
@@ -2200,7 +2200,7 @@
         <v>47053</v>
       </c>
       <c r="D64">
-        <v>4.505938144329896</v>
+        <v>4.505938144329898</v>
       </c>
       <c r="E64" t="s">
         <v>170</v>
@@ -2234,7 +2234,7 @@
         <v>47166</v>
       </c>
       <c r="D66">
-        <v>7.528407216494845</v>
+        <v>7.528407216494846</v>
       </c>
       <c r="E66" t="s">
         <v>170</v>
@@ -2319,7 +2319,7 @@
         <v>47495</v>
       </c>
       <c r="D71">
-        <v>6.393989690721649</v>
+        <v>6.39398969072165</v>
       </c>
       <c r="E71" t="s">
         <v>170</v>
@@ -2472,7 +2472,7 @@
         <v>44532</v>
       </c>
       <c r="D80">
-        <v>1.388273195876289</v>
+        <v>1.388273195876288</v>
       </c>
       <c r="E80" t="s">
         <v>170</v>
@@ -2489,7 +2489,7 @@
         <v>44536</v>
       </c>
       <c r="D81">
-        <v>1.665927835051546</v>
+        <v>1.665927835051547</v>
       </c>
       <c r="E81" t="s">
         <v>170</v>
@@ -2523,7 +2523,7 @@
         <v>15562</v>
       </c>
       <c r="D83">
-        <v>1.96738144329897</v>
+        <v>1.967381443298969</v>
       </c>
       <c r="E83" t="s">
         <v>170</v>
@@ -2659,7 +2659,7 @@
         <v>6258</v>
       </c>
       <c r="D91">
-        <v>1.34860824742268</v>
+        <v>1.348608247422681</v>
       </c>
       <c r="E91" t="s">
         <v>170</v>
@@ -2710,7 +2710,7 @@
         <v>6638</v>
       </c>
       <c r="D94">
-        <v>6.917567010309277</v>
+        <v>6.917567010309281</v>
       </c>
       <c r="E94" t="s">
         <v>170</v>
@@ -2778,7 +2778,7 @@
         <v>6766</v>
       </c>
       <c r="D98">
-        <v>0.9519587628865979</v>
+        <v>0.9519587628865978</v>
       </c>
       <c r="E98" t="s">
         <v>170</v>
@@ -2880,7 +2880,7 @@
         <v>50997</v>
       </c>
       <c r="D104">
-        <v>2.356097938144329</v>
+        <v>2.35609793814433</v>
       </c>
       <c r="E104" t="s">
         <v>170</v>
@@ -2897,7 +2897,7 @@
         <v>51371</v>
       </c>
       <c r="D105">
-        <v>1.761123711340207</v>
+        <v>1.761123711340206</v>
       </c>
       <c r="E105" t="s">
         <v>170</v>
@@ -2948,7 +2948,7 @@
         <v>51465</v>
       </c>
       <c r="D108">
-        <v>0.9678247422680413</v>
+        <v>0.9678247422680412</v>
       </c>
       <c r="E108" t="s">
         <v>170</v>
@@ -3033,7 +3033,7 @@
         <v>35576</v>
       </c>
       <c r="D113">
-        <v>0.8726288659793812</v>
+        <v>0.8726288659793813</v>
       </c>
       <c r="E113" t="s">
         <v>170</v>
@@ -3101,7 +3101,7 @@
         <v>36266</v>
       </c>
       <c r="D117">
-        <v>1.697659793814434</v>
+        <v>1.697659793814433</v>
       </c>
       <c r="E117" t="s">
         <v>170</v>
@@ -3220,7 +3220,7 @@
         <v>53557</v>
       </c>
       <c r="D124">
-        <v>0.9995567010309282</v>
+        <v>0.9995567010309281</v>
       </c>
       <c r="E124" t="s">
         <v>170</v>
@@ -3339,7 +3339,7 @@
         <v>1983</v>
       </c>
       <c r="D131">
-        <v>1.577528044083465</v>
+        <v>1.753190721649485</v>
       </c>
       <c r="E131" t="s">
         <v>170</v>
@@ -3356,7 +3356,7 @@
         <v>1987</v>
       </c>
       <c r="D132">
-        <v>3.36358762886598</v>
+        <v>3.187924951300077</v>
       </c>
       <c r="E132" t="s">
         <v>170</v>

</xml_diff>

<commit_message>
Corrected the summation of hydrogen uses. Now sums up to the incoming hydrogen connection, not the total transformer input.
To fix: electricity
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="120">
   <si>
     <t>Total Cost</t>
   </si>
@@ -32,6 +32,9 @@
     <t>hydrogen</t>
   </si>
   <si>
+    <t>electricity</t>
+  </si>
+  <si>
     <t>RefineryProduction</t>
   </si>
   <si>
@@ -41,6 +44,18 @@
     <t>Refinery-diesel</t>
   </si>
   <si>
+    <t>Refinery-kerosene</t>
+  </si>
+  <si>
+    <t>Refinery2Production</t>
+  </si>
+  <si>
+    <t>Refinery2-gasoline</t>
+  </si>
+  <si>
+    <t>Refinery2-diesel</t>
+  </si>
+  <si>
     <t>BtDProduction</t>
   </si>
   <si>
@@ -53,18 +68,33 @@
     <t>BtL-gasoline</t>
   </si>
   <si>
-    <t>MtDProduction</t>
-  </si>
-  <si>
-    <t>MtD-diesel</t>
-  </si>
-  <si>
     <t>MtGProduction</t>
   </si>
   <si>
     <t>MtG-gasoline</t>
   </si>
   <si>
+    <t>PtF-FT1Production</t>
+  </si>
+  <si>
+    <t>PtF-FT1-gasoline</t>
+  </si>
+  <si>
+    <t>PtF-FT1-diesel</t>
+  </si>
+  <si>
+    <t>PtF-FT2Production</t>
+  </si>
+  <si>
+    <t>PtF-FT2-gasoline</t>
+  </si>
+  <si>
+    <t>PtF-FT2-diesel</t>
+  </si>
+  <si>
+    <t>PtF-FT2-kerosene</t>
+  </si>
+  <si>
     <t>PVGasProduction</t>
   </si>
   <si>
@@ -107,15 +137,21 @@
     <t>DieselHubUsage</t>
   </si>
   <si>
+    <t>KeroseneHubUsage</t>
+  </si>
+  <si>
+    <t>tkm-N2Usage</t>
+  </si>
+  <si>
+    <t>tkm-N3Usage</t>
+  </si>
+  <si>
+    <t>keroseneUsage</t>
+  </si>
+  <si>
     <t>tkm-SZMUsage</t>
   </si>
   <si>
-    <t>tkm-N2Usage</t>
-  </si>
-  <si>
-    <t>tkm-N3Usage</t>
-  </si>
-  <si>
     <t>pkmUsage</t>
   </si>
   <si>
@@ -272,6 +308,9 @@
     <t>Zellstoff Stendal GmbH</t>
   </si>
   <si>
+    <t>EUROGLAS AG</t>
+  </si>
+  <si>
     <t>Rheinkalk GmbH Werk Hönnetal</t>
   </si>
   <si>
@@ -323,13 +362,19 @@
     <t>CEMEX Zement GmbH</t>
   </si>
   <si>
+    <t>SKW Stickstoffwerke Piesteritz GmbH</t>
+  </si>
+  <si>
+    <t>RWE Power AG-Fabrik Frechen</t>
+  </si>
+  <si>
+    <t>Basell Polyolefine GmbH Werk Wesseling</t>
+  </si>
+  <si>
     <t>Shell Deutschland Oil GmbH Rheinland Raffinerie, Werk Süd</t>
   </si>
   <si>
-    <t>Shell Deutschland Oil GmbH Rheinland Raffinerie Werk Nord</t>
-  </si>
-  <si>
-    <t>MtD</t>
+    <t>PtF-FT1</t>
   </si>
 </sst>
 </file>
@@ -687,13 +732,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AJ2"/>
+  <dimension ref="A1:AV2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:36">
+    <row r="1" spans="1:48">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -799,114 +844,186 @@
       <c r="AJ1" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:36">
+      <c r="AK1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:48">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>14126786177.81083</v>
+        <v>15200173417.69366</v>
       </c>
       <c r="C2">
-        <v>87.14279999999999</v>
+        <v>96</v>
       </c>
       <c r="D2">
-        <v>1190.475409836065</v>
+        <v>1311.475409836066</v>
       </c>
       <c r="E2">
         <v>400</v>
       </c>
       <c r="F2">
-        <v>343.481450724496</v>
+        <v>368.3920002072201</v>
       </c>
       <c r="G2">
-        <v>1107.142131147541</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>365.3569032786885</v>
+        <v>858.4615384615382</v>
       </c>
       <c r="I2">
-        <v>741.7852278688525</v>
+        <v>240</v>
       </c>
       <c r="J2">
+        <v>498.4615384615383</v>
+      </c>
+      <c r="K2">
+        <v>120</v>
+      </c>
+      <c r="L2">
+        <v>361.2105926860029</v>
+      </c>
+      <c r="M2">
+        <v>117.4668594100823</v>
+      </c>
+      <c r="N2">
+        <v>243.7437332759206</v>
+      </c>
+      <c r="O2">
         <v>216</v>
       </c>
-      <c r="K2">
+      <c r="P2">
         <v>216</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>288.5244186085766</v>
-      </c>
-      <c r="O2">
-        <v>288.5244186085766</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>288.4396604831751</v>
+        <v>0</v>
       </c>
       <c r="S2">
-        <v>288.4396604831752</v>
+        <v>0</v>
       </c>
       <c r="T2">
-        <v>561.560339516825</v>
+        <v>0</v>
       </c>
       <c r="U2">
-        <v>561.5603395168248</v>
+        <v>310.2248422797642</v>
       </c>
       <c r="V2">
+        <v>95.86809362117717</v>
+      </c>
+      <c r="W2">
+        <v>214.3567486585871</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>1.4210854715202e-14</v>
+      </c>
+      <c r="AB2">
+        <v>357.8960155509943</v>
+      </c>
+      <c r="AC2">
+        <v>357.8960155509943</v>
+      </c>
+      <c r="AD2">
+        <v>500.1039844490057</v>
+      </c>
+      <c r="AE2">
+        <v>500.1039844490057</v>
+      </c>
+      <c r="AF2">
         <v>7.5</v>
       </c>
-      <c r="W2">
+      <c r="AG2">
         <v>7.5</v>
       </c>
-      <c r="X2">
+      <c r="AH2">
         <v>24.2</v>
       </c>
-      <c r="Y2">
+      <c r="AI2">
         <v>24.2</v>
       </c>
-      <c r="Z2">
+      <c r="AJ2">
         <v>130.3</v>
       </c>
-      <c r="AA2">
+      <c r="AK2">
         <v>130.3</v>
       </c>
-      <c r="AB2">
+      <c r="AL2">
         <v>414.5</v>
       </c>
-      <c r="AC2">
+      <c r="AM2">
         <v>414.5</v>
       </c>
-      <c r="AD2">
-        <v>365.3569032786885</v>
-      </c>
-      <c r="AE2">
-        <v>1246.309646477429</v>
-      </c>
-      <c r="AF2">
+      <c r="AN2">
+        <v>453.3349530312595</v>
+      </c>
+      <c r="AO2">
+        <v>1172.562020396046</v>
+      </c>
+      <c r="AP2">
+        <v>120</v>
+      </c>
+      <c r="AQ2">
+        <v>24.2</v>
+      </c>
+      <c r="AR2">
+        <v>130.3</v>
+      </c>
+      <c r="AS2">
+        <v>120</v>
+      </c>
+      <c r="AT2">
         <v>414.5</v>
       </c>
-      <c r="AG2">
-        <v>24.2</v>
-      </c>
-      <c r="AH2">
-        <v>130.3</v>
-      </c>
-      <c r="AI2">
-        <v>850</v>
-      </c>
-      <c r="AJ2">
+      <c r="AU2">
+        <v>858</v>
+      </c>
+      <c r="AV2">
         <v>7.5</v>
       </c>
     </row>
@@ -917,7 +1034,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E66"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -925,16 +1042,16 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -942,7 +1059,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="C2">
         <v>25541</v>
@@ -951,7 +1068,7 @@
         <v>1.483469072164948</v>
       </c>
       <c r="E2" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -959,7 +1076,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="C3">
         <v>25541</v>
@@ -968,7 +1085,7 @@
         <v>1.316876288659794</v>
       </c>
       <c r="E3" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -976,7 +1093,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="C4">
         <v>25572</v>
@@ -985,7 +1102,7 @@
         <v>6.790639175257732</v>
       </c>
       <c r="E4" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -993,7 +1110,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="C5">
         <v>25734</v>
@@ -1002,7 +1119,7 @@
         <v>7.718798969072166</v>
       </c>
       <c r="E5" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1010,7 +1127,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="C6">
         <v>26388</v>
@@ -1019,7 +1136,7 @@
         <v>1.166149484536083</v>
       </c>
       <c r="E6" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1027,7 +1144,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C7">
         <v>25566</v>
@@ -1036,7 +1153,7 @@
         <v>9.28159793814433</v>
       </c>
       <c r="E7" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1044,16 +1161,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="C8">
         <v>26316</v>
       </c>
       <c r="D8">
-        <v>2.35609793814433</v>
+        <v>2.356097938144329</v>
       </c>
       <c r="E8" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1061,7 +1178,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="C9">
         <v>26954</v>
@@ -1070,7 +1187,7 @@
         <v>1.00748969072165</v>
       </c>
       <c r="E9" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1078,7 +1195,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="C10">
         <v>27570</v>
@@ -1087,7 +1204,7 @@
         <v>2.26090206185567</v>
       </c>
       <c r="E10" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1095,7 +1212,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="C11">
         <v>26892</v>
@@ -1104,7 +1221,7 @@
         <v>2.15777319587629</v>
       </c>
       <c r="E11" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1112,7 +1229,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="C12">
         <v>24534</v>
@@ -1121,7 +1238,7 @@
         <v>3.173195876288661</v>
       </c>
       <c r="E12" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1129,7 +1246,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="C13">
         <v>20457</v>
@@ -1138,7 +1255,7 @@
         <v>1.213747422680412</v>
       </c>
       <c r="E13" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1146,7 +1263,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="C14">
         <v>20539</v>
@@ -1155,7 +1272,7 @@
         <v>1.356541237113402</v>
       </c>
       <c r="E14" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1163,7 +1280,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="C15">
         <v>21079</v>
@@ -1172,7 +1289,7 @@
         <v>6.108402061855671</v>
       </c>
       <c r="E15" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1180,7 +1297,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="C16">
         <v>21107</v>
@@ -1189,7 +1306,7 @@
         <v>2.554422680412372</v>
       </c>
       <c r="E16" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1197,7 +1314,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="C17">
         <v>21107</v>
@@ -1206,7 +1323,7 @@
         <v>1.769056701030928</v>
       </c>
       <c r="E17" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1214,7 +1331,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="C18">
         <v>21119</v>
@@ -1223,7 +1340,7 @@
         <v>2.562355670103094</v>
       </c>
       <c r="E18" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1231,7 +1348,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="C19">
         <v>21129</v>
@@ -1240,7 +1357,7 @@
         <v>1.784922680412372</v>
       </c>
       <c r="E19" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1248,7 +1365,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="C20">
         <v>21683</v>
@@ -1257,7 +1374,7 @@
         <v>4.728061855670104</v>
       </c>
       <c r="E20" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1265,7 +1382,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C21">
         <v>21683</v>
@@ -1274,7 +1391,7 @@
         <v>3.284257731958763</v>
       </c>
       <c r="E21" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1282,7 +1399,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="C22">
         <v>22113</v>
@@ -1291,7 +1408,7 @@
         <v>3.879231958762888</v>
       </c>
       <c r="E22" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1299,7 +1416,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="C23">
         <v>22145</v>
@@ -1308,7 +1425,7 @@
         <v>2.562355670103094</v>
       </c>
       <c r="E23" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1316,7 +1433,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C24">
         <v>24114</v>
@@ -1325,7 +1442,7 @@
         <v>1.039221649484536</v>
       </c>
       <c r="E24" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1333,7 +1450,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="C25">
         <v>28237</v>
@@ -1342,7 +1459,7 @@
         <v>11.52</v>
       </c>
       <c r="E25" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1350,7 +1467,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="C26">
         <v>28237</v>
@@ -1359,7 +1476,7 @@
         <v>4.355211340206187</v>
       </c>
       <c r="E26" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1367,7 +1484,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="C27">
         <v>28237</v>
@@ -1376,7 +1493,7 @@
         <v>2.133974226804124</v>
       </c>
       <c r="E27" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1384,7 +1501,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="C28">
         <v>26197</v>
@@ -1393,7 +1510,7 @@
         <v>9.360927835051548</v>
       </c>
       <c r="E28" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1401,7 +1518,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="C29">
         <v>29525</v>
@@ -1410,7 +1527,7 @@
         <v>1.308943298969072</v>
       </c>
       <c r="E29" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1418,7 +1535,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C30">
         <v>30659</v>
@@ -1427,7 +1544,7 @@
         <v>1.951515463917526</v>
       </c>
       <c r="E30" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1435,7 +1552,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="C31">
         <v>49124</v>
@@ -1444,7 +1561,7 @@
         <v>1.158216494845361</v>
       </c>
       <c r="E31" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1452,7 +1569,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="C32">
         <v>49525</v>
@@ -1461,7 +1578,7 @@
         <v>8.012319587628866</v>
       </c>
       <c r="E32" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1469,7 +1586,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="C33">
         <v>49536</v>
@@ -1478,7 +1595,7 @@
         <v>1.182015463917526</v>
       </c>
       <c r="E33" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1486,7 +1603,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="C34">
         <v>49808</v>
@@ -1495,7 +1612,7 @@
         <v>9.04360824742268</v>
       </c>
       <c r="E34" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1503,7 +1620,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="C35">
         <v>49824</v>
@@ -1512,7 +1629,7 @@
         <v>3.054201030927835</v>
       </c>
       <c r="E35" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1520,7 +1637,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="C36">
         <v>49824</v>
@@ -1529,7 +1646,7 @@
         <v>1.269278350515464</v>
       </c>
       <c r="E36" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1537,7 +1654,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="C37">
         <v>31226</v>
@@ -1546,7 +1663,7 @@
         <v>1.30101030927835</v>
       </c>
       <c r="E37" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1554,7 +1671,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="C38">
         <v>31319</v>
@@ -1563,7 +1680,7 @@
         <v>4.894654639175258</v>
       </c>
       <c r="E38" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1571,7 +1688,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="C39">
         <v>31789</v>
@@ -1580,7 +1697,7 @@
         <v>3.300123711340206</v>
       </c>
       <c r="E39" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1588,7 +1705,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="C40">
         <v>38239</v>
@@ -1597,7 +1714,7 @@
         <v>11.52</v>
       </c>
       <c r="E40" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1605,7 +1722,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="C41">
         <v>31061</v>
@@ -1614,7 +1731,7 @@
         <v>2.625819587628866</v>
       </c>
       <c r="E41" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1622,7 +1739,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="C42">
         <v>33106</v>
@@ -1631,7 +1748,7 @@
         <v>1.832520618556702</v>
       </c>
       <c r="E42" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1639,7 +1756,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="C43">
         <v>33332</v>
@@ -1648,7 +1765,7 @@
         <v>2.046711340206186</v>
       </c>
       <c r="E43" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1656,7 +1773,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="C44">
         <v>33609</v>
@@ -1665,7 +1782,7 @@
         <v>3.078</v>
       </c>
       <c r="E44" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1673,7 +1790,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="C45">
         <v>38372</v>
@@ -1682,7 +1799,7 @@
         <v>3.546046391752578</v>
       </c>
       <c r="E45" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1690,7 +1807,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="C46">
         <v>38723</v>
@@ -1699,7 +1816,7 @@
         <v>2.665484536082475</v>
       </c>
       <c r="E46" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1707,7 +1824,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="C47">
         <v>39596</v>
@@ -1716,7 +1833,7 @@
         <v>11.52</v>
       </c>
       <c r="E47" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1724,16 +1841,16 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="C48">
-        <v>58710</v>
+        <v>39171</v>
       </c>
       <c r="D48">
-        <v>6.39398969072165</v>
+        <v>1.134417525773196</v>
       </c>
       <c r="E48" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1741,16 +1858,16 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="C49">
-        <v>37218</v>
+        <v>58710</v>
       </c>
       <c r="D49">
-        <v>2.966938144329897</v>
+        <v>6.39398969072165</v>
       </c>
       <c r="E49" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1758,16 +1875,16 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C50">
-        <v>37355</v>
+        <v>37218</v>
       </c>
       <c r="D50">
-        <v>8.091649484536084</v>
+        <v>2.966938144329897</v>
       </c>
       <c r="E50" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1775,16 +1892,16 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C51">
-        <v>45329</v>
+        <v>37355</v>
       </c>
       <c r="D51">
-        <v>4.910520618556702</v>
+        <v>8.091649484536084</v>
       </c>
       <c r="E51" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1792,16 +1909,16 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C52">
-        <v>45699</v>
+        <v>45329</v>
       </c>
       <c r="D52">
-        <v>5.307170103092785</v>
+        <v>4.910520618556702</v>
       </c>
       <c r="E52" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1809,16 +1926,16 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="C53">
-        <v>45772</v>
+        <v>45699</v>
       </c>
       <c r="D53">
-        <v>11.52</v>
+        <v>5.307170103092785</v>
       </c>
       <c r="E53" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1826,16 +1943,16 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="C54">
-        <v>45896</v>
+        <v>45772</v>
       </c>
       <c r="D54">
         <v>11.52</v>
       </c>
       <c r="E54" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1843,16 +1960,16 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="C55">
-        <v>45899</v>
+        <v>45896</v>
       </c>
       <c r="D55">
-        <v>9.122938144329899</v>
+        <v>11.52000000000001</v>
       </c>
       <c r="E55" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -1860,16 +1977,16 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="C56">
-        <v>46049</v>
+        <v>45899</v>
       </c>
       <c r="D56">
-        <v>5.545159793814434</v>
+        <v>9.122938144329899</v>
       </c>
       <c r="E56" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -1877,16 +1994,16 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="C57">
-        <v>47166</v>
+        <v>46049</v>
       </c>
       <c r="D57">
-        <v>11.52</v>
+        <v>5.545159793814434</v>
       </c>
       <c r="E57" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -1894,7 +2011,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="C58">
         <v>47166</v>
@@ -1903,7 +2020,7 @@
         <v>11.52</v>
       </c>
       <c r="E58" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -1911,16 +2028,16 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="C59">
         <v>47166</v>
       </c>
       <c r="D59">
-        <v>10.07489690721649</v>
+        <v>11.52</v>
       </c>
       <c r="E59" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -1928,16 +2045,16 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="C60">
         <v>47166</v>
       </c>
       <c r="D60">
-        <v>7.528407216494846</v>
+        <v>10.07489690721649</v>
       </c>
       <c r="E60" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -1945,16 +2062,16 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="C61">
-        <v>47259</v>
+        <v>47166</v>
       </c>
       <c r="D61">
-        <v>11.52</v>
+        <v>7.528407216494846</v>
       </c>
       <c r="E61" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -1962,16 +2079,16 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="C62">
-        <v>47495</v>
+        <v>47259</v>
       </c>
       <c r="D62">
-        <v>6.39398969072165</v>
+        <v>11.52</v>
       </c>
       <c r="E62" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -1979,16 +2096,16 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="C63">
-        <v>42489</v>
+        <v>47495</v>
       </c>
       <c r="D63">
-        <v>11.52</v>
+        <v>6.39398969072165</v>
       </c>
       <c r="E63" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -1996,16 +2113,16 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="C64">
-        <v>15562</v>
+        <v>42489</v>
       </c>
       <c r="D64">
         <v>11.52</v>
       </c>
       <c r="E64" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -2013,16 +2130,16 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="C65">
-        <v>50389</v>
+        <v>15562</v>
       </c>
       <c r="D65">
         <v>11.52</v>
       </c>
       <c r="E65" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -2030,16 +2147,67 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="C66">
-        <v>50997</v>
+        <v>6886</v>
       </c>
       <c r="D66">
-        <v>10.74964144614546</v>
+        <v>11.48577340309642</v>
       </c>
       <c r="E66" t="s">
-        <v>104</v>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="1">
+        <v>65</v>
+      </c>
+      <c r="B67" t="s">
+        <v>116</v>
+      </c>
+      <c r="C67">
+        <v>50226</v>
+      </c>
+      <c r="D67">
+        <v>11.52</v>
+      </c>
+      <c r="E67" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="1">
+        <v>66</v>
+      </c>
+      <c r="B68" t="s">
+        <v>117</v>
+      </c>
+      <c r="C68">
+        <v>50389</v>
+      </c>
+      <c r="D68">
+        <v>11.52</v>
+      </c>
+      <c r="E68" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="1">
+        <v>67</v>
+      </c>
+      <c r="B69" t="s">
+        <v>118</v>
+      </c>
+      <c r="C69">
+        <v>50389</v>
+      </c>
+      <c r="D69">
+        <v>11.52</v>
+      </c>
+      <c r="E69" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added More CO2 Info in Output
Added distance, K value, H2 opex, CO2 opex, and indirect opex values for
each CO2 location in the output folder on the appropriate sheet.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="125">
   <si>
     <t>Total Cost</t>
   </si>
@@ -140,24 +140,24 @@
     <t>KeroseneHubUsage</t>
   </si>
   <si>
+    <t>tkm-N1Usage</t>
+  </si>
+  <si>
+    <t>keroseneUsage</t>
+  </si>
+  <si>
     <t>tkm-SZMUsage</t>
   </si>
   <si>
+    <t>tkm-N3Usage</t>
+  </si>
+  <si>
+    <t>tkm-N2Usage</t>
+  </si>
+  <si>
     <t>pkmUsage</t>
   </si>
   <si>
-    <t>tkm-N2Usage</t>
-  </si>
-  <si>
-    <t>tkm-N3Usage</t>
-  </si>
-  <si>
-    <t>tkm-N1Usage</t>
-  </si>
-  <si>
-    <t>keroseneUsage</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -170,6 +170,21 @@
     <t>Process Used</t>
   </si>
   <si>
+    <t>Distance</t>
+  </si>
+  <si>
+    <t>K Value</t>
+  </si>
+  <si>
+    <t>H2 Opex</t>
+  </si>
+  <si>
+    <t>CO2 Opex</t>
+  </si>
+  <si>
+    <t>Indirect Opex</t>
+  </si>
+  <si>
     <t>Sasol Germany GmbH</t>
   </si>
   <si>
@@ -311,15 +326,18 @@
     <t>Rheinkalk GmbH Werk Hönnetal</t>
   </si>
   <si>
+    <t>MHB Hamm Betriebsführungsgesell schaft mbH</t>
+  </si>
+  <si>
+    <t>Energieversorgung DSS Paper B+T Energie GmbH</t>
+  </si>
+  <si>
     <t>Deuna Zement GmbH</t>
   </si>
   <si>
     <t>RWE Generation SE MHKW Karnap</t>
   </si>
   <si>
-    <t>AGR mbH</t>
-  </si>
-  <si>
     <t>Evonik Degussa GmbH</t>
   </si>
   <si>
@@ -368,7 +386,7 @@
     <t>RWE Power AG-Fabrik Frechen</t>
   </si>
   <si>
-    <t>INEOS Köln GmbH</t>
+    <t>Basell Polyolefine GmbH Werk Wesseling</t>
   </si>
   <si>
     <t>PtF-FT1</t>
@@ -883,7 +901,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>15200160460.66891</v>
+        <v>15200035772.30962</v>
       </c>
       <c r="C2">
         <v>96</v>
@@ -895,10 +913,10 @@
         <v>400</v>
       </c>
       <c r="F2">
-        <v>368.3920002072201</v>
+        <v>368.3920002072203</v>
       </c>
       <c r="G2">
-        <v>37.70093569372136</v>
+        <v>37.70093569372138</v>
       </c>
       <c r="H2">
         <v>858.4615384615383</v>
@@ -940,13 +958,13 @@
         <v>0</v>
       </c>
       <c r="U2">
-        <v>310.2248422797642</v>
+        <v>310.2248422797644</v>
       </c>
       <c r="V2">
-        <v>95.86809362117717</v>
+        <v>95.86809362117722</v>
       </c>
       <c r="W2">
-        <v>214.3567486585871</v>
+        <v>214.3567486585872</v>
       </c>
       <c r="X2">
         <v>0</v>
@@ -1006,22 +1024,22 @@
         <v>120</v>
       </c>
       <c r="AQ2">
+        <v>7.5</v>
+      </c>
+      <c r="AR2">
+        <v>120</v>
+      </c>
+      <c r="AS2">
         <v>414.5</v>
-      </c>
-      <c r="AR2">
-        <v>858</v>
-      </c>
-      <c r="AS2">
-        <v>24.2</v>
       </c>
       <c r="AT2">
         <v>130.3</v>
       </c>
       <c r="AU2">
-        <v>7.5</v>
+        <v>24.2</v>
       </c>
       <c r="AV2">
-        <v>120</v>
+        <v>858</v>
       </c>
     </row>
   </sheetData>
@@ -1031,13 +1049,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:J69"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:10">
       <c r="B1" s="1" t="s">
         <v>47</v>
       </c>
@@ -1050,13 +1068,28 @@
       <c r="E1" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C2">
         <v>25541</v>
@@ -1065,15 +1098,30 @@
         <v>1.483469072164948</v>
       </c>
       <c r="E2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>3487393.97800187</v>
+      </c>
+      <c r="H2">
+        <v>33331633.33333333</v>
+      </c>
+      <c r="I2">
+        <v>100</v>
+      </c>
+      <c r="J2">
+        <v>3211279.34822684</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="C3">
         <v>25541</v>
@@ -1082,15 +1130,30 @@
         <v>1.316876288659794</v>
       </c>
       <c r="E3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>3095903.241680239</v>
+      </c>
+      <c r="H3">
+        <v>33331633.33333333</v>
+      </c>
+      <c r="I3">
+        <v>100</v>
+      </c>
+      <c r="J3">
+        <v>3120028.598903444</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C4">
         <v>25572</v>
@@ -1099,15 +1162,30 @@
         <v>6.790639175257732</v>
       </c>
       <c r="E4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F4">
+        <v>0.1</v>
+      </c>
+      <c r="G4">
+        <v>15940434.28455345</v>
+      </c>
+      <c r="H4">
+        <v>33429264.21745752</v>
+      </c>
+      <c r="I4">
+        <v>100</v>
+      </c>
+      <c r="J4">
+        <v>4640353.526253123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C5">
         <v>25734</v>
@@ -1116,15 +1194,30 @@
         <v>7.718798969072166</v>
       </c>
       <c r="E5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F5">
+        <v>0.1</v>
+      </c>
+      <c r="G5">
+        <v>18114593.9106332</v>
+      </c>
+      <c r="H5">
+        <v>33429264.21745752</v>
+      </c>
+      <c r="I5">
+        <v>100</v>
+      </c>
+      <c r="J5">
+        <v>4786474.22858194</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C6">
         <v>26388</v>
@@ -1133,15 +1226,30 @@
         <v>1.166149484536083</v>
       </c>
       <c r="E6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F6">
+        <v>0.1</v>
+      </c>
+      <c r="G6">
+        <v>2741666.444831646</v>
+      </c>
+      <c r="H6">
+        <v>33429264.21745752</v>
+      </c>
+      <c r="I6">
+        <v>100</v>
+      </c>
+      <c r="J6">
+        <v>3029585.493423196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C7">
         <v>25566</v>
@@ -1150,15 +1258,30 @@
         <v>9.28159793814433</v>
       </c>
       <c r="E7" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F7">
+        <v>0.2</v>
+      </c>
+      <c r="G7">
+        <v>21772856.99976025</v>
+      </c>
+      <c r="H7">
+        <v>33609222.38641504</v>
+      </c>
+      <c r="I7">
+        <v>100</v>
+      </c>
+      <c r="J7">
+        <v>5004876.854845014</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C8">
         <v>26316</v>
@@ -1167,15 +1290,30 @@
         <v>2.35609793814433</v>
       </c>
       <c r="E8" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F8">
+        <v>0.2</v>
+      </c>
+      <c r="G8">
+        <v>5537474.182711428</v>
+      </c>
+      <c r="H8">
+        <v>33609222.38641504</v>
+      </c>
+      <c r="I8">
+        <v>100</v>
+      </c>
+      <c r="J8">
+        <v>3591695.233391508</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C9">
         <v>26954</v>
@@ -1184,15 +1322,30 @@
         <v>1.00748969072165</v>
       </c>
       <c r="E9" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F9">
+        <v>0.2</v>
+      </c>
+      <c r="G9">
+        <v>2368753.896578679</v>
+      </c>
+      <c r="H9">
+        <v>33609222.38641504</v>
+      </c>
+      <c r="I9">
+        <v>100</v>
+      </c>
+      <c r="J9">
+        <v>2924239.357757165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C10">
         <v>27570</v>
@@ -1201,15 +1354,30 @@
         <v>2.26090206185567</v>
       </c>
       <c r="E10" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F10">
+        <v>0.2</v>
+      </c>
+      <c r="G10">
+        <v>5313876.844978522</v>
+      </c>
+      <c r="H10">
+        <v>33609222.38641504</v>
+      </c>
+      <c r="I10">
+        <v>100</v>
+      </c>
+      <c r="J10">
+        <v>3556025.558079649</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C11">
         <v>26892</v>
@@ -1218,15 +1386,30 @@
         <v>2.15777319587629</v>
       </c>
       <c r="E11" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F11">
+        <v>0.5</v>
+      </c>
+      <c r="G11">
+        <v>5071633.194829957</v>
+      </c>
+      <c r="H11">
+        <v>34374076.88937075</v>
+      </c>
+      <c r="I11">
+        <v>100</v>
+      </c>
+      <c r="J11">
+        <v>3516074.693055412</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C12">
         <v>24534</v>
@@ -1235,15 +1418,30 @@
         <v>3.173195876288661</v>
       </c>
       <c r="E12" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F12">
+        <v>0.7</v>
+      </c>
+      <c r="G12">
+        <v>7456203.669209288</v>
+      </c>
+      <c r="H12">
+        <v>34962685.86338257</v>
+      </c>
+      <c r="I12">
+        <v>100</v>
+      </c>
+      <c r="J12">
+        <v>3860032.27064468</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C13">
         <v>20457</v>
@@ -1252,15 +1450,30 @@
         <v>1.213747422680412</v>
       </c>
       <c r="E13" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F13">
+        <v>0.75</v>
+      </c>
+      <c r="G13">
+        <v>2853533.867243568</v>
+      </c>
+      <c r="H13">
+        <v>35112131.13005736</v>
+      </c>
+      <c r="I13">
+        <v>100</v>
+      </c>
+      <c r="J13">
+        <v>3059058.228987825</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C14">
         <v>20539</v>
@@ -1269,15 +1482,30 @@
         <v>1.356541237113402</v>
       </c>
       <c r="E14" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F14">
+        <v>0.75</v>
+      </c>
+      <c r="G14">
+        <v>3189118.573443136</v>
+      </c>
+      <c r="H14">
+        <v>35112131.13005736</v>
+      </c>
+      <c r="I14">
+        <v>100</v>
+      </c>
+      <c r="J14">
+        <v>3142515.846107772</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C15">
         <v>21079</v>
@@ -1286,15 +1514,30 @@
         <v>6.108402061855671</v>
       </c>
       <c r="E15" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F15">
+        <v>0.75</v>
+      </c>
+      <c r="G15">
+        <v>14341627.49504883</v>
+      </c>
+      <c r="H15">
+        <v>35112131.13005736</v>
+      </c>
+      <c r="I15">
+        <v>100</v>
+      </c>
+      <c r="J15">
+        <v>4522964.437644095</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C16">
         <v>21107</v>
@@ -1303,15 +1546,30 @@
         <v>2.554422680412372</v>
       </c>
       <c r="E16" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F16">
+        <v>0.75</v>
+      </c>
+      <c r="G16">
+        <v>6003264.40165077</v>
+      </c>
+      <c r="H16">
+        <v>35112131.13005736</v>
+      </c>
+      <c r="I16">
+        <v>100</v>
+      </c>
+      <c r="J16">
+        <v>3662634.134160224</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C17">
         <v>21107</v>
@@ -1320,15 +1578,30 @@
         <v>1.769056701030928</v>
       </c>
       <c r="E17" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F17">
+        <v>0.75</v>
+      </c>
+      <c r="G17">
+        <v>4158437.557793059</v>
+      </c>
+      <c r="H17">
+        <v>35112131.13005736</v>
+      </c>
+      <c r="I17">
+        <v>100</v>
+      </c>
+      <c r="J17">
+        <v>3351059.927308201</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C18">
         <v>21119</v>
@@ -1337,15 +1610,30 @@
         <v>2.562355670103094</v>
       </c>
       <c r="E18" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F18">
+        <v>0.75</v>
+      </c>
+      <c r="G18">
+        <v>6021894.954526041</v>
+      </c>
+      <c r="H18">
+        <v>35112131.13005736</v>
+      </c>
+      <c r="I18">
+        <v>100</v>
+      </c>
+      <c r="J18">
+        <v>3665383.563029062</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C19">
         <v>21129</v>
@@ -1354,15 +1642,30 @@
         <v>1.784922680412372</v>
       </c>
       <c r="E19" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F19">
+        <v>0.75</v>
+      </c>
+      <c r="G19">
+        <v>4195714.668279373</v>
+      </c>
+      <c r="H19">
+        <v>35112131.13005736</v>
+      </c>
+      <c r="I19">
+        <v>100</v>
+      </c>
+      <c r="J19">
+        <v>3358308.48673273</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C20">
         <v>21683</v>
@@ -1371,15 +1674,30 @@
         <v>4.728061855670104</v>
       </c>
       <c r="E20" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F20">
+        <v>0.75</v>
+      </c>
+      <c r="G20">
+        <v>11104999.99920032</v>
+      </c>
+      <c r="H20">
+        <v>35112131.13005736</v>
+      </c>
+      <c r="I20">
+        <v>100</v>
+      </c>
+      <c r="J20">
+        <v>4251106.766759329</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C21">
         <v>21683</v>
@@ -1388,15 +1706,30 @@
         <v>3.284257731958763</v>
       </c>
       <c r="E21" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F21">
+        <v>0.75</v>
+      </c>
+      <c r="G21">
+        <v>7716935.354567016</v>
+      </c>
+      <c r="H21">
+        <v>35112131.13005736</v>
+      </c>
+      <c r="I21">
+        <v>100</v>
+      </c>
+      <c r="J21">
+        <v>3892301.737650325</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C22">
         <v>22113</v>
@@ -1405,49 +1738,94 @@
         <v>3.879231958762888</v>
       </c>
       <c r="E22" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F22">
+        <v>0.75</v>
+      </c>
+      <c r="G22">
+        <v>9113441.365831105</v>
+      </c>
+      <c r="H22">
+        <v>35112131.13005736</v>
+      </c>
+      <c r="I22">
+        <v>100</v>
+      </c>
+      <c r="J22">
+        <v>4052333.328712357</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C23">
         <v>22145</v>
       </c>
       <c r="D23">
-        <v>2.562355670103094</v>
+        <v>2.562355670103093</v>
       </c>
       <c r="E23" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F23">
+        <v>0.8</v>
+      </c>
+      <c r="G23">
+        <v>6021894.954526041</v>
+      </c>
+      <c r="H23">
+        <v>35261419.93911113</v>
+      </c>
+      <c r="I23">
+        <v>100</v>
+      </c>
+      <c r="J23">
+        <v>3665383.563029062</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C24">
         <v>24114</v>
       </c>
       <c r="D24">
-        <v>1.039221649484536</v>
+        <v>1.039221649484535</v>
       </c>
       <c r="E24" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F24">
+        <v>0.8</v>
+      </c>
+      <c r="G24">
+        <v>2443339.008220378</v>
+      </c>
+      <c r="H24">
+        <v>35261419.93911113</v>
+      </c>
+      <c r="I24">
+        <v>100</v>
+      </c>
+      <c r="J24">
+        <v>2946266.794435292</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C25">
         <v>28237</v>
@@ -1456,15 +1834,30 @@
         <v>11.52</v>
       </c>
       <c r="E25" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F25">
+        <v>0.8</v>
+      </c>
+      <c r="G25">
+        <v>27007138.60142434</v>
+      </c>
+      <c r="H25">
+        <v>35261419.93911113</v>
+      </c>
+      <c r="I25">
+        <v>100</v>
+      </c>
+      <c r="J25">
+        <v>5273515.054654035</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C26">
         <v>28237</v>
@@ -1473,15 +1866,30 @@
         <v>4.355211340206187</v>
       </c>
       <c r="E26" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F26">
+        <v>0.8</v>
+      </c>
+      <c r="G26">
+        <v>10230317.57467575</v>
+      </c>
+      <c r="H26">
+        <v>35261419.93911113</v>
+      </c>
+      <c r="I26">
+        <v>100</v>
+      </c>
+      <c r="J26">
+        <v>4167435.864813926</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C27">
         <v>28237</v>
@@ -1490,15 +1898,30 @@
         <v>2.133974226804124</v>
       </c>
       <c r="E27" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F27">
+        <v>0.8</v>
+      </c>
+      <c r="G27">
+        <v>5015728.864236233</v>
+      </c>
+      <c r="H27">
+        <v>35261419.93911113</v>
+      </c>
+      <c r="I27">
+        <v>100</v>
+      </c>
+      <c r="J27">
+        <v>3506650.390632065</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C28">
         <v>26197</v>
@@ -1507,15 +1930,30 @@
         <v>9.360927835051548</v>
       </c>
       <c r="E28" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>21958471.98347329</v>
+      </c>
+      <c r="H28">
+        <v>35849408.31499194</v>
+      </c>
+      <c r="I28">
+        <v>100</v>
+      </c>
+      <c r="J28">
+        <v>5015195.456029908</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="C29">
         <v>29525</v>
@@ -1524,15 +1962,30 @@
         <v>1.308943298969072</v>
       </c>
       <c r="E29" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F29">
+        <v>1.4</v>
+      </c>
+      <c r="G29">
+        <v>3077259.93144006</v>
+      </c>
+      <c r="H29">
+        <v>36933299.30390043</v>
+      </c>
+      <c r="I29">
+        <v>100</v>
+      </c>
+      <c r="J29">
+        <v>3115469.701891457</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C30">
         <v>30659</v>
@@ -1541,15 +1994,30 @@
         <v>1.951515463917526</v>
       </c>
       <c r="E30" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F30">
+        <v>1.7</v>
+      </c>
+      <c r="G30">
+        <v>4587104.703249776</v>
+      </c>
+      <c r="H30">
+        <v>37640511.58399763</v>
+      </c>
+      <c r="I30">
+        <v>100</v>
+      </c>
+      <c r="J30">
+        <v>3431616.232505888</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C31">
         <v>49124</v>
@@ -1558,15 +2026,30 @@
         <v>1.158216494845361</v>
       </c>
       <c r="E31" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F31">
+        <v>1.8</v>
+      </c>
+      <c r="G31">
+        <v>2723021.589861078</v>
+      </c>
+      <c r="H31">
+        <v>37855437.77268496</v>
+      </c>
+      <c r="I31">
+        <v>100</v>
+      </c>
+      <c r="J31">
+        <v>3024585.102161352</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C32">
         <v>49525</v>
@@ -1575,15 +2058,30 @@
         <v>8.012319587628866</v>
       </c>
       <c r="E32" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F32">
+        <v>1.8</v>
+      </c>
+      <c r="G32">
+        <v>18801918.17235561</v>
+      </c>
+      <c r="H32">
+        <v>37855437.77268496</v>
+      </c>
+      <c r="I32">
+        <v>100</v>
+      </c>
+      <c r="J32">
+        <v>4829900.566914583</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C33">
         <v>49536</v>
@@ -1592,15 +2090,30 @@
         <v>1.182015463917526</v>
       </c>
       <c r="E33" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F33">
+        <v>1.8</v>
+      </c>
+      <c r="G33">
+        <v>2778955.910854831</v>
+      </c>
+      <c r="H33">
+        <v>37855437.77268496</v>
+      </c>
+      <c r="I33">
+        <v>100</v>
+      </c>
+      <c r="J33">
+        <v>3039509.425943215</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C34">
         <v>49808</v>
@@ -1609,15 +2122,30 @@
         <v>9.04360824742268</v>
       </c>
       <c r="E34" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F34">
+        <v>1.8</v>
+      </c>
+      <c r="G34">
+        <v>21215963.57252571</v>
+      </c>
+      <c r="H34">
+        <v>37855437.77268496</v>
+      </c>
+      <c r="I34">
+        <v>100</v>
+      </c>
+      <c r="J34">
+        <v>4973514.536159209</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C35">
         <v>49824</v>
@@ -1626,15 +2154,30 @@
         <v>3.054201030927835</v>
       </c>
       <c r="E35" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F35">
+        <v>1.8</v>
+      </c>
+      <c r="G35">
+        <v>7176830.63573128</v>
+      </c>
+      <c r="H35">
+        <v>37855437.77268496</v>
+      </c>
+      <c r="I35">
+        <v>100</v>
+      </c>
+      <c r="J35">
+        <v>3824493.385265881</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C36">
         <v>49824</v>
@@ -1643,15 +2186,30 @@
         <v>1.269278350515464</v>
       </c>
       <c r="E36" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F36">
+        <v>1.8</v>
+      </c>
+      <c r="G36">
+        <v>2984042.160773337</v>
+      </c>
+      <c r="H36">
+        <v>37855437.77268496</v>
+      </c>
+      <c r="I36">
+        <v>100</v>
+      </c>
+      <c r="J36">
+        <v>3092355.773228031</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C37">
         <v>31226</v>
@@ -1660,32 +2218,62 @@
         <v>1.30101030927835</v>
       </c>
       <c r="E37" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F37">
+        <v>1.9</v>
+      </c>
+      <c r="G37">
+        <v>3058616.539902832</v>
+      </c>
+      <c r="H37">
+        <v>38060293.37896816</v>
+      </c>
+      <c r="I37">
+        <v>100</v>
+      </c>
+      <c r="J37">
+        <v>3110889.813225406</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C38">
         <v>31319</v>
       </c>
       <c r="D38">
-        <v>4.894654639175258</v>
+        <v>4.894654639175257</v>
       </c>
       <c r="E38" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F38">
+        <v>1.9</v>
+      </c>
+      <c r="G38">
+        <v>11495757.65683257</v>
+      </c>
+      <c r="H38">
+        <v>38060293.37896816</v>
+      </c>
+      <c r="I38">
+        <v>100</v>
+      </c>
+      <c r="J38">
+        <v>4286880.992309345</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C39">
         <v>31789</v>
@@ -1694,15 +2282,30 @@
         <v>3.300123711340206</v>
       </c>
       <c r="E39" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F39">
+        <v>1.9</v>
+      </c>
+      <c r="G39">
+        <v>7754181.439418147</v>
+      </c>
+      <c r="H39">
+        <v>38060293.37896816</v>
+      </c>
+      <c r="I39">
+        <v>100</v>
+      </c>
+      <c r="J39">
+        <v>3896843.850100604</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="C40">
         <v>38239</v>
@@ -1711,15 +2314,30 @@
         <v>11.52</v>
       </c>
       <c r="E40" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F40">
+        <v>2</v>
+      </c>
+      <c r="G40">
+        <v>27007138.60142434</v>
+      </c>
+      <c r="H40">
+        <v>38255392.02166688</v>
+      </c>
+      <c r="I40">
+        <v>100</v>
+      </c>
+      <c r="J40">
+        <v>5273515.054654035</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C41">
         <v>31061</v>
@@ -1728,15 +2346,30 @@
         <v>2.625819587628866</v>
       </c>
       <c r="E41" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F41">
+        <v>2.1</v>
+      </c>
+      <c r="G41">
+        <v>6170936.453752637</v>
+      </c>
+      <c r="H41">
+        <v>38441090.93970785</v>
+      </c>
+      <c r="I41">
+        <v>100</v>
+      </c>
+      <c r="J41">
+        <v>3687149.882920415</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42" s="1">
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C42">
         <v>33106</v>
@@ -1745,15 +2378,30 @@
         <v>1.832520618556702</v>
       </c>
       <c r="E42" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F42">
+        <v>2.3</v>
+      </c>
+      <c r="G42">
+        <v>4307544.049353574</v>
+      </c>
+      <c r="H42">
+        <v>38785844.374162</v>
+      </c>
+      <c r="I42">
+        <v>100</v>
+      </c>
+      <c r="J42">
+        <v>3379765.097364126</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43" s="1">
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C43">
         <v>33332</v>
@@ -1762,15 +2410,30 @@
         <v>2.046711340206186</v>
       </c>
       <c r="E43" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F43">
+        <v>2.3</v>
+      </c>
+      <c r="G43">
+        <v>4810740.062798683</v>
+      </c>
+      <c r="H43">
+        <v>38785844.374162</v>
+      </c>
+      <c r="I43">
+        <v>100</v>
+      </c>
+      <c r="J43">
+        <v>3471397.820165223</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44" s="1">
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="C44">
         <v>33609</v>
@@ -1779,15 +2442,30 @@
         <v>3.078</v>
       </c>
       <c r="E44" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F44">
+        <v>2.3</v>
+      </c>
+      <c r="G44">
+        <v>7232706.703717464</v>
+      </c>
+      <c r="H44">
+        <v>38785844.374162</v>
+      </c>
+      <c r="I44">
+        <v>100</v>
+      </c>
+      <c r="J44">
+        <v>3831684.085287054</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45" s="1">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C45">
         <v>38372</v>
@@ -1796,15 +2474,30 @@
         <v>3.546046391752578</v>
       </c>
       <c r="E45" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F45">
+        <v>2.3</v>
+      </c>
+      <c r="G45">
+        <v>8331454.23855985</v>
+      </c>
+      <c r="H45">
+        <v>38785844.374162</v>
+      </c>
+      <c r="I45">
+        <v>100</v>
+      </c>
+      <c r="J45">
+        <v>3965215.892681056</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
       <c r="A46" s="1">
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C46">
         <v>38723</v>
@@ -1813,15 +2506,30 @@
         <v>2.665484536082475</v>
       </c>
       <c r="E46" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F46">
+        <v>2.3</v>
+      </c>
+      <c r="G46">
+        <v>6264084.751326288</v>
+      </c>
+      <c r="H46">
+        <v>38785844.374162</v>
+      </c>
+      <c r="I46">
+        <v>100</v>
+      </c>
+      <c r="J46">
+        <v>3700552.097367561</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47" s="1">
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="C47">
         <v>39596</v>
@@ -1830,15 +2538,30 @@
         <v>11.52</v>
       </c>
       <c r="E47" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F47">
+        <v>2.3</v>
+      </c>
+      <c r="G47">
+        <v>27007138.60142434</v>
+      </c>
+      <c r="H47">
+        <v>38785844.374162</v>
+      </c>
+      <c r="I47">
+        <v>100</v>
+      </c>
+      <c r="J47">
+        <v>5273515.054654035</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
       <c r="A48" s="1">
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C48">
         <v>58710</v>
@@ -1847,168 +2570,318 @@
         <v>6.39398969072165</v>
       </c>
       <c r="E48" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F48">
+        <v>2.5</v>
+      </c>
+      <c r="G48">
+        <v>15010968.32739887</v>
+      </c>
+      <c r="H48">
+        <v>39097761.98338025</v>
+      </c>
+      <c r="I48">
+        <v>100</v>
+      </c>
+      <c r="J48">
+        <v>4573255.840545377</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
       <c r="A49" s="1">
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="C49">
-        <v>37355</v>
+        <v>59075</v>
       </c>
       <c r="D49">
-        <v>8.091649484536084</v>
+        <v>2.022912371134021</v>
       </c>
       <c r="E49" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F49">
+        <v>2.5</v>
+      </c>
+      <c r="G49">
+        <v>4754832.319820861</v>
+      </c>
+      <c r="H49">
+        <v>39097761.98338025</v>
+      </c>
+      <c r="I49">
+        <v>100</v>
+      </c>
+      <c r="J49">
+        <v>3461586.123553794</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
       <c r="A50" s="1">
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="C50">
-        <v>45329</v>
+        <v>37218</v>
       </c>
       <c r="D50">
-        <v>4.910520618556704</v>
+        <v>2.966938144329897</v>
       </c>
       <c r="E50" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F50">
+        <v>2.7</v>
+      </c>
+      <c r="G50">
+        <v>6971945.468368442</v>
+      </c>
+      <c r="H50">
+        <v>39380047.41901974</v>
+      </c>
+      <c r="I50">
+        <v>100</v>
+      </c>
+      <c r="J50">
+        <v>3797758.507656866</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
       <c r="A51" s="1">
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="C51">
-        <v>45699</v>
+        <v>37355</v>
       </c>
       <c r="D51">
-        <v>5.307170103092785</v>
+        <v>8.091649484536084</v>
       </c>
       <c r="E51" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F51">
+        <v>2.9</v>
+      </c>
+      <c r="G51">
+        <v>18987662.48066654</v>
+      </c>
+      <c r="H51">
+        <v>39635749.05499732</v>
+      </c>
+      <c r="I51">
+        <v>100</v>
+      </c>
+      <c r="J51">
+        <v>4841430.024186624</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
       <c r="A52" s="1">
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="C52">
-        <v>45772</v>
+        <v>45329</v>
       </c>
       <c r="D52">
-        <v>11.52</v>
+        <v>4.910520618556702</v>
       </c>
       <c r="E52" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F52">
+        <v>3</v>
+      </c>
+      <c r="G52">
+        <v>11532970.80719121</v>
+      </c>
+      <c r="H52">
+        <v>39754521.5981693</v>
+      </c>
+      <c r="I52">
+        <v>100</v>
+      </c>
+      <c r="J52">
+        <v>4290239.673387973</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
       <c r="A53" s="1">
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="C53">
-        <v>45896</v>
+        <v>45772</v>
       </c>
       <c r="D53">
         <v>11.52</v>
       </c>
       <c r="E53" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F53">
+        <v>3</v>
+      </c>
+      <c r="G53">
+        <v>27007138.60142434</v>
+      </c>
+      <c r="H53">
+        <v>39754521.5981693</v>
+      </c>
+      <c r="I53">
+        <v>100</v>
+      </c>
+      <c r="J53">
+        <v>5273515.054654035</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
       <c r="A54" s="1">
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="C54">
-        <v>45899</v>
+        <v>45896</v>
       </c>
       <c r="D54">
-        <v>9.122938144329899</v>
+        <v>11.52</v>
       </c>
       <c r="E54" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F54">
+        <v>3</v>
+      </c>
+      <c r="G54">
+        <v>27007138.60142434</v>
+      </c>
+      <c r="H54">
+        <v>39754521.5981693</v>
+      </c>
+      <c r="I54">
+        <v>100</v>
+      </c>
+      <c r="J54">
+        <v>5273515.054654035</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
       <c r="A55" s="1">
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="C55">
-        <v>46049</v>
+        <v>45899</v>
       </c>
       <c r="D55">
-        <v>5.545159793814434</v>
+        <v>9.122938144329895</v>
       </c>
       <c r="E55" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F55">
+        <v>3</v>
+      </c>
+      <c r="G55">
+        <v>21401602.79478948</v>
+      </c>
+      <c r="H55">
+        <v>39754521.5981693</v>
+      </c>
+      <c r="I55">
+        <v>100</v>
+      </c>
+      <c r="J55">
+        <v>4984037.426968283</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
       <c r="A56" s="1">
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="C56">
-        <v>47053</v>
+        <v>46049</v>
       </c>
       <c r="D56">
-        <v>4.505938144329896</v>
+        <v>5.545159793814434</v>
       </c>
       <c r="E56" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F56">
+        <v>3</v>
+      </c>
+      <c r="G56">
+        <v>13021230.96247917</v>
+      </c>
+      <c r="H56">
+        <v>39754521.5981693</v>
+      </c>
+      <c r="I56">
+        <v>100</v>
+      </c>
+      <c r="J56">
+        <v>4418307.05254629</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
       <c r="A57" s="1">
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="C57">
-        <v>47166</v>
+        <v>47053</v>
       </c>
       <c r="D57">
-        <v>11.52</v>
+        <v>4.505938144329896</v>
       </c>
       <c r="E57" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F57">
+        <v>3</v>
+      </c>
+      <c r="G57">
+        <v>10583934.16780851</v>
+      </c>
+      <c r="H57">
+        <v>39754521.5981693</v>
+      </c>
+      <c r="I57">
+        <v>100</v>
+      </c>
+      <c r="J57">
+        <v>4201890.346963244</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
       <c r="A58" s="1">
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C58">
         <v>47166</v>
@@ -2017,177 +2890,374 @@
         <v>11.52</v>
       </c>
       <c r="E58" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F58">
+        <v>3</v>
+      </c>
+      <c r="G58">
+        <v>27007138.60142434</v>
+      </c>
+      <c r="H58">
+        <v>39754521.5981693</v>
+      </c>
+      <c r="I58">
+        <v>100</v>
+      </c>
+      <c r="J58">
+        <v>5273515.054654035</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
       <c r="A59" s="1">
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="C59">
         <v>47166</v>
       </c>
       <c r="D59">
-        <v>10.07489690721649</v>
+        <v>11.52</v>
       </c>
       <c r="E59" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F59">
+        <v>3</v>
+      </c>
+      <c r="G59">
+        <v>27007138.60142434</v>
+      </c>
+      <c r="H59">
+        <v>39754521.5981693</v>
+      </c>
+      <c r="I59">
+        <v>100</v>
+      </c>
+      <c r="J59">
+        <v>5273515.054654035</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
       <c r="A60" s="1">
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="C60">
         <v>47166</v>
       </c>
       <c r="D60">
-        <v>7.528407216494846</v>
+        <v>10.07489690721649</v>
       </c>
       <c r="E60" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F60">
+        <v>3</v>
+      </c>
+      <c r="G60">
+        <v>23628643.36424644</v>
+      </c>
+      <c r="H60">
+        <v>39754521.5981693</v>
+      </c>
+      <c r="I60">
+        <v>100</v>
+      </c>
+      <c r="J60">
+        <v>5105201.851214484</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
       <c r="A61" s="1">
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C61">
-        <v>47259</v>
+        <v>47166</v>
       </c>
       <c r="D61">
-        <v>11.52</v>
+        <v>7.528407216494846</v>
       </c>
       <c r="E61" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F61">
+        <v>3</v>
+      </c>
+      <c r="G61">
+        <v>17668702.74772677</v>
+      </c>
+      <c r="H61">
+        <v>39754521.5981693</v>
+      </c>
+      <c r="I61">
+        <v>100</v>
+      </c>
+      <c r="J61">
+        <v>4757631.938664145</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
       <c r="A62" s="1">
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="C62">
-        <v>47495</v>
+        <v>47259</v>
       </c>
       <c r="D62">
-        <v>6.39398969072165</v>
+        <v>11.52</v>
       </c>
       <c r="E62" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F62">
+        <v>3</v>
+      </c>
+      <c r="G62">
+        <v>27007138.60142434</v>
+      </c>
+      <c r="H62">
+        <v>39754521.5981693</v>
+      </c>
+      <c r="I62">
+        <v>100</v>
+      </c>
+      <c r="J62">
+        <v>5273515.054654035</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
       <c r="A63" s="1">
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C63">
-        <v>42489</v>
+        <v>47495</v>
       </c>
       <c r="D63">
-        <v>11.52</v>
+        <v>6.39398969072165</v>
       </c>
       <c r="E63" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F63">
+        <v>3</v>
+      </c>
+      <c r="G63">
+        <v>15010968.32739887</v>
+      </c>
+      <c r="H63">
+        <v>39754521.5981693</v>
+      </c>
+      <c r="I63">
+        <v>100</v>
+      </c>
+      <c r="J63">
+        <v>4573255.840545377</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
       <c r="A64" s="1">
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="C64">
-        <v>15562</v>
+        <v>42489</v>
       </c>
       <c r="D64">
         <v>11.52</v>
       </c>
       <c r="E64" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F64">
+        <v>3.2</v>
+      </c>
+      <c r="G64">
+        <v>27007138.60142434</v>
+      </c>
+      <c r="H64">
+        <v>39975550.38970821</v>
+      </c>
+      <c r="I64">
+        <v>100</v>
+      </c>
+      <c r="J64">
+        <v>5273515.054654035</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
       <c r="A65" s="1">
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="C65">
-        <v>6237</v>
+        <v>15562</v>
       </c>
       <c r="D65">
         <v>11.52</v>
       </c>
       <c r="E65" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F65">
+        <v>3.4</v>
+      </c>
+      <c r="G65">
+        <v>27007138.60142434</v>
+      </c>
+      <c r="H65">
+        <v>40176551.31533918</v>
+      </c>
+      <c r="I65">
+        <v>100</v>
+      </c>
+      <c r="J65">
+        <v>5273515.054654035</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
       <c r="A66" s="1">
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C66">
-        <v>6886</v>
+        <v>6237</v>
       </c>
       <c r="D66">
         <v>11.52</v>
       </c>
       <c r="E66" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F66">
+        <v>3.5</v>
+      </c>
+      <c r="G66">
+        <v>27007138.60142434</v>
+      </c>
+      <c r="H66">
+        <v>40270228.28044015</v>
+      </c>
+      <c r="I66">
+        <v>100</v>
+      </c>
+      <c r="J66">
+        <v>5273515.054654035</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
       <c r="A67" s="1">
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="C67">
-        <v>50226</v>
+        <v>6886</v>
       </c>
       <c r="D67">
         <v>11.52</v>
       </c>
       <c r="E67" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5">
+        <v>124</v>
+      </c>
+      <c r="F67">
+        <v>3.5</v>
+      </c>
+      <c r="G67">
+        <v>27007138.60142434</v>
+      </c>
+      <c r="H67">
+        <v>40270228.28044015</v>
+      </c>
+      <c r="I67">
+        <v>100</v>
+      </c>
+      <c r="J67">
+        <v>5273515.054654035</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
       <c r="A68" s="1">
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C68">
-        <v>50769</v>
+        <v>50226</v>
       </c>
       <c r="D68">
-        <v>11.08119092886961</v>
+        <v>11.39851051649873</v>
       </c>
       <c r="E68" t="s">
-        <v>118</v>
+        <v>124</v>
+      </c>
+      <c r="F68">
+        <v>3.5</v>
+      </c>
+      <c r="G68">
+        <v>27007138.60142434</v>
+      </c>
+      <c r="H68">
+        <v>40270228.28044015</v>
+      </c>
+      <c r="I68">
+        <v>100</v>
+      </c>
+      <c r="J68">
+        <v>5273515.054654035</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
+      <c r="A69" s="1">
+        <v>67</v>
+      </c>
+      <c r="B69" t="s">
+        <v>123</v>
+      </c>
+      <c r="C69">
+        <v>50389</v>
+      </c>
+      <c r="D69">
+        <v>11.52</v>
+      </c>
+      <c r="E69" t="s">
+        <v>124</v>
+      </c>
+      <c r="F69">
+        <v>3.5</v>
+      </c>
+      <c r="G69">
+        <v>27007138.60142434</v>
+      </c>
+      <c r="H69">
+        <v>40270228.28044015</v>
+      </c>
+      <c r="I69">
+        <v>100</v>
+      </c>
+      <c r="J69">
+        <v>5273515.054654035</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cleaned up some. deleted redundant sink constraint
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="124">
   <si>
     <t>Total Cost</t>
   </si>
@@ -140,24 +140,24 @@
     <t>KeroseneHubUsage</t>
   </si>
   <si>
+    <t>tkm-SZMUsage</t>
+  </si>
+  <si>
+    <t>tkm-N3Usage</t>
+  </si>
+  <si>
     <t>keroseneUsage</t>
   </si>
   <si>
     <t>pkmUsage</t>
   </si>
   <si>
-    <t>tkm-SZMUsage</t>
-  </si>
-  <si>
-    <t>tkm-N3Usage</t>
+    <t>tkm-N1Usage</t>
   </si>
   <si>
     <t>tkm-N2Usage</t>
   </si>
   <si>
-    <t>tkm-N1Usage</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -374,175 +374,19 @@
     <t>CEMEX Zement GmbH</t>
   </si>
   <si>
+    <t>TOTAL Raffinerie Mitteldeutschland GmbH (Raffinerie/POX)</t>
+  </si>
+  <si>
     <t>SKW Stickstoffwerke Piesteritz GmbH</t>
   </si>
   <si>
-    <t>RWE Power AG-Fabrik Frechen</t>
-  </si>
-  <si>
-    <t>Basell Polyolefine GmbH Werk Wesseling</t>
-  </si>
-  <si>
     <t>Shell Deutschland Oil GmbH Rheinland Raffinerie, Werk Süd</t>
   </si>
   <si>
+    <t>INEOS Köln GmbH</t>
+  </si>
+  <si>
     <t>PtF-FT1</t>
-  </si>
-  <si>
-    <t>{165: 3211279.3482268397}</t>
-  </si>
-  <si>
-    <t>{165: 3120028.598903444}</t>
-  </si>
-  <si>
-    <t>{165: 4640353.526253123}</t>
-  </si>
-  <si>
-    <t>{165: 4786474.22858194}</t>
-  </si>
-  <si>
-    <t>{165: 3029585.4934231965}</t>
-  </si>
-  <si>
-    <t>{165: 5004876.854845014}</t>
-  </si>
-  <si>
-    <t>{165: 3591695.2333915075}</t>
-  </si>
-  <si>
-    <t>{165: 2924239.357757165}</t>
-  </si>
-  <si>
-    <t>{165: 3556025.558079649}</t>
-  </si>
-  <si>
-    <t>{165: 3516074.6930554123}</t>
-  </si>
-  <si>
-    <t>{165: 3860032.27064468}</t>
-  </si>
-  <si>
-    <t>{165: 3059058.228987825}</t>
-  </si>
-  <si>
-    <t>{165: 3142515.846107772}</t>
-  </si>
-  <si>
-    <t>{165: 4522964.437644095}</t>
-  </si>
-  <si>
-    <t>{165: 3662634.1341602243}</t>
-  </si>
-  <si>
-    <t>{165: 3351059.927308201}</t>
-  </si>
-  <si>
-    <t>{165: 3665383.563029062}</t>
-  </si>
-  <si>
-    <t>{165: 3358308.4867327297}</t>
-  </si>
-  <si>
-    <t>{165: 4251106.7667593295}</t>
-  </si>
-  <si>
-    <t>{165: 3892301.737650325}</t>
-  </si>
-  <si>
-    <t>{165: 4052333.328712357}</t>
-  </si>
-  <si>
-    <t>{165: 2946266.794435292}</t>
-  </si>
-  <si>
-    <t>{165: 5273515.054654035}</t>
-  </si>
-  <si>
-    <t>{165: 4167435.8648139257}</t>
-  </si>
-  <si>
-    <t>{165: 3506650.3906320655}</t>
-  </si>
-  <si>
-    <t>{165: 5015195.456029908}</t>
-  </si>
-  <si>
-    <t>{165: 3115469.701891457}</t>
-  </si>
-  <si>
-    <t>{165: 3431616.2325058877}</t>
-  </si>
-  <si>
-    <t>{165: 3024585.1021613516}</t>
-  </si>
-  <si>
-    <t>{165: 4829900.566914583}</t>
-  </si>
-  <si>
-    <t>{165: 3039509.425943215}</t>
-  </si>
-  <si>
-    <t>{165: 4973514.536159209}</t>
-  </si>
-  <si>
-    <t>{165: 3824493.385265881}</t>
-  </si>
-  <si>
-    <t>{165: 3092355.773228031}</t>
-  </si>
-  <si>
-    <t>{165: 3110889.8132254058}</t>
-  </si>
-  <si>
-    <t>{165: 4286880.992309345}</t>
-  </si>
-  <si>
-    <t>{165: 3896843.8501006044}</t>
-  </si>
-  <si>
-    <t>{165: 3687149.882920415}</t>
-  </si>
-  <si>
-    <t>{165: 3379765.097364126}</t>
-  </si>
-  <si>
-    <t>{165: 3471397.820165223}</t>
-  </si>
-  <si>
-    <t>{165: 3831684.0852870536}</t>
-  </si>
-  <si>
-    <t>{165: 3965215.892681056}</t>
-  </si>
-  <si>
-    <t>{165: 3700552.097367561}</t>
-  </si>
-  <si>
-    <t>{165: 4573255.840545377}</t>
-  </si>
-  <si>
-    <t>{165: 4841430.024186624}</t>
-  </si>
-  <si>
-    <t>{165: 4290239.673387973}</t>
-  </si>
-  <si>
-    <t>{165: 4371651.5460272655}</t>
-  </si>
-  <si>
-    <t>{165: 4984037.426968283}</t>
-  </si>
-  <si>
-    <t>{165: 4418307.05254629}</t>
-  </si>
-  <si>
-    <t>{165: 4201890.346963244}</t>
-  </si>
-  <si>
-    <t>{165: 5105201.851214484}</t>
-  </si>
-  <si>
-    <t>{165: 4757631.938664145}</t>
   </si>
 </sst>
 </file>
@@ -1054,7 +898,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>15200386757.43914</v>
+        <v>15200201566.93848</v>
       </c>
       <c r="C2">
         <v>96</v>
@@ -1066,31 +910,31 @@
         <v>400</v>
       </c>
       <c r="F2">
-        <v>368.3920002072203</v>
+        <v>368.3920002064119</v>
       </c>
       <c r="G2">
-        <v>37.70093569372138</v>
+        <v>37.70093569363865</v>
       </c>
       <c r="H2">
-        <v>858.4615384615386</v>
+        <v>858.4615384615383</v>
       </c>
       <c r="I2">
-        <v>240.0000000000001</v>
+        <v>240</v>
       </c>
       <c r="J2">
-        <v>498.4615384615385</v>
+        <v>498.4615384615384</v>
       </c>
       <c r="K2">
         <v>120</v>
       </c>
       <c r="L2">
-        <v>361.2105926860026</v>
+        <v>361.2105926860028</v>
       </c>
       <c r="M2">
         <v>117.4668594100822</v>
       </c>
       <c r="N2">
-        <v>243.7437332759204</v>
+        <v>243.7437332759206</v>
       </c>
       <c r="O2">
         <v>216</v>
@@ -1111,37 +955,37 @@
         <v>0</v>
       </c>
       <c r="U2">
-        <v>310.2248422797645</v>
+        <v>310.2248422790836</v>
       </c>
       <c r="V2">
-        <v>95.86809362117725</v>
+        <v>95.86809362096685</v>
       </c>
       <c r="W2">
-        <v>214.3567486585872</v>
+        <v>214.3567486581168</v>
       </c>
       <c r="X2">
-        <v>-5.377501535670861e-14</v>
+        <v>0</v>
       </c>
       <c r="Y2">
-        <v>-1.317487876239361e-14</v>
+        <v>0</v>
       </c>
       <c r="Z2">
-        <v>-1.613250460701259e-15</v>
+        <v>0</v>
       </c>
       <c r="AA2">
-        <v>-2.842170943040401e-14</v>
+        <v>0</v>
       </c>
       <c r="AB2">
-        <v>357.8960155509943</v>
+        <v>357.8960155508282</v>
       </c>
       <c r="AC2">
-        <v>357.8960155509943</v>
+        <v>357.8960155508282</v>
       </c>
       <c r="AD2">
-        <v>500.1039844490058</v>
+        <v>500.1039844491718</v>
       </c>
       <c r="AE2">
-        <v>500.1039844490057</v>
+        <v>500.1039844491718</v>
       </c>
       <c r="AF2">
         <v>7.5</v>
@@ -1150,49 +994,49 @@
         <v>7.5</v>
       </c>
       <c r="AH2">
-        <v>24.2</v>
+        <v>24.19999999973852</v>
       </c>
       <c r="AI2">
-        <v>24.2</v>
+        <v>24.19999999973852</v>
       </c>
       <c r="AJ2">
-        <v>130.3</v>
+        <v>130.2999999998167</v>
       </c>
       <c r="AK2">
-        <v>130.3</v>
+        <v>130.2999999998167</v>
       </c>
       <c r="AL2">
-        <v>414.5</v>
+        <v>414.499999999951</v>
       </c>
       <c r="AM2">
-        <v>414.5</v>
+        <v>414.499999999951</v>
       </c>
       <c r="AN2">
-        <v>453.3349530312594</v>
+        <v>453.3349530310491</v>
       </c>
       <c r="AO2">
-        <v>1172.562020396046</v>
+        <v>1172.562020395576</v>
       </c>
       <c r="AP2">
         <v>120</v>
       </c>
       <c r="AQ2">
+        <v>414.499999999951</v>
+      </c>
+      <c r="AR2">
+        <v>130.2999999998167</v>
+      </c>
+      <c r="AS2">
         <v>120</v>
       </c>
-      <c r="AR2">
+      <c r="AT2">
         <v>858</v>
       </c>
-      <c r="AS2">
-        <v>414.5</v>
-      </c>
-      <c r="AT2">
-        <v>130.3</v>
-      </c>
       <c r="AU2">
-        <v>24.2</v>
+        <v>7.5</v>
       </c>
       <c r="AV2">
-        <v>7.5</v>
+        <v>24.19999999973852</v>
       </c>
     </row>
   </sheetData>
@@ -1265,8 +1109,8 @@
       <c r="I2">
         <v>100</v>
       </c>
-      <c r="J2" t="s">
-        <v>124</v>
+      <c r="J2">
+        <v>3211279.34822684</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1297,8 +1141,8 @@
       <c r="I3">
         <v>100</v>
       </c>
-      <c r="J3" t="s">
-        <v>125</v>
+      <c r="J3">
+        <v>3120028.598903444</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1329,8 +1173,8 @@
       <c r="I4">
         <v>100</v>
       </c>
-      <c r="J4" t="s">
-        <v>126</v>
+      <c r="J4">
+        <v>4640353.526253123</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1344,7 +1188,7 @@
         <v>25734</v>
       </c>
       <c r="D5">
-        <v>7.718798969072166</v>
+        <v>7.718798969072163</v>
       </c>
       <c r="E5" t="s">
         <v>123</v>
@@ -1361,8 +1205,8 @@
       <c r="I5">
         <v>100</v>
       </c>
-      <c r="J5" t="s">
-        <v>127</v>
+      <c r="J5">
+        <v>4786474.22858194</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1393,8 +1237,8 @@
       <c r="I6">
         <v>100</v>
       </c>
-      <c r="J6" t="s">
-        <v>128</v>
+      <c r="J6">
+        <v>3029585.493423196</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1425,8 +1269,8 @@
       <c r="I7">
         <v>100</v>
       </c>
-      <c r="J7" t="s">
-        <v>129</v>
+      <c r="J7">
+        <v>5004876.854845014</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1457,8 +1301,8 @@
       <c r="I8">
         <v>100</v>
       </c>
-      <c r="J8" t="s">
-        <v>130</v>
+      <c r="J8">
+        <v>3591695.233391508</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1489,8 +1333,8 @@
       <c r="I9">
         <v>100</v>
       </c>
-      <c r="J9" t="s">
-        <v>131</v>
+      <c r="J9">
+        <v>2924239.357757165</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1521,8 +1365,8 @@
       <c r="I10">
         <v>100</v>
       </c>
-      <c r="J10" t="s">
-        <v>132</v>
+      <c r="J10">
+        <v>3556025.558079649</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1553,8 +1397,8 @@
       <c r="I11">
         <v>100</v>
       </c>
-      <c r="J11" t="s">
-        <v>133</v>
+      <c r="J11">
+        <v>3516074.693055412</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1585,8 +1429,8 @@
       <c r="I12">
         <v>100</v>
       </c>
-      <c r="J12" t="s">
-        <v>134</v>
+      <c r="J12">
+        <v>3860032.27064468</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1617,8 +1461,8 @@
       <c r="I13">
         <v>100</v>
       </c>
-      <c r="J13" t="s">
-        <v>135</v>
+      <c r="J13">
+        <v>3059058.228987825</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1649,8 +1493,8 @@
       <c r="I14">
         <v>100</v>
       </c>
-      <c r="J14" t="s">
-        <v>136</v>
+      <c r="J14">
+        <v>3142515.846107772</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1681,8 +1525,8 @@
       <c r="I15">
         <v>100</v>
       </c>
-      <c r="J15" t="s">
-        <v>137</v>
+      <c r="J15">
+        <v>4522964.437644095</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1713,8 +1557,8 @@
       <c r="I16">
         <v>100</v>
       </c>
-      <c r="J16" t="s">
-        <v>138</v>
+      <c r="J16">
+        <v>3662634.134160224</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1745,8 +1589,8 @@
       <c r="I17">
         <v>100</v>
       </c>
-      <c r="J17" t="s">
-        <v>139</v>
+      <c r="J17">
+        <v>3351059.927308201</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1760,7 +1604,7 @@
         <v>21119</v>
       </c>
       <c r="D18">
-        <v>2.562355670103093</v>
+        <v>2.562355670103094</v>
       </c>
       <c r="E18" t="s">
         <v>123</v>
@@ -1777,8 +1621,8 @@
       <c r="I18">
         <v>100</v>
       </c>
-      <c r="J18" t="s">
-        <v>140</v>
+      <c r="J18">
+        <v>3665383.563029062</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1809,8 +1653,8 @@
       <c r="I19">
         <v>100</v>
       </c>
-      <c r="J19" t="s">
-        <v>141</v>
+      <c r="J19">
+        <v>3358308.48673273</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1824,7 +1668,7 @@
         <v>21683</v>
       </c>
       <c r="D20">
-        <v>4.728061855670103</v>
+        <v>4.728061855670104</v>
       </c>
       <c r="E20" t="s">
         <v>123</v>
@@ -1841,8 +1685,8 @@
       <c r="I20">
         <v>100</v>
       </c>
-      <c r="J20" t="s">
-        <v>142</v>
+      <c r="J20">
+        <v>4251106.766759329</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1873,8 +1717,8 @@
       <c r="I21">
         <v>100</v>
       </c>
-      <c r="J21" t="s">
-        <v>143</v>
+      <c r="J21">
+        <v>3892301.737650325</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1888,7 +1732,7 @@
         <v>22113</v>
       </c>
       <c r="D22">
-        <v>3.879231958762888</v>
+        <v>3.879231958762887</v>
       </c>
       <c r="E22" t="s">
         <v>123</v>
@@ -1905,8 +1749,8 @@
       <c r="I22">
         <v>100</v>
       </c>
-      <c r="J22" t="s">
-        <v>144</v>
+      <c r="J22">
+        <v>4052333.328712357</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1920,7 +1764,7 @@
         <v>22145</v>
       </c>
       <c r="D23">
-        <v>2.562355670103093</v>
+        <v>2.562355670103094</v>
       </c>
       <c r="E23" t="s">
         <v>123</v>
@@ -1937,8 +1781,8 @@
       <c r="I23">
         <v>100</v>
       </c>
-      <c r="J23" t="s">
-        <v>140</v>
+      <c r="J23">
+        <v>3665383.563029062</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1969,8 +1813,8 @@
       <c r="I24">
         <v>100</v>
       </c>
-      <c r="J24" t="s">
-        <v>145</v>
+      <c r="J24">
+        <v>2946266.794435292</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -2001,8 +1845,8 @@
       <c r="I25">
         <v>100</v>
       </c>
-      <c r="J25" t="s">
-        <v>146</v>
+      <c r="J25">
+        <v>5273515.054654035</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -2033,8 +1877,8 @@
       <c r="I26">
         <v>100</v>
       </c>
-      <c r="J26" t="s">
-        <v>147</v>
+      <c r="J26">
+        <v>4167435.864813926</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -2065,8 +1909,8 @@
       <c r="I27">
         <v>100</v>
       </c>
-      <c r="J27" t="s">
-        <v>148</v>
+      <c r="J27">
+        <v>3506650.390632065</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -2080,7 +1924,7 @@
         <v>26197</v>
       </c>
       <c r="D28">
-        <v>9.360927835051548</v>
+        <v>9.36092783505155</v>
       </c>
       <c r="E28" t="s">
         <v>123</v>
@@ -2097,8 +1941,8 @@
       <c r="I28">
         <v>100</v>
       </c>
-      <c r="J28" t="s">
-        <v>149</v>
+      <c r="J28">
+        <v>5015195.456029908</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -2129,8 +1973,8 @@
       <c r="I29">
         <v>100</v>
       </c>
-      <c r="J29" t="s">
-        <v>150</v>
+      <c r="J29">
+        <v>3115469.701891457</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -2161,8 +2005,8 @@
       <c r="I30">
         <v>100</v>
       </c>
-      <c r="J30" t="s">
-        <v>151</v>
+      <c r="J30">
+        <v>3431616.232505888</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -2193,8 +2037,8 @@
       <c r="I31">
         <v>100</v>
       </c>
-      <c r="J31" t="s">
-        <v>152</v>
+      <c r="J31">
+        <v>3024585.102161352</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -2225,8 +2069,8 @@
       <c r="I32">
         <v>100</v>
       </c>
-      <c r="J32" t="s">
-        <v>153</v>
+      <c r="J32">
+        <v>4829900.566914583</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -2257,8 +2101,8 @@
       <c r="I33">
         <v>100</v>
       </c>
-      <c r="J33" t="s">
-        <v>154</v>
+      <c r="J33">
+        <v>3039509.425943215</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -2289,8 +2133,8 @@
       <c r="I34">
         <v>100</v>
       </c>
-      <c r="J34" t="s">
-        <v>155</v>
+      <c r="J34">
+        <v>4973514.536159209</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -2321,8 +2165,8 @@
       <c r="I35">
         <v>100</v>
       </c>
-      <c r="J35" t="s">
-        <v>156</v>
+      <c r="J35">
+        <v>3824493.385265881</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -2353,8 +2197,8 @@
       <c r="I36">
         <v>100</v>
       </c>
-      <c r="J36" t="s">
-        <v>157</v>
+      <c r="J36">
+        <v>3092355.773228031</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -2385,8 +2229,8 @@
       <c r="I37">
         <v>100</v>
       </c>
-      <c r="J37" t="s">
-        <v>158</v>
+      <c r="J37">
+        <v>3110889.813225406</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -2417,8 +2261,8 @@
       <c r="I38">
         <v>100</v>
       </c>
-      <c r="J38" t="s">
-        <v>159</v>
+      <c r="J38">
+        <v>4286880.992309345</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -2449,8 +2293,8 @@
       <c r="I39">
         <v>100</v>
       </c>
-      <c r="J39" t="s">
-        <v>160</v>
+      <c r="J39">
+        <v>3896843.850100604</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -2481,8 +2325,8 @@
       <c r="I40">
         <v>100</v>
       </c>
-      <c r="J40" t="s">
-        <v>146</v>
+      <c r="J40">
+        <v>5273515.054654035</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -2513,8 +2357,8 @@
       <c r="I41">
         <v>100</v>
       </c>
-      <c r="J41" t="s">
-        <v>161</v>
+      <c r="J41">
+        <v>3687149.882920415</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -2545,8 +2389,8 @@
       <c r="I42">
         <v>100</v>
       </c>
-      <c r="J42" t="s">
-        <v>162</v>
+      <c r="J42">
+        <v>3379765.097364126</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -2577,8 +2421,8 @@
       <c r="I43">
         <v>100</v>
       </c>
-      <c r="J43" t="s">
-        <v>163</v>
+      <c r="J43">
+        <v>3471397.820165223</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -2609,8 +2453,8 @@
       <c r="I44">
         <v>100</v>
       </c>
-      <c r="J44" t="s">
-        <v>164</v>
+      <c r="J44">
+        <v>3831684.085287054</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -2641,8 +2485,8 @@
       <c r="I45">
         <v>100</v>
       </c>
-      <c r="J45" t="s">
-        <v>165</v>
+      <c r="J45">
+        <v>3965215.892681056</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -2673,8 +2517,8 @@
       <c r="I46">
         <v>100</v>
       </c>
-      <c r="J46" t="s">
-        <v>166</v>
+      <c r="J46">
+        <v>3700552.097367561</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -2705,8 +2549,8 @@
       <c r="I47">
         <v>100</v>
       </c>
-      <c r="J47" t="s">
-        <v>146</v>
+      <c r="J47">
+        <v>5273515.054654035</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -2737,8 +2581,8 @@
       <c r="I48">
         <v>100</v>
       </c>
-      <c r="J48" t="s">
-        <v>167</v>
+      <c r="J48">
+        <v>4573255.840545377</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -2769,8 +2613,8 @@
       <c r="I49">
         <v>100</v>
       </c>
-      <c r="J49" t="s">
-        <v>168</v>
+      <c r="J49">
+        <v>4841430.024186624</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -2801,8 +2645,8 @@
       <c r="I50">
         <v>100</v>
       </c>
-      <c r="J50" t="s">
-        <v>169</v>
+      <c r="J50">
+        <v>4290239.673387973</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -2816,7 +2660,7 @@
         <v>45699</v>
       </c>
       <c r="D51">
-        <v>4.868361031963745</v>
+        <v>5.307170103092785</v>
       </c>
       <c r="E51" t="s">
         <v>123</v>
@@ -2833,8 +2677,8 @@
       <c r="I51">
         <v>100</v>
       </c>
-      <c r="J51" t="s">
-        <v>170</v>
+      <c r="J51">
+        <v>4371651.546027265</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -2848,7 +2692,7 @@
         <v>45772</v>
       </c>
       <c r="D52">
-        <v>11.52</v>
+        <v>11.51999999999999</v>
       </c>
       <c r="E52" t="s">
         <v>123</v>
@@ -2865,8 +2709,8 @@
       <c r="I52">
         <v>100</v>
       </c>
-      <c r="J52" t="s">
-        <v>146</v>
+      <c r="J52">
+        <v>5273515.054654035</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -2897,8 +2741,8 @@
       <c r="I53">
         <v>100</v>
       </c>
-      <c r="J53" t="s">
-        <v>146</v>
+      <c r="J53">
+        <v>5273515.054654035</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -2929,8 +2773,8 @@
       <c r="I54">
         <v>100</v>
       </c>
-      <c r="J54" t="s">
-        <v>171</v>
+      <c r="J54">
+        <v>4984037.426968283</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -2961,8 +2805,8 @@
       <c r="I55">
         <v>100</v>
       </c>
-      <c r="J55" t="s">
-        <v>172</v>
+      <c r="J55">
+        <v>4418307.05254629</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -2976,7 +2820,7 @@
         <v>47053</v>
       </c>
       <c r="D56">
-        <v>4.505938144329896</v>
+        <v>4.505938144329895</v>
       </c>
       <c r="E56" t="s">
         <v>123</v>
@@ -2993,8 +2837,8 @@
       <c r="I56">
         <v>100</v>
       </c>
-      <c r="J56" t="s">
-        <v>173</v>
+      <c r="J56">
+        <v>4201890.346963244</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -3025,8 +2869,8 @@
       <c r="I57">
         <v>100</v>
       </c>
-      <c r="J57" t="s">
-        <v>146</v>
+      <c r="J57">
+        <v>5273515.054654035</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -3057,8 +2901,8 @@
       <c r="I58">
         <v>100</v>
       </c>
-      <c r="J58" t="s">
-        <v>146</v>
+      <c r="J58">
+        <v>5273515.054654035</v>
       </c>
     </row>
     <row r="59" spans="1:10">
@@ -3089,8 +2933,8 @@
       <c r="I59">
         <v>100</v>
       </c>
-      <c r="J59" t="s">
-        <v>174</v>
+      <c r="J59">
+        <v>5105201.851214484</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -3121,8 +2965,8 @@
       <c r="I60">
         <v>100</v>
       </c>
-      <c r="J60" t="s">
-        <v>175</v>
+      <c r="J60">
+        <v>4757631.938664145</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -3153,8 +2997,8 @@
       <c r="I61">
         <v>100</v>
       </c>
-      <c r="J61" t="s">
-        <v>146</v>
+      <c r="J61">
+        <v>5273515.054654035</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -3168,7 +3012,7 @@
         <v>47495</v>
       </c>
       <c r="D62">
-        <v>6.393989690721652</v>
+        <v>6.39398969072165</v>
       </c>
       <c r="E62" t="s">
         <v>123</v>
@@ -3185,8 +3029,8 @@
       <c r="I62">
         <v>100</v>
       </c>
-      <c r="J62" t="s">
-        <v>167</v>
+      <c r="J62">
+        <v>4573255.840545377</v>
       </c>
     </row>
     <row r="63" spans="1:10">
@@ -3217,8 +3061,8 @@
       <c r="I63">
         <v>100</v>
       </c>
-      <c r="J63" t="s">
-        <v>146</v>
+      <c r="J63">
+        <v>5273515.054654035</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -3232,7 +3076,7 @@
         <v>15562</v>
       </c>
       <c r="D64">
-        <v>11.52</v>
+        <v>11.08119092806143</v>
       </c>
       <c r="E64" t="s">
         <v>123</v>
@@ -3249,8 +3093,8 @@
       <c r="I64">
         <v>100</v>
       </c>
-      <c r="J64" t="s">
-        <v>146</v>
+      <c r="J64">
+        <v>5273515.054654035</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -3261,10 +3105,10 @@
         <v>119</v>
       </c>
       <c r="C65">
-        <v>6886</v>
+        <v>6237</v>
       </c>
       <c r="D65">
-        <v>11.51999999999888</v>
+        <v>11.52</v>
       </c>
       <c r="E65" t="s">
         <v>123</v>
@@ -3281,8 +3125,8 @@
       <c r="I65">
         <v>100</v>
       </c>
-      <c r="J65" t="s">
-        <v>146</v>
+      <c r="J65">
+        <v>5273515.054654035</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -3293,7 +3137,7 @@
         <v>120</v>
       </c>
       <c r="C66">
-        <v>50226</v>
+        <v>6886</v>
       </c>
       <c r="D66">
         <v>11.52</v>
@@ -3313,8 +3157,8 @@
       <c r="I66">
         <v>100</v>
       </c>
-      <c r="J66" t="s">
-        <v>146</v>
+      <c r="J66">
+        <v>5273515.054654035</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -3345,8 +3189,8 @@
       <c r="I67">
         <v>100</v>
       </c>
-      <c r="J67" t="s">
-        <v>146</v>
+      <c r="J67">
+        <v>5273515.054654035</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -3357,7 +3201,7 @@
         <v>122</v>
       </c>
       <c r="C68">
-        <v>50389</v>
+        <v>50769</v>
       </c>
       <c r="D68">
         <v>11.52</v>
@@ -3377,8 +3221,8 @@
       <c r="I68">
         <v>100</v>
       </c>
-      <c r="J68" t="s">
-        <v>146</v>
+      <c r="J68">
+        <v>5273515.054654035</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Have to commit to pull
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="141">
   <si>
     <t>Total Cost</t>
   </si>
@@ -194,24 +194,24 @@
     <t>MethaneHubUsage</t>
   </si>
   <si>
+    <t>tkm-N2Usage</t>
+  </si>
+  <si>
+    <t>keroseneUsage</t>
+  </si>
+  <si>
+    <t>pkmUsage</t>
+  </si>
+  <si>
     <t>tkm-SZMUsage</t>
   </si>
   <si>
-    <t>tkm-N2Usage</t>
-  </si>
-  <si>
-    <t>pkmUsage</t>
-  </si>
-  <si>
-    <t>keroseneUsage</t>
+    <t>tkm-N1Usage</t>
   </si>
   <si>
     <t>tkm-N3Usage</t>
   </si>
   <si>
-    <t>tkm-N1Usage</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -326,9 +326,6 @@
     <t>EEW Energy from Waste Hannover GmbH</t>
   </si>
   <si>
-    <t>Schoeller Technocell GmbH &amp; Co. KG</t>
-  </si>
-  <si>
     <t>Georgsmarienhütte GmbH</t>
   </si>
   <si>
@@ -347,6 +344,9 @@
     <t>EBE Holzheizkraftwerk GmbH</t>
   </si>
   <si>
+    <t>Nordzucker AG Werk Nordstemmen</t>
+  </si>
+  <si>
     <t>Peiner Träger GmbH</t>
   </si>
   <si>
@@ -383,6 +383,9 @@
     <t>Rheinkalk GmbH Werk Hönnetal</t>
   </si>
   <si>
+    <t>Energieversorgung DSS Paper B+T Energie GmbH</t>
+  </si>
+  <si>
     <t>Deuna Zement GmbH</t>
   </si>
   <si>
@@ -404,6 +407,9 @@
     <t>GMVA Gemeinschafts-Müllverbrennungsanlage Niederrhein GmbH</t>
   </si>
   <si>
+    <t>DK Recycling und Roheisen GmbH</t>
+  </si>
+  <si>
     <t>ThyssenKrupp Steel Europe AG Werk Schwelgern</t>
   </si>
   <si>
@@ -416,6 +422,9 @@
     <t>ThyssenKrupp Steel Europe AG Werk Beeckerwerth</t>
   </si>
   <si>
+    <t>ThyssenKrupp Steel Europe AG Werk Bruckhausen</t>
+  </si>
+  <si>
     <t>Hüttenwerke Krupp Mannesmann GmbH</t>
   </si>
   <si>
@@ -426,9 +435,6 @@
   </si>
   <si>
     <t>CEMEX Zement GmbH</t>
-  </si>
-  <si>
-    <t>SKW Stickstoffwerke Piesteritz GmbH</t>
   </si>
   <si>
     <t>PtF-FT1</t>
@@ -997,10 +1003,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>13567537369.02723</v>
+        <v>13567275360.45065</v>
       </c>
       <c r="C2">
-        <v>96</v>
+        <v>95.99999999999997</v>
       </c>
       <c r="D2">
         <v>1190.511948111309</v>
@@ -1012,10 +1018,10 @@
         <v>400</v>
       </c>
       <c r="G2">
-        <v>330.4949195865013</v>
+        <v>330.4949195865016</v>
       </c>
       <c r="H2">
-        <v>33.82257948984662</v>
+        <v>33.82257948984665</v>
       </c>
       <c r="I2">
         <v>858.4615384615383</v>
@@ -1030,13 +1036,13 @@
         <v>120</v>
       </c>
       <c r="M2">
-        <v>248.7145732819791</v>
+        <v>248.7145732819787</v>
       </c>
       <c r="N2">
-        <v>80.88278805918021</v>
+        <v>80.88278805918009</v>
       </c>
       <c r="O2">
-        <v>167.8317852227989</v>
+        <v>167.8317852227987</v>
       </c>
       <c r="P2">
         <v>154.0911111111111</v>
@@ -1069,13 +1075,13 @@
         <v>0</v>
       </c>
       <c r="Z2">
-        <v>278.3115112307378</v>
+        <v>278.3115112307381</v>
       </c>
       <c r="AA2">
-        <v>86.00598784560998</v>
+        <v>86.00598784561005</v>
       </c>
       <c r="AB2">
-        <v>192.3055233851279</v>
+        <v>192.305523385128</v>
       </c>
       <c r="AC2">
         <v>0</v>
@@ -1096,10 +1102,10 @@
         <v>0</v>
       </c>
       <c r="AI2">
-        <v>321.227980977466</v>
+        <v>321.2279809774659</v>
       </c>
       <c r="AJ2">
-        <v>321.227980977466</v>
+        <v>321.2279809774659</v>
       </c>
       <c r="AK2">
         <v>450.772019022534</v>
@@ -1162,7 +1168,7 @@
         <v>41.45</v>
       </c>
       <c r="BE2">
-        <v>406.8887759047902</v>
+        <v>406.8887759047901</v>
       </c>
       <c r="BF2">
         <v>1074.598847069465</v>
@@ -1174,22 +1180,22 @@
         <v>154.0911111111111</v>
       </c>
       <c r="BI2">
+        <v>24.2</v>
+      </c>
+      <c r="BJ2">
+        <v>120</v>
+      </c>
+      <c r="BK2">
+        <v>857.9999999999999</v>
+      </c>
+      <c r="BL2">
         <v>414.5</v>
       </c>
-      <c r="BJ2">
-        <v>24.2</v>
-      </c>
-      <c r="BK2">
-        <v>858</v>
-      </c>
-      <c r="BL2">
-        <v>120</v>
-      </c>
       <c r="BM2">
+        <v>7.5</v>
+      </c>
+      <c r="BN2">
         <v>130.3</v>
-      </c>
-      <c r="BN2">
-        <v>7.5</v>
       </c>
     </row>
   </sheetData>
@@ -1199,7 +1205,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J65"/>
+  <dimension ref="A1:J67"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1248,7 +1254,7 @@
         <v>1.483469072164948</v>
       </c>
       <c r="E2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -1280,7 +1286,7 @@
         <v>1.316876288659794</v>
       </c>
       <c r="E3" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1312,7 +1318,7 @@
         <v>6.790639175257732</v>
       </c>
       <c r="E4" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F4">
         <v>0.1</v>
@@ -1344,7 +1350,7 @@
         <v>7.718798969072166</v>
       </c>
       <c r="E5" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F5">
         <v>0.1</v>
@@ -1373,10 +1379,10 @@
         <v>26388</v>
       </c>
       <c r="D6">
-        <v>1.166149484536083</v>
+        <v>1.166149484536082</v>
       </c>
       <c r="E6" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F6">
         <v>0.1</v>
@@ -1405,10 +1411,10 @@
         <v>25566</v>
       </c>
       <c r="D7">
-        <v>9.281597938144325</v>
+        <v>9.28159793814433</v>
       </c>
       <c r="E7" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F7">
         <v>0.2</v>
@@ -1440,7 +1446,7 @@
         <v>2.35609793814433</v>
       </c>
       <c r="E8" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F8">
         <v>0.2</v>
@@ -1472,7 +1478,7 @@
         <v>1.00748969072165</v>
       </c>
       <c r="E9" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F9">
         <v>0.2</v>
@@ -1504,7 +1510,7 @@
         <v>2.26090206185567</v>
       </c>
       <c r="E10" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F10">
         <v>0.2</v>
@@ -1533,10 +1539,10 @@
         <v>26892</v>
       </c>
       <c r="D11">
-        <v>2.15777319587629</v>
+        <v>2.157773195876289</v>
       </c>
       <c r="E11" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F11">
         <v>0.5</v>
@@ -1568,7 +1574,7 @@
         <v>3.173195876288661</v>
       </c>
       <c r="E12" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F12">
         <v>0.7</v>
@@ -1600,7 +1606,7 @@
         <v>1.213747422680412</v>
       </c>
       <c r="E13" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F13">
         <v>0.75</v>
@@ -1632,7 +1638,7 @@
         <v>1.356541237113402</v>
       </c>
       <c r="E14" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F14">
         <v>0.75</v>
@@ -1664,7 +1670,7 @@
         <v>6.108402061855671</v>
       </c>
       <c r="E15" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F15">
         <v>0.75</v>
@@ -1696,7 +1702,7 @@
         <v>2.554422680412372</v>
       </c>
       <c r="E16" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F16">
         <v>0.75</v>
@@ -1728,7 +1734,7 @@
         <v>1.769056701030928</v>
       </c>
       <c r="E17" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F17">
         <v>0.75</v>
@@ -1757,10 +1763,10 @@
         <v>21119</v>
       </c>
       <c r="D18">
-        <v>2.562355670103092</v>
+        <v>2.562355670103093</v>
       </c>
       <c r="E18" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F18">
         <v>0.75</v>
@@ -1792,7 +1798,7 @@
         <v>1.784922680412372</v>
       </c>
       <c r="E19" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F19">
         <v>0.75</v>
@@ -1824,7 +1830,7 @@
         <v>4.728061855670104</v>
       </c>
       <c r="E20" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F20">
         <v>0.75</v>
@@ -1853,10 +1859,10 @@
         <v>21683</v>
       </c>
       <c r="D21">
-        <v>3.284257731958761</v>
+        <v>3.284257731958762</v>
       </c>
       <c r="E21" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F21">
         <v>0.75</v>
@@ -1888,7 +1894,7 @@
         <v>3.879231958762888</v>
       </c>
       <c r="E22" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F22">
         <v>0.75</v>
@@ -1917,10 +1923,10 @@
         <v>22145</v>
       </c>
       <c r="D23">
-        <v>2.562355670103093</v>
+        <v>2.562355670103094</v>
       </c>
       <c r="E23" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F23">
         <v>0.8</v>
@@ -1952,7 +1958,7 @@
         <v>1.039221649484536</v>
       </c>
       <c r="E24" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F24">
         <v>0.8</v>
@@ -1984,7 +1990,7 @@
         <v>11.52</v>
       </c>
       <c r="E25" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F25">
         <v>0.8</v>
@@ -2013,10 +2019,10 @@
         <v>28237</v>
       </c>
       <c r="D26">
-        <v>4.355211340206187</v>
+        <v>4.35521134020618</v>
       </c>
       <c r="E26" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F26">
         <v>0.8</v>
@@ -2045,10 +2051,10 @@
         <v>28237</v>
       </c>
       <c r="D27">
-        <v>2.133974226804124</v>
+        <v>2.1339742268041</v>
       </c>
       <c r="E27" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F27">
         <v>0.8</v>
@@ -2080,7 +2086,7 @@
         <v>9.360927835051548</v>
       </c>
       <c r="E28" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F28">
         <v>1</v>
@@ -2112,7 +2118,7 @@
         <v>1.308943298969072</v>
       </c>
       <c r="E29" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F29">
         <v>1.4</v>
@@ -2144,7 +2150,7 @@
         <v>1.951515463917526</v>
       </c>
       <c r="E30" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F30">
         <v>1.7</v>
@@ -2170,19 +2176,19 @@
         <v>103</v>
       </c>
       <c r="C31">
-        <v>49086</v>
+        <v>49124</v>
       </c>
       <c r="D31">
-        <v>0.8726288659793813</v>
+        <v>1.158216494845361</v>
       </c>
       <c r="E31" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F31">
         <v>1.8</v>
       </c>
       <c r="G31">
-        <v>2051752.656756106</v>
+        <v>2723021.589861078</v>
       </c>
       <c r="H31">
         <v>37855437.77268496</v>
@@ -2191,7 +2197,7 @@
         <v>100</v>
       </c>
       <c r="J31">
-        <v>2824291.034417088</v>
+        <v>3024585.102161352</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -2202,19 +2208,19 @@
         <v>104</v>
       </c>
       <c r="C32">
-        <v>49124</v>
+        <v>49525</v>
       </c>
       <c r="D32">
-        <v>1.158216494845361</v>
+        <v>8.012319587628866</v>
       </c>
       <c r="E32" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F32">
         <v>1.8</v>
       </c>
       <c r="G32">
-        <v>2723021.589861078</v>
+        <v>18801918.17235561</v>
       </c>
       <c r="H32">
         <v>37855437.77268496</v>
@@ -2223,7 +2229,7 @@
         <v>100</v>
       </c>
       <c r="J32">
-        <v>3024585.102161352</v>
+        <v>4829900.566914583</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -2234,19 +2240,19 @@
         <v>105</v>
       </c>
       <c r="C33">
-        <v>49525</v>
+        <v>49536</v>
       </c>
       <c r="D33">
-        <v>8.012319587628866</v>
+        <v>1.182015463917526</v>
       </c>
       <c r="E33" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F33">
         <v>1.8</v>
       </c>
       <c r="G33">
-        <v>18801918.17235561</v>
+        <v>2778955.910854831</v>
       </c>
       <c r="H33">
         <v>37855437.77268496</v>
@@ -2255,7 +2261,7 @@
         <v>100</v>
       </c>
       <c r="J33">
-        <v>4829900.566914583</v>
+        <v>3039509.425943215</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -2266,19 +2272,19 @@
         <v>106</v>
       </c>
       <c r="C34">
-        <v>49536</v>
+        <v>49808</v>
       </c>
       <c r="D34">
-        <v>1.182015463917526</v>
+        <v>9.043608247422679</v>
       </c>
       <c r="E34" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F34">
         <v>1.8</v>
       </c>
       <c r="G34">
-        <v>2778955.910854831</v>
+        <v>21215963.57252571</v>
       </c>
       <c r="H34">
         <v>37855437.77268496</v>
@@ -2287,7 +2293,7 @@
         <v>100</v>
       </c>
       <c r="J34">
-        <v>3039509.425943215</v>
+        <v>4973514.536159209</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -2298,19 +2304,19 @@
         <v>107</v>
       </c>
       <c r="C35">
-        <v>49808</v>
+        <v>49824</v>
       </c>
       <c r="D35">
-        <v>9.04360824742268</v>
+        <v>3.054201030927835</v>
       </c>
       <c r="E35" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F35">
         <v>1.8</v>
       </c>
       <c r="G35">
-        <v>21215963.57252571</v>
+        <v>7176830.63573128</v>
       </c>
       <c r="H35">
         <v>37855437.77268496</v>
@@ -2319,7 +2325,7 @@
         <v>100</v>
       </c>
       <c r="J35">
-        <v>4973514.536159209</v>
+        <v>3824493.385265881</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -2333,16 +2339,16 @@
         <v>49824</v>
       </c>
       <c r="D36">
-        <v>3.054201030927835</v>
+        <v>1.269278350515464</v>
       </c>
       <c r="E36" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F36">
         <v>1.8</v>
       </c>
       <c r="G36">
-        <v>7176830.63573128</v>
+        <v>2984042.160773337</v>
       </c>
       <c r="H36">
         <v>37855437.77268496</v>
@@ -2351,7 +2357,7 @@
         <v>100</v>
       </c>
       <c r="J36">
-        <v>3824493.385265881</v>
+        <v>3092355.773228031</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -2362,28 +2368,28 @@
         <v>109</v>
       </c>
       <c r="C37">
-        <v>49824</v>
+        <v>31171</v>
       </c>
       <c r="D37">
-        <v>1.269278350515464</v>
+        <v>0.9598917525773194</v>
       </c>
       <c r="E37" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F37">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="G37">
-        <v>2984042.160773337</v>
+        <v>2256873.78961794</v>
       </c>
       <c r="H37">
-        <v>37855437.77268496</v>
+        <v>38060293.37896816</v>
       </c>
       <c r="I37">
         <v>100</v>
       </c>
       <c r="J37">
-        <v>3092355.773228031</v>
+        <v>2890190.553294488</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -2400,7 +2406,7 @@
         <v>1.30101030927835</v>
       </c>
       <c r="E38" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F38">
         <v>1.9</v>
@@ -2432,7 +2438,7 @@
         <v>4.894654639175258</v>
       </c>
       <c r="E39" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F39">
         <v>1.9</v>
@@ -2464,7 +2470,7 @@
         <v>3.300123711340206</v>
       </c>
       <c r="E40" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F40">
         <v>1.9</v>
@@ -2496,7 +2502,7 @@
         <v>11.52</v>
       </c>
       <c r="E41" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F41">
         <v>2</v>
@@ -2528,7 +2534,7 @@
         <v>2.625819587628866</v>
       </c>
       <c r="E42" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F42">
         <v>2.1</v>
@@ -2560,7 +2566,7 @@
         <v>1.832520618556702</v>
       </c>
       <c r="E43" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F43">
         <v>2.3</v>
@@ -2592,7 +2598,7 @@
         <v>2.046711340206186</v>
       </c>
       <c r="E44" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F44">
         <v>2.3</v>
@@ -2624,7 +2630,7 @@
         <v>3.078</v>
       </c>
       <c r="E45" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F45">
         <v>2.3</v>
@@ -2656,7 +2662,7 @@
         <v>3.546046391752578</v>
       </c>
       <c r="E46" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F46">
         <v>2.3</v>
@@ -2685,10 +2691,10 @@
         <v>38723</v>
       </c>
       <c r="D47">
-        <v>2.665484536082474</v>
+        <v>2.665484536082475</v>
       </c>
       <c r="E47" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F47">
         <v>2.3</v>
@@ -2720,7 +2726,7 @@
         <v>11.52</v>
       </c>
       <c r="E48" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F48">
         <v>2.3</v>
@@ -2752,7 +2758,7 @@
         <v>6.39398969072165</v>
       </c>
       <c r="E49" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F49">
         <v>2.5</v>
@@ -2778,28 +2784,28 @@
         <v>122</v>
       </c>
       <c r="C50">
-        <v>37355</v>
+        <v>37218</v>
       </c>
       <c r="D50">
-        <v>8.091649484536084</v>
+        <v>2.966938144329896</v>
       </c>
       <c r="E50" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F50">
-        <v>2.9</v>
+        <v>2.7</v>
       </c>
       <c r="G50">
-        <v>18987662.48066654</v>
+        <v>6971945.468368442</v>
       </c>
       <c r="H50">
-        <v>39635749.05499732</v>
+        <v>39380047.41901974</v>
       </c>
       <c r="I50">
         <v>100</v>
       </c>
       <c r="J50">
-        <v>4841430.024186624</v>
+        <v>3797758.507656866</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -2810,28 +2816,28 @@
         <v>123</v>
       </c>
       <c r="C51">
-        <v>45329</v>
+        <v>37355</v>
       </c>
       <c r="D51">
-        <v>4.910520618556702</v>
+        <v>8.091649484536084</v>
       </c>
       <c r="E51" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F51">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="G51">
-        <v>11532970.80719121</v>
+        <v>18987662.48066654</v>
       </c>
       <c r="H51">
-        <v>39754521.5981693</v>
+        <v>39635749.05499732</v>
       </c>
       <c r="I51">
         <v>100</v>
       </c>
       <c r="J51">
-        <v>4290239.673387973</v>
+        <v>4841430.024186624</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -2842,19 +2848,19 @@
         <v>124</v>
       </c>
       <c r="C52">
-        <v>45699</v>
+        <v>45329</v>
       </c>
       <c r="D52">
-        <v>5.307170103092785</v>
+        <v>4.910520618556698</v>
       </c>
       <c r="E52" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F52">
         <v>3</v>
       </c>
       <c r="G52">
-        <v>12463194.18863161</v>
+        <v>11532970.80719121</v>
       </c>
       <c r="H52">
         <v>39754521.5981693</v>
@@ -2863,7 +2869,7 @@
         <v>100</v>
       </c>
       <c r="J52">
-        <v>4371651.546027265</v>
+        <v>4290239.673387973</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -2874,19 +2880,19 @@
         <v>125</v>
       </c>
       <c r="C53">
-        <v>45772</v>
+        <v>45699</v>
       </c>
       <c r="D53">
-        <v>11.52</v>
+        <v>5.307170103092782</v>
       </c>
       <c r="E53" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F53">
         <v>3</v>
       </c>
       <c r="G53">
-        <v>27007138.60142434</v>
+        <v>12463194.18863161</v>
       </c>
       <c r="H53">
         <v>39754521.5981693</v>
@@ -2895,7 +2901,7 @@
         <v>100</v>
       </c>
       <c r="J53">
-        <v>5273515.054654035</v>
+        <v>4371651.546027265</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -2906,13 +2912,13 @@
         <v>126</v>
       </c>
       <c r="C54">
-        <v>45896</v>
+        <v>45772</v>
       </c>
       <c r="D54">
         <v>11.52</v>
       </c>
       <c r="E54" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F54">
         <v>3</v>
@@ -2938,19 +2944,19 @@
         <v>127</v>
       </c>
       <c r="C55">
-        <v>45899</v>
+        <v>45896</v>
       </c>
       <c r="D55">
-        <v>9.122938144329899</v>
+        <v>11.52</v>
       </c>
       <c r="E55" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F55">
         <v>3</v>
       </c>
       <c r="G55">
-        <v>21401602.79478948</v>
+        <v>27007138.60142434</v>
       </c>
       <c r="H55">
         <v>39754521.5981693</v>
@@ -2959,7 +2965,7 @@
         <v>100</v>
       </c>
       <c r="J55">
-        <v>4984037.426968283</v>
+        <v>5273515.054654035</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -2970,19 +2976,19 @@
         <v>128</v>
       </c>
       <c r="C56">
-        <v>46049</v>
+        <v>45899</v>
       </c>
       <c r="D56">
-        <v>5.545159793814434</v>
+        <v>9.122938144329899</v>
       </c>
       <c r="E56" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F56">
         <v>3</v>
       </c>
       <c r="G56">
-        <v>13021230.96247917</v>
+        <v>21401602.79478948</v>
       </c>
       <c r="H56">
         <v>39754521.5981693</v>
@@ -2991,7 +2997,7 @@
         <v>100</v>
       </c>
       <c r="J56">
-        <v>4418307.05254629</v>
+        <v>4984037.426968283</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -3002,19 +3008,19 @@
         <v>129</v>
       </c>
       <c r="C57">
-        <v>47166</v>
+        <v>46049</v>
       </c>
       <c r="D57">
-        <v>11.52</v>
+        <v>5.545159793814434</v>
       </c>
       <c r="E57" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F57">
         <v>3</v>
       </c>
       <c r="G57">
-        <v>27007138.60142434</v>
+        <v>13021230.96247917</v>
       </c>
       <c r="H57">
         <v>39754521.5981693</v>
@@ -3023,7 +3029,7 @@
         <v>100</v>
       </c>
       <c r="J57">
-        <v>5273515.054654035</v>
+        <v>4418307.05254629</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -3034,19 +3040,19 @@
         <v>130</v>
       </c>
       <c r="C58">
-        <v>47166</v>
+        <v>47053</v>
       </c>
       <c r="D58">
-        <v>11.52</v>
+        <v>4.505938144329896</v>
       </c>
       <c r="E58" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F58">
         <v>3</v>
       </c>
       <c r="G58">
-        <v>27007138.60142434</v>
+        <v>10583934.16780851</v>
       </c>
       <c r="H58">
         <v>39754521.5981693</v>
@@ -3055,7 +3061,7 @@
         <v>100</v>
       </c>
       <c r="J58">
-        <v>5273515.054654035</v>
+        <v>4201890.346963244</v>
       </c>
     </row>
     <row r="59" spans="1:10">
@@ -3069,16 +3075,16 @@
         <v>47166</v>
       </c>
       <c r="D59">
-        <v>10.07489690721649</v>
+        <v>11.52</v>
       </c>
       <c r="E59" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F59">
         <v>3</v>
       </c>
       <c r="G59">
-        <v>23628643.36424644</v>
+        <v>27007138.60142434</v>
       </c>
       <c r="H59">
         <v>39754521.5981693</v>
@@ -3087,7 +3093,7 @@
         <v>100</v>
       </c>
       <c r="J59">
-        <v>5105201.851214484</v>
+        <v>5273515.054654035</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -3101,16 +3107,16 @@
         <v>47166</v>
       </c>
       <c r="D60">
-        <v>7.528407216494846</v>
+        <v>11.52</v>
       </c>
       <c r="E60" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F60">
         <v>3</v>
       </c>
       <c r="G60">
-        <v>17668702.74772677</v>
+        <v>27007138.60142434</v>
       </c>
       <c r="H60">
         <v>39754521.5981693</v>
@@ -3119,7 +3125,7 @@
         <v>100</v>
       </c>
       <c r="J60">
-        <v>4757631.938664145</v>
+        <v>5273515.054654035</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -3130,19 +3136,19 @@
         <v>133</v>
       </c>
       <c r="C61">
-        <v>47259</v>
+        <v>47166</v>
       </c>
       <c r="D61">
-        <v>11.52</v>
+        <v>10.07489690721649</v>
       </c>
       <c r="E61" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F61">
         <v>3</v>
       </c>
       <c r="G61">
-        <v>27007138.60142434</v>
+        <v>23628643.36424644</v>
       </c>
       <c r="H61">
         <v>39754521.5981693</v>
@@ -3151,7 +3157,7 @@
         <v>100</v>
       </c>
       <c r="J61">
-        <v>5273515.054654035</v>
+        <v>5105201.851214484</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -3162,19 +3168,19 @@
         <v>134</v>
       </c>
       <c r="C62">
-        <v>47495</v>
+        <v>47166</v>
       </c>
       <c r="D62">
-        <v>6.39398969072165</v>
+        <v>7.528407216494846</v>
       </c>
       <c r="E62" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F62">
         <v>3</v>
       </c>
       <c r="G62">
-        <v>15010968.32739887</v>
+        <v>17668702.74772677</v>
       </c>
       <c r="H62">
         <v>39754521.5981693</v>
@@ -3183,7 +3189,7 @@
         <v>100</v>
       </c>
       <c r="J62">
-        <v>4573255.840545377</v>
+        <v>4757631.938664145</v>
       </c>
     </row>
     <row r="63" spans="1:10">
@@ -3194,28 +3200,28 @@
         <v>135</v>
       </c>
       <c r="C63">
-        <v>42489</v>
+        <v>47166</v>
       </c>
       <c r="D63">
-        <v>11.51999999999999</v>
+        <v>3.879231958762886</v>
       </c>
       <c r="E63" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F63">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="G63">
-        <v>27007138.60142434</v>
+        <v>9113441.365831105</v>
       </c>
       <c r="H63">
-        <v>39975550.38970821</v>
+        <v>39754521.5981693</v>
       </c>
       <c r="I63">
         <v>100</v>
       </c>
       <c r="J63">
-        <v>5273515.054654035</v>
+        <v>4052333.328712357</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -3226,22 +3232,22 @@
         <v>136</v>
       </c>
       <c r="C64">
-        <v>15562</v>
+        <v>47259</v>
       </c>
       <c r="D64">
         <v>11.52</v>
       </c>
       <c r="E64" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F64">
-        <v>3.4</v>
+        <v>3</v>
       </c>
       <c r="G64">
         <v>27007138.60142434</v>
       </c>
       <c r="H64">
-        <v>40176551.31533918</v>
+        <v>39754521.5981693</v>
       </c>
       <c r="I64">
         <v>100</v>
@@ -3258,27 +3264,91 @@
         <v>137</v>
       </c>
       <c r="C65">
-        <v>6886</v>
+        <v>47495</v>
       </c>
       <c r="D65">
-        <v>11.37741958650125</v>
+        <v>6.39398969072165</v>
       </c>
       <c r="E65" t="s">
+        <v>140</v>
+      </c>
+      <c r="F65">
+        <v>3</v>
+      </c>
+      <c r="G65">
+        <v>15010968.32739887</v>
+      </c>
+      <c r="H65">
+        <v>39754521.5981693</v>
+      </c>
+      <c r="I65">
+        <v>100</v>
+      </c>
+      <c r="J65">
+        <v>4573255.840545377</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
+      <c r="A66" s="1">
+        <v>64</v>
+      </c>
+      <c r="B66" t="s">
         <v>138</v>
       </c>
-      <c r="F65">
-        <v>3.5</v>
-      </c>
-      <c r="G65">
+      <c r="C66">
+        <v>42489</v>
+      </c>
+      <c r="D66">
+        <v>11.52</v>
+      </c>
+      <c r="E66" t="s">
+        <v>140</v>
+      </c>
+      <c r="F66">
+        <v>3.2</v>
+      </c>
+      <c r="G66">
         <v>27007138.60142434</v>
       </c>
-      <c r="H65">
-        <v>40270228.28044015</v>
-      </c>
-      <c r="I65">
-        <v>100</v>
-      </c>
-      <c r="J65">
+      <c r="H66">
+        <v>39975550.38970821</v>
+      </c>
+      <c r="I66">
+        <v>100</v>
+      </c>
+      <c r="J66">
+        <v>5273515.054654035</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
+      <c r="A67" s="1">
+        <v>65</v>
+      </c>
+      <c r="B67" t="s">
+        <v>139</v>
+      </c>
+      <c r="C67">
+        <v>15562</v>
+      </c>
+      <c r="D67">
+        <v>11.45804845248085</v>
+      </c>
+      <c r="E67" t="s">
+        <v>140</v>
+      </c>
+      <c r="F67">
+        <v>3.4</v>
+      </c>
+      <c r="G67">
+        <v>27007138.60142434</v>
+      </c>
+      <c r="H67">
+        <v>40176551.31533918</v>
+      </c>
+      <c r="I67">
+        <v>100</v>
+      </c>
+      <c r="J67">
         <v>5273515.054654035</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Completed changing max by process. NOTE. the 200 needs to be changed
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -194,24 +194,24 @@
     <t>MethaneHubUsage</t>
   </si>
   <si>
+    <t>pkmUsage</t>
+  </si>
+  <si>
+    <t>tkm-SZMUsage</t>
+  </si>
+  <si>
+    <t>tkm-N1Usage</t>
+  </si>
+  <si>
+    <t>tkm-N2Usage</t>
+  </si>
+  <si>
     <t>keroseneUsage</t>
   </si>
   <si>
-    <t>tkm-N1Usage</t>
-  </si>
-  <si>
     <t>tkm-N3Usage</t>
   </si>
   <si>
-    <t>pkmUsage</t>
-  </si>
-  <si>
-    <t>tkm-N2Usage</t>
-  </si>
-  <si>
-    <t>tkm-SZMUsage</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -332,6 +332,9 @@
     <t>EEW Energy from Waste Hannover GmbH</t>
   </si>
   <si>
+    <t>Schoeller Technocell GmbH &amp; Co. KG</t>
+  </si>
+  <si>
     <t>Georgsmarienhütte GmbH</t>
   </si>
   <si>
@@ -386,9 +389,18 @@
     <t>Zellstoff Stendal GmbH</t>
   </si>
   <si>
+    <t>Werk  Zielitz</t>
+  </si>
+  <si>
+    <t>CIECH Soda Deutschland GmbH &amp; Co. KG</t>
+  </si>
+  <si>
     <t>Rheinkalk GmbH Werk Hönnetal</t>
   </si>
   <si>
+    <t>MHB Hamm Betriebsführungsgesell schaft mbH</t>
+  </si>
+  <si>
     <t>Energieversorgung DSS Paper B+T Energie GmbH</t>
   </si>
   <si>
@@ -398,12 +410,12 @@
     <t>RWE Generation SE MHKW Karnap</t>
   </si>
   <si>
+    <t>TRIMET Aluminium SE</t>
+  </si>
+  <si>
     <t>AGR mbH</t>
   </si>
   <si>
-    <t>Evonik Degussa GmbH</t>
-  </si>
-  <si>
     <t>Ruhr Oel GmbH Werk Scholven</t>
   </si>
   <si>
@@ -416,12 +428,6 @@
     <t>DK Recycling und Roheisen GmbH</t>
   </si>
   <si>
-    <t>ThyssenKrupp Steel Europe AG Werk Schwelgern</t>
-  </si>
-  <si>
-    <t>Pruna Betreiber GmbH vertreten durch die KBS GmbH Werk Schwelgern</t>
-  </si>
-  <si>
     <t>ThyssenKrupp Steel Europe AG Werk Hamborn</t>
   </si>
   <si>
@@ -431,16 +437,10 @@
     <t>ThyssenKrupp Steel Europe AG Werk Bruckhausen</t>
   </si>
   <si>
-    <t>Hüttenwerke Krupp Mannesmann GmbH</t>
+    <t>Huntsman P&amp;A Germany GmbH ehemals Sachtleben Chemie GmbH</t>
   </si>
   <si>
     <t>Solvay Chemicals GmbH</t>
-  </si>
-  <si>
-    <t>Rheinkalk GmbH</t>
-  </si>
-  <si>
-    <t>CEMEX Zement GmbH</t>
   </si>
   <si>
     <t>PtF-FT1</t>
@@ -1009,10 +1009,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>13567275360.45065</v>
+        <v>13267234387.58621</v>
       </c>
       <c r="C2">
-        <v>95.99999999999999</v>
+        <v>96.00000000000001</v>
       </c>
       <c r="D2">
         <v>1190.511948111309</v>
@@ -1024,31 +1024,31 @@
         <v>400</v>
       </c>
       <c r="G2">
-        <v>330.4949195865013</v>
+        <v>330.4949195865012</v>
       </c>
       <c r="H2">
         <v>33.82257948984662</v>
       </c>
       <c r="I2">
-        <v>858.4615384615383</v>
+        <v>858.4615384615399</v>
       </c>
       <c r="J2">
-        <v>240</v>
+        <v>240.0000000000005</v>
       </c>
       <c r="K2">
-        <v>498.4615384615384</v>
+        <v>498.4615384615393</v>
       </c>
       <c r="L2">
-        <v>120</v>
+        <v>120.0000000000002</v>
       </c>
       <c r="M2">
-        <v>248.7145732819789</v>
+        <v>248.7145732819777</v>
       </c>
       <c r="N2">
-        <v>80.88278805918016</v>
+        <v>80.88278805917975</v>
       </c>
       <c r="O2">
-        <v>167.8317852227988</v>
+        <v>167.8317852227979</v>
       </c>
       <c r="P2">
         <v>154.0911111111111</v>
@@ -1084,10 +1084,10 @@
         <v>278.3115112307378</v>
       </c>
       <c r="AA2">
-        <v>86.00598784560998</v>
+        <v>86.00598784560997</v>
       </c>
       <c r="AB2">
-        <v>192.3055233851279</v>
+        <v>192.3055233851278</v>
       </c>
       <c r="AC2">
         <v>0</v>
@@ -1108,16 +1108,16 @@
         <v>0</v>
       </c>
       <c r="AI2">
-        <v>321.2279809774659</v>
+        <v>321.227980977466</v>
       </c>
       <c r="AJ2">
-        <v>321.2279809774659</v>
+        <v>321.227980977466</v>
       </c>
       <c r="AK2">
-        <v>450.7720190225339</v>
+        <v>450.772019022534</v>
       </c>
       <c r="AL2">
-        <v>450.7720190225339</v>
+        <v>450.772019022534</v>
       </c>
       <c r="AM2">
         <v>6.75</v>
@@ -1174,7 +1174,7 @@
         <v>41.45</v>
       </c>
       <c r="BE2">
-        <v>406.8887759047901</v>
+        <v>406.8887759047903</v>
       </c>
       <c r="BF2">
         <v>1074.598847069465</v>
@@ -1186,22 +1186,22 @@
         <v>154.0911111111111</v>
       </c>
       <c r="BI2">
+        <v>858</v>
+      </c>
+      <c r="BJ2">
+        <v>414.5</v>
+      </c>
+      <c r="BK2">
+        <v>7.5</v>
+      </c>
+      <c r="BL2">
+        <v>24.2</v>
+      </c>
+      <c r="BM2">
         <v>120</v>
       </c>
-      <c r="BJ2">
-        <v>7.5</v>
-      </c>
-      <c r="BK2">
+      <c r="BN2">
         <v>130.3</v>
-      </c>
-      <c r="BL2">
-        <v>857.9999999999998</v>
-      </c>
-      <c r="BM2">
-        <v>24.2</v>
-      </c>
-      <c r="BN2">
-        <v>414.5</v>
       </c>
     </row>
   </sheetData>
@@ -1263,7 +1263,7 @@
         <v>25541</v>
       </c>
       <c r="D2">
-        <v>1.483469072164948</v>
+        <v>1.870000000000004</v>
       </c>
       <c r="E2" t="s">
         <v>142</v>
@@ -1278,13 +1278,13 @@
         <v>33331633.33333333</v>
       </c>
       <c r="I2">
-        <v>49446447.17474227</v>
+        <v>62330154.33333347</v>
       </c>
       <c r="J2">
         <v>100</v>
       </c>
       <c r="K2">
-        <v>14.83469072164948</v>
+        <v>18.70000000000004</v>
       </c>
       <c r="L2">
         <v>3211279.34822684</v>
@@ -1301,7 +1301,7 @@
         <v>25541</v>
       </c>
       <c r="D3">
-        <v>1.316876288659794</v>
+        <v>1.659999999999997</v>
       </c>
       <c r="E3" t="s">
         <v>142</v>
@@ -1316,13 +1316,13 @@
         <v>33331633.33333333</v>
       </c>
       <c r="I3">
-        <v>43893637.59896907</v>
+        <v>55330511.33333322</v>
       </c>
       <c r="J3">
         <v>100</v>
       </c>
       <c r="K3">
-        <v>13.16876288659794</v>
+        <v>16.59999999999997</v>
       </c>
       <c r="L3">
         <v>3120028.598903444</v>
@@ -1339,7 +1339,7 @@
         <v>25572</v>
       </c>
       <c r="D4">
-        <v>6.790639175257732</v>
+        <v>8.560000000000002</v>
       </c>
       <c r="E4" t="s">
         <v>142</v>
@@ -1354,13 +1354,13 @@
         <v>33429264.21745752</v>
       </c>
       <c r="I4">
-        <v>227006071.1951085</v>
+        <v>286154501.7014364</v>
       </c>
       <c r="J4">
         <v>100</v>
       </c>
       <c r="K4">
-        <v>67.90639175257732</v>
+        <v>85.60000000000002</v>
       </c>
       <c r="L4">
         <v>4640353.526253123</v>
@@ -1377,7 +1377,7 @@
         <v>25734</v>
       </c>
       <c r="D5">
-        <v>7.718798969072166</v>
+        <v>9.72999999999999</v>
       </c>
       <c r="E5" t="s">
         <v>142</v>
@@ -1392,13 +1392,13 @@
         <v>33429264.21745752</v>
       </c>
       <c r="I5">
-        <v>258033770.1785522</v>
+        <v>325266740.8358613</v>
       </c>
       <c r="J5">
         <v>100</v>
       </c>
       <c r="K5">
-        <v>77.18798969072166</v>
+        <v>97.2999999999999</v>
       </c>
       <c r="L5">
         <v>4786474.22858194</v>
@@ -1415,7 +1415,7 @@
         <v>26388</v>
       </c>
       <c r="D6">
-        <v>1.166149484536082</v>
+        <v>1.469999999999999</v>
       </c>
       <c r="E6" t="s">
         <v>142</v>
@@ -1430,13 +1430,13 @@
         <v>33429264.21745752</v>
       </c>
       <c r="I6">
-        <v>38983519.23560859</v>
+        <v>49141018.39966252</v>
       </c>
       <c r="J6">
         <v>100</v>
       </c>
       <c r="K6">
-        <v>11.66149484536082</v>
+        <v>14.69999999999999</v>
       </c>
       <c r="L6">
         <v>3029585.493423196</v>
@@ -1453,7 +1453,7 @@
         <v>25566</v>
       </c>
       <c r="D7">
-        <v>9.28159793814433</v>
+        <v>11.51999999999974</v>
       </c>
       <c r="E7" t="s">
         <v>142</v>
@@ -1468,13 +1468,13 @@
         <v>33609222.38641504</v>
       </c>
       <c r="I7">
-        <v>311947289.2043841</v>
+        <v>387178241.8914925</v>
       </c>
       <c r="J7">
         <v>100</v>
       </c>
       <c r="K7">
-        <v>92.8159793814433</v>
+        <v>115.1999999999974</v>
       </c>
       <c r="L7">
         <v>5004876.854845014</v>
@@ -1491,7 +1491,7 @@
         <v>26316</v>
       </c>
       <c r="D8">
-        <v>2.35609793814433</v>
+        <v>2.969999999999998</v>
       </c>
       <c r="E8" t="s">
         <v>142</v>
@@ -1506,13 +1506,13 @@
         <v>33609222.38641504</v>
       </c>
       <c r="I8">
-        <v>79186619.56726673</v>
+        <v>99819390.4876526</v>
       </c>
       <c r="J8">
         <v>100</v>
       </c>
       <c r="K8">
-        <v>23.5609793814433</v>
+        <v>29.69999999999998</v>
       </c>
       <c r="L8">
         <v>3591695.233391508</v>
@@ -1529,7 +1529,7 @@
         <v>26954</v>
       </c>
       <c r="D9">
-        <v>1.00748969072165</v>
+        <v>1.270000000000011</v>
       </c>
       <c r="E9" t="s">
         <v>142</v>
@@ -1544,13 +1544,13 @@
         <v>33609222.38641504</v>
       </c>
       <c r="I9">
-        <v>33860945.06748443</v>
+        <v>42683712.43074746</v>
       </c>
       <c r="J9">
         <v>100</v>
       </c>
       <c r="K9">
-        <v>10.07489690721649</v>
+        <v>12.70000000000011</v>
       </c>
       <c r="L9">
         <v>2924239.357757165</v>
@@ -1567,7 +1567,7 @@
         <v>27570</v>
       </c>
       <c r="D10">
-        <v>2.26090206185567</v>
+        <v>2.849999999999995</v>
       </c>
       <c r="E10" t="s">
         <v>142</v>
@@ -1582,13 +1582,13 @@
         <v>33609222.38641504</v>
       </c>
       <c r="I10">
-        <v>75987160.19081151</v>
+        <v>95786283.8012827</v>
       </c>
       <c r="J10">
         <v>100</v>
       </c>
       <c r="K10">
-        <v>22.6090206185567</v>
+        <v>28.49999999999995</v>
       </c>
       <c r="L10">
         <v>3556025.558079649</v>
@@ -1605,7 +1605,7 @@
         <v>26892</v>
       </c>
       <c r="D11">
-        <v>2.15777319587629</v>
+        <v>2.719999999999996</v>
       </c>
       <c r="E11" t="s">
         <v>142</v>
@@ -1620,13 +1620,13 @@
         <v>34374076.88937075</v>
       </c>
       <c r="I11">
-        <v>74171461.74487484</v>
+        <v>93497489.1390883</v>
       </c>
       <c r="J11">
         <v>100</v>
       </c>
       <c r="K11">
-        <v>21.5777319587629</v>
+        <v>27.19999999999996</v>
       </c>
       <c r="L11">
         <v>3516074.693055412</v>
@@ -1643,7 +1643,7 @@
         <v>24534</v>
       </c>
       <c r="D12">
-        <v>3.173195876288661</v>
+        <v>4</v>
       </c>
       <c r="E12" t="s">
         <v>142</v>
@@ -1658,13 +1658,13 @@
         <v>34962685.86338257</v>
       </c>
       <c r="I12">
-        <v>110943450.6056614</v>
+        <v>139850743.4535303</v>
       </c>
       <c r="J12">
         <v>100</v>
       </c>
       <c r="K12">
-        <v>31.73195876288661</v>
+        <v>40</v>
       </c>
       <c r="L12">
         <v>3860032.27064468</v>
@@ -1681,7 +1681,7 @@
         <v>20457</v>
       </c>
       <c r="D13">
-        <v>1.213747422680412</v>
+        <v>1.530000000000001</v>
       </c>
       <c r="E13" t="s">
         <v>142</v>
@@ -1696,13 +1696,13 @@
         <v>35112131.13005736</v>
       </c>
       <c r="I13">
-        <v>42617258.66392379</v>
+        <v>53721560.62898781</v>
       </c>
       <c r="J13">
         <v>100</v>
       </c>
       <c r="K13">
-        <v>12.13747422680412</v>
+        <v>15.30000000000001</v>
       </c>
       <c r="L13">
         <v>3059058.228987825</v>
@@ -1719,7 +1719,7 @@
         <v>20539</v>
       </c>
       <c r="D14">
-        <v>1.356541237113402</v>
+        <v>1.710000000000008</v>
       </c>
       <c r="E14" t="s">
         <v>142</v>
@@ -1734,13 +1734,13 @@
         <v>35112131.13005736</v>
       </c>
       <c r="I14">
-        <v>47631053.80085601</v>
+        <v>60041744.23239836</v>
       </c>
       <c r="J14">
         <v>100</v>
       </c>
       <c r="K14">
-        <v>13.56541237113402</v>
+        <v>17.10000000000008</v>
       </c>
       <c r="L14">
         <v>3142515.846107772</v>
@@ -1757,7 +1757,7 @@
         <v>21079</v>
       </c>
       <c r="D15">
-        <v>6.108402061855671</v>
+        <v>7.69999999999999</v>
       </c>
       <c r="E15" t="s">
         <v>142</v>
@@ -1772,13 +1772,13 @@
         <v>35112131.13005736</v>
       </c>
       <c r="I15">
-        <v>214479014.1909891</v>
+        <v>270363409.7014413</v>
       </c>
       <c r="J15">
         <v>100</v>
       </c>
       <c r="K15">
-        <v>61.08402061855671</v>
+        <v>76.9999999999999</v>
       </c>
       <c r="L15">
         <v>4522964.437644095</v>
@@ -1795,7 +1795,7 @@
         <v>21107</v>
       </c>
       <c r="D16">
-        <v>2.554422680412372</v>
+        <v>3.219999999999998</v>
       </c>
       <c r="E16" t="s">
         <v>142</v>
@@ -1810,13 +1810,13 @@
         <v>35112131.13005736</v>
       </c>
       <c r="I16">
-        <v>89691224.1162318</v>
+        <v>113061062.2387846</v>
       </c>
       <c r="J16">
         <v>100</v>
       </c>
       <c r="K16">
-        <v>25.54422680412372</v>
+        <v>32.19999999999998</v>
       </c>
       <c r="L16">
         <v>3662634.134160224</v>
@@ -1833,7 +1833,7 @@
         <v>21107</v>
       </c>
       <c r="D17">
-        <v>1.769056701030928</v>
+        <v>2.22999999999999</v>
       </c>
       <c r="E17" t="s">
         <v>142</v>
@@ -1848,13 +1848,13 @@
         <v>35112131.13005736</v>
       </c>
       <c r="I17">
-        <v>62115350.86310463</v>
+        <v>78300052.42002758</v>
       </c>
       <c r="J17">
         <v>100</v>
       </c>
       <c r="K17">
-        <v>17.69056701030928</v>
+        <v>22.2999999999999</v>
       </c>
       <c r="L17">
         <v>3351059.927308201</v>
@@ -1871,7 +1871,7 @@
         <v>21119</v>
       </c>
       <c r="D18">
-        <v>2.562355670103094</v>
+        <v>3.22999999999999</v>
       </c>
       <c r="E18" t="s">
         <v>142</v>
@@ -1886,13 +1886,13 @@
         <v>35112131.13005736</v>
       </c>
       <c r="I18">
-        <v>89969768.29050583</v>
+        <v>113412183.5500849</v>
       </c>
       <c r="J18">
         <v>100</v>
       </c>
       <c r="K18">
-        <v>25.62355670103094</v>
+        <v>32.2999999999999</v>
       </c>
       <c r="L18">
         <v>3665383.563029062</v>
@@ -1909,7 +1909,7 @@
         <v>21129</v>
       </c>
       <c r="D19">
-        <v>1.784922680412372</v>
+        <v>2.25</v>
       </c>
       <c r="E19" t="s">
         <v>142</v>
@@ -1924,13 +1924,13 @@
         <v>35112131.13005736</v>
       </c>
       <c r="I19">
-        <v>62672439.21165267</v>
+        <v>79002295.04262909</v>
       </c>
       <c r="J19">
         <v>100</v>
       </c>
       <c r="K19">
-        <v>17.84922680412372</v>
+        <v>22.5</v>
       </c>
       <c r="L19">
         <v>3358308.48673273</v>
@@ -1947,7 +1947,7 @@
         <v>21683</v>
       </c>
       <c r="D20">
-        <v>4.728061855670104</v>
+        <v>5.960000000000004</v>
       </c>
       <c r="E20" t="s">
         <v>142</v>
@@ -1962,13 +1962,13 @@
         <v>35112131.13005736</v>
       </c>
       <c r="I20">
-        <v>166012327.8673111</v>
+        <v>209268301.535142</v>
       </c>
       <c r="J20">
         <v>100</v>
       </c>
       <c r="K20">
-        <v>47.28061855670104</v>
+        <v>59.60000000000004</v>
       </c>
       <c r="L20">
         <v>4251106.766759329</v>
@@ -1985,7 +1985,7 @@
         <v>21683</v>
       </c>
       <c r="D21">
-        <v>3.284257731958763</v>
+        <v>4.139999999999986</v>
       </c>
       <c r="E21" t="s">
         <v>142</v>
@@ -2000,13 +2000,13 @@
         <v>35112131.13005736</v>
       </c>
       <c r="I21">
-        <v>115317288.1494409</v>
+        <v>145364222.878437</v>
       </c>
       <c r="J21">
         <v>100</v>
       </c>
       <c r="K21">
-        <v>32.84257731958763</v>
+        <v>41.39999999999986</v>
       </c>
       <c r="L21">
         <v>3892301.737650325</v>
@@ -2023,7 +2023,7 @@
         <v>22113</v>
       </c>
       <c r="D22">
-        <v>3.879231958762887</v>
+        <v>4.889999999999985</v>
       </c>
       <c r="E22" t="s">
         <v>142</v>
@@ -2038,13 +2038,13 @@
         <v>35112131.13005736</v>
       </c>
       <c r="I22">
-        <v>136208101.2199918</v>
+        <v>171698321.22598</v>
       </c>
       <c r="J22">
         <v>100</v>
       </c>
       <c r="K22">
-        <v>38.79231958762887</v>
+        <v>48.89999999999986</v>
       </c>
       <c r="L22">
         <v>4052333.328712357</v>
@@ -2061,7 +2061,7 @@
         <v>22145</v>
       </c>
       <c r="D23">
-        <v>2.562355670103093</v>
+        <v>3.229999999999991</v>
       </c>
       <c r="E23" t="s">
         <v>142</v>
@@ -2076,13 +2076,13 @@
         <v>35261419.93911113</v>
       </c>
       <c r="I23">
-        <v>90352299.31686766</v>
+        <v>113894386.4033286</v>
       </c>
       <c r="J23">
         <v>100</v>
       </c>
       <c r="K23">
-        <v>25.62355670103093</v>
+        <v>32.2999999999999</v>
       </c>
       <c r="L23">
         <v>3665383.563029062</v>
@@ -2099,7 +2099,7 @@
         <v>24114</v>
       </c>
       <c r="D24">
-        <v>1.039221649484536</v>
+        <v>1.310000000000002</v>
       </c>
       <c r="E24" t="s">
         <v>142</v>
@@ -2114,13 +2114,13 @@
         <v>35261419.93911113</v>
       </c>
       <c r="I24">
-        <v>36644430.99228998</v>
+        <v>46192460.12023566</v>
       </c>
       <c r="J24">
         <v>100</v>
       </c>
       <c r="K24">
-        <v>10.39221649484536</v>
+        <v>13.10000000000002</v>
       </c>
       <c r="L24">
         <v>2946266.794435292</v>
@@ -2137,7 +2137,7 @@
         <v>28237</v>
       </c>
       <c r="D25">
-        <v>11.52</v>
+        <v>11.52000000000001</v>
       </c>
       <c r="E25" t="s">
         <v>142</v>
@@ -2152,13 +2152,13 @@
         <v>35261419.93911113</v>
       </c>
       <c r="I25">
-        <v>406211557.6985601</v>
+        <v>406211557.6985605</v>
       </c>
       <c r="J25">
         <v>100</v>
       </c>
       <c r="K25">
-        <v>115.2</v>
+        <v>115.2000000000001</v>
       </c>
       <c r="L25">
         <v>5273515.054654035</v>
@@ -2175,7 +2175,7 @@
         <v>28237</v>
       </c>
       <c r="D26">
-        <v>4.355211340206187</v>
+        <v>5.490000000000009</v>
       </c>
       <c r="E26" t="s">
         <v>142</v>
@@ -2190,13 +2190,13 @@
         <v>35261419.93911113</v>
       </c>
       <c r="I26">
-        <v>153570935.9905894</v>
+        <v>193585195.4657204</v>
       </c>
       <c r="J26">
         <v>100</v>
       </c>
       <c r="K26">
-        <v>43.55211340206188</v>
+        <v>54.90000000000009</v>
       </c>
       <c r="L26">
         <v>4167435.864813926</v>
@@ -2213,7 +2213,7 @@
         <v>28237</v>
       </c>
       <c r="D27">
-        <v>2.133974226804124</v>
+        <v>2.689999999999959</v>
       </c>
       <c r="E27" t="s">
         <v>142</v>
@@ -2228,13 +2228,13 @@
         <v>35261419.93911113</v>
       </c>
       <c r="I27">
-        <v>75246961.35058019</v>
+        <v>94853219.63620749</v>
       </c>
       <c r="J27">
         <v>100</v>
       </c>
       <c r="K27">
-        <v>21.33974226804124</v>
+        <v>26.89999999999959</v>
       </c>
       <c r="L27">
         <v>3506650.390632065</v>
@@ -2251,7 +2251,7 @@
         <v>26197</v>
       </c>
       <c r="D28">
-        <v>9.360927835051548</v>
+        <v>11.52000000000001</v>
       </c>
       <c r="E28" t="s">
         <v>142</v>
@@ -2266,13 +2266,13 @@
         <v>35849408.31499194</v>
       </c>
       <c r="I28">
-        <v>335583724.1659365</v>
+        <v>412985183.7887076</v>
       </c>
       <c r="J28">
         <v>100</v>
       </c>
       <c r="K28">
-        <v>93.60927835051548</v>
+        <v>115.2000000000001</v>
       </c>
       <c r="L28">
         <v>5015195.456029908</v>
@@ -2289,7 +2289,7 @@
         <v>29525</v>
       </c>
       <c r="D29">
-        <v>1.308943298969072</v>
+        <v>1.650000000000005</v>
       </c>
       <c r="E29" t="s">
         <v>142</v>
@@ -2304,13 +2304,13 @@
         <v>36933299.30390043</v>
       </c>
       <c r="I29">
-        <v>48343594.63265957</v>
+        <v>60939943.85143591</v>
       </c>
       <c r="J29">
         <v>100</v>
       </c>
       <c r="K29">
-        <v>13.08943298969072</v>
+        <v>16.50000000000005</v>
       </c>
       <c r="L29">
         <v>3115469.701891457</v>
@@ -2327,7 +2327,7 @@
         <v>30659</v>
       </c>
       <c r="D30">
-        <v>1.951515463917526</v>
+        <v>2.460000000000005</v>
       </c>
       <c r="E30" t="s">
         <v>142</v>
@@ -2342,13 +2342,13 @@
         <v>37640511.58399763</v>
       </c>
       <c r="I30">
-        <v>73456040.42593816</v>
+        <v>92595658.49663435</v>
       </c>
       <c r="J30">
         <v>100</v>
       </c>
       <c r="K30">
-        <v>19.51515463917526</v>
+        <v>24.60000000000005</v>
       </c>
       <c r="L30">
         <v>3431616.232505888</v>
@@ -2362,10 +2362,10 @@
         <v>105</v>
       </c>
       <c r="C31">
-        <v>49124</v>
+        <v>49086</v>
       </c>
       <c r="D31">
-        <v>1.158216494845361</v>
+        <v>1.099999999999995</v>
       </c>
       <c r="E31" t="s">
         <v>142</v>
@@ -2374,22 +2374,22 @@
         <v>1.8</v>
       </c>
       <c r="G31">
-        <v>2723021.589861078</v>
+        <v>2051752.656756106</v>
       </c>
       <c r="H31">
         <v>37855437.77268496</v>
       </c>
       <c r="I31">
-        <v>43844792.44791586</v>
+        <v>41640981.54995326</v>
       </c>
       <c r="J31">
         <v>100</v>
       </c>
       <c r="K31">
-        <v>11.58216494845361</v>
+        <v>10.99999999999995</v>
       </c>
       <c r="L31">
-        <v>3024585.102161352</v>
+        <v>2824291.034417088</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -2400,10 +2400,10 @@
         <v>106</v>
       </c>
       <c r="C32">
-        <v>49525</v>
+        <v>49124</v>
       </c>
       <c r="D32">
-        <v>8.012319587628866</v>
+        <v>1.460000000000009</v>
       </c>
       <c r="E32" t="s">
         <v>142</v>
@@ -2412,22 +2412,22 @@
         <v>1.8</v>
       </c>
       <c r="G32">
-        <v>18801918.17235561</v>
+        <v>2723021.589861078</v>
       </c>
       <c r="H32">
         <v>37855437.77268496</v>
       </c>
       <c r="I32">
-        <v>303309865.5643494</v>
+        <v>55268939.14812037</v>
       </c>
       <c r="J32">
         <v>100</v>
       </c>
       <c r="K32">
-        <v>80.12319587628866</v>
+        <v>14.60000000000009</v>
       </c>
       <c r="L32">
-        <v>4829900.566914583</v>
+        <v>3024585.102161352</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -2438,10 +2438,10 @@
         <v>107</v>
       </c>
       <c r="C33">
-        <v>49536</v>
+        <v>49525</v>
       </c>
       <c r="D33">
-        <v>1.182015463917526</v>
+        <v>10.09999999999999</v>
       </c>
       <c r="E33" t="s">
         <v>142</v>
@@ -2450,22 +2450,22 @@
         <v>1.8</v>
       </c>
       <c r="G33">
-        <v>2778955.910854831</v>
+        <v>18801918.17235561</v>
       </c>
       <c r="H33">
         <v>37855437.77268496</v>
       </c>
       <c r="I33">
-        <v>44745712.84068125</v>
+        <v>382339921.5041179</v>
       </c>
       <c r="J33">
         <v>100</v>
       </c>
       <c r="K33">
-        <v>11.82015463917526</v>
+        <v>100.9999999999999</v>
       </c>
       <c r="L33">
-        <v>3039509.425943215</v>
+        <v>4829900.566914583</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -2476,10 +2476,10 @@
         <v>108</v>
       </c>
       <c r="C34">
-        <v>49808</v>
+        <v>49536</v>
       </c>
       <c r="D34">
-        <v>9.04360824742268</v>
+        <v>1.49000000000001</v>
       </c>
       <c r="E34" t="s">
         <v>142</v>
@@ -2488,22 +2488,22 @@
         <v>1.8</v>
       </c>
       <c r="G34">
-        <v>21215963.57252571</v>
+        <v>2778955.910854831</v>
       </c>
       <c r="H34">
         <v>37855437.77268496</v>
       </c>
       <c r="I34">
-        <v>342349749.2508498</v>
+        <v>56404602.28130095</v>
       </c>
       <c r="J34">
         <v>100</v>
       </c>
       <c r="K34">
-        <v>90.43608247422681</v>
+        <v>14.90000000000009</v>
       </c>
       <c r="L34">
-        <v>4973514.536159209</v>
+        <v>3039509.425943215</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -2514,10 +2514,10 @@
         <v>109</v>
       </c>
       <c r="C35">
-        <v>49824</v>
+        <v>49808</v>
       </c>
       <c r="D35">
-        <v>3.054201030927835</v>
+        <v>11.40000000000001</v>
       </c>
       <c r="E35" t="s">
         <v>142</v>
@@ -2526,22 +2526,22 @@
         <v>1.8</v>
       </c>
       <c r="G35">
-        <v>7176830.63573128</v>
+        <v>21215963.57252571</v>
       </c>
       <c r="H35">
         <v>37855437.77268496</v>
       </c>
       <c r="I35">
-        <v>115618117.0715589</v>
+        <v>431551990.6086088</v>
       </c>
       <c r="J35">
         <v>100</v>
       </c>
       <c r="K35">
-        <v>30.54201030927835</v>
+        <v>114.0000000000001</v>
       </c>
       <c r="L35">
-        <v>3824493.385265881</v>
+        <v>4973514.536159209</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -2555,7 +2555,7 @@
         <v>49824</v>
       </c>
       <c r="D36">
-        <v>1.269278350515464</v>
+        <v>3.849999999999994</v>
       </c>
       <c r="E36" t="s">
         <v>142</v>
@@ -2564,22 +2564,22 @@
         <v>1.8</v>
       </c>
       <c r="G36">
-        <v>2984042.160773337</v>
+        <v>7176830.63573128</v>
       </c>
       <c r="H36">
         <v>37855437.77268496</v>
       </c>
       <c r="I36">
-        <v>48049087.61415436</v>
+        <v>145743435.4248369</v>
       </c>
       <c r="J36">
         <v>100</v>
       </c>
       <c r="K36">
-        <v>12.69278350515464</v>
+        <v>38.49999999999994</v>
       </c>
       <c r="L36">
-        <v>3092355.773228031</v>
+        <v>3824493.385265881</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -2590,34 +2590,34 @@
         <v>111</v>
       </c>
       <c r="C37">
-        <v>31171</v>
+        <v>49824</v>
       </c>
       <c r="D37">
-        <v>0.9598917525773196</v>
+        <v>1.599999999999977</v>
       </c>
       <c r="E37" t="s">
         <v>142</v>
       </c>
       <c r="F37">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="G37">
-        <v>2256873.78961794</v>
+        <v>2984042.160773337</v>
       </c>
       <c r="H37">
-        <v>38060293.37896816</v>
+        <v>37855437.77268496</v>
       </c>
       <c r="I37">
-        <v>36533761.71514471</v>
+        <v>60568700.43629505</v>
       </c>
       <c r="J37">
         <v>100</v>
       </c>
       <c r="K37">
-        <v>9.598917525773196</v>
+        <v>15.99999999999977</v>
       </c>
       <c r="L37">
-        <v>2890190.553294488</v>
+        <v>3092355.773228031</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -2628,10 +2628,10 @@
         <v>112</v>
       </c>
       <c r="C38">
-        <v>31226</v>
+        <v>31171</v>
       </c>
       <c r="D38">
-        <v>1.30101030927835</v>
+        <v>1.210000000000012</v>
       </c>
       <c r="E38" t="s">
         <v>142</v>
@@ -2640,22 +2640,22 @@
         <v>1.9</v>
       </c>
       <c r="G38">
-        <v>3058616.539902832</v>
+        <v>2256873.78961794</v>
       </c>
       <c r="H38">
         <v>38060293.37896816</v>
       </c>
       <c r="I38">
-        <v>49516834.06019612</v>
+        <v>46052954.98855191</v>
       </c>
       <c r="J38">
         <v>100</v>
       </c>
       <c r="K38">
-        <v>13.0101030927835</v>
+        <v>12.10000000000012</v>
       </c>
       <c r="L38">
-        <v>3110889.813225406</v>
+        <v>2890190.553294488</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -2666,10 +2666,10 @@
         <v>113</v>
       </c>
       <c r="C39">
-        <v>31319</v>
+        <v>31226</v>
       </c>
       <c r="D39">
-        <v>4.894654639175258</v>
+        <v>1.639999999999986</v>
       </c>
       <c r="E39" t="s">
         <v>142</v>
@@ -2678,22 +2678,22 @@
         <v>1.9</v>
       </c>
       <c r="G39">
-        <v>11495757.65683257</v>
+        <v>3058616.539902832</v>
       </c>
       <c r="H39">
         <v>38060293.37896816</v>
       </c>
       <c r="I39">
-        <v>186291991.5557379</v>
+        <v>62418881.14150725</v>
       </c>
       <c r="J39">
         <v>100</v>
       </c>
       <c r="K39">
-        <v>48.94654639175258</v>
+        <v>16.39999999999986</v>
       </c>
       <c r="L39">
-        <v>4286880.992309345</v>
+        <v>3110889.813225406</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -2704,10 +2704,10 @@
         <v>114</v>
       </c>
       <c r="C40">
-        <v>31789</v>
+        <v>31319</v>
       </c>
       <c r="D40">
-        <v>3.300123711340206</v>
+        <v>6.169999999999987</v>
       </c>
       <c r="E40" t="s">
         <v>142</v>
@@ -2716,22 +2716,22 @@
         <v>1.9</v>
       </c>
       <c r="G40">
-        <v>7754181.439418147</v>
+        <v>11495757.65683257</v>
       </c>
       <c r="H40">
         <v>38060293.37896816</v>
       </c>
       <c r="I40">
-        <v>125603676.6404975</v>
+        <v>234832010.1482331</v>
       </c>
       <c r="J40">
         <v>100</v>
       </c>
       <c r="K40">
-        <v>33.00123711340206</v>
+        <v>61.69999999999987</v>
       </c>
       <c r="L40">
-        <v>3896843.850100604</v>
+        <v>4286880.992309345</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -2742,34 +2742,34 @@
         <v>115</v>
       </c>
       <c r="C41">
-        <v>38239</v>
+        <v>31789</v>
       </c>
       <c r="D41">
-        <v>11.52</v>
+        <v>4.159999999999997</v>
       </c>
       <c r="E41" t="s">
         <v>142</v>
       </c>
       <c r="F41">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="G41">
-        <v>27007138.60142434</v>
+        <v>7754181.439418147</v>
       </c>
       <c r="H41">
-        <v>38255392.02166688</v>
+        <v>38060293.37896816</v>
       </c>
       <c r="I41">
-        <v>440702116.0896024</v>
+        <v>158330820.4565074</v>
       </c>
       <c r="J41">
         <v>100</v>
       </c>
       <c r="K41">
-        <v>115.2</v>
+        <v>41.59999999999997</v>
       </c>
       <c r="L41">
-        <v>5273515.054654035</v>
+        <v>3896843.850100604</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -2780,34 +2780,34 @@
         <v>116</v>
       </c>
       <c r="C42">
-        <v>31061</v>
+        <v>38239</v>
       </c>
       <c r="D42">
-        <v>2.625819587628866</v>
+        <v>11.52000000000001</v>
       </c>
       <c r="E42" t="s">
         <v>142</v>
       </c>
       <c r="F42">
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="G42">
-        <v>6170936.453752637</v>
+        <v>27007138.60142434</v>
       </c>
       <c r="H42">
-        <v>38441090.93970785</v>
+        <v>38255392.02166688</v>
       </c>
       <c r="I42">
-        <v>100939369.5593074</v>
+        <v>440702116.0896028</v>
       </c>
       <c r="J42">
         <v>100</v>
       </c>
       <c r="K42">
-        <v>26.25819587628866</v>
+        <v>115.2000000000001</v>
       </c>
       <c r="L42">
-        <v>3687149.882920415</v>
+        <v>5273515.054654035</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -2818,34 +2818,34 @@
         <v>117</v>
       </c>
       <c r="C43">
-        <v>33106</v>
+        <v>31061</v>
       </c>
       <c r="D43">
-        <v>1.832520618556701</v>
+        <v>3.31</v>
       </c>
       <c r="E43" t="s">
         <v>142</v>
       </c>
       <c r="F43">
-        <v>2.3</v>
+        <v>2.1</v>
       </c>
       <c r="G43">
-        <v>4307544.049353574</v>
+        <v>6170936.453752637</v>
       </c>
       <c r="H43">
-        <v>38785844.374162</v>
+        <v>38441090.93970785</v>
       </c>
       <c r="I43">
-        <v>71075859.52378328</v>
+        <v>127240011.010433</v>
       </c>
       <c r="J43">
         <v>100</v>
       </c>
       <c r="K43">
-        <v>18.32520618556701</v>
+        <v>33.09999999999999</v>
       </c>
       <c r="L43">
-        <v>3379765.097364126</v>
+        <v>3687149.882920415</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -2856,10 +2856,10 @@
         <v>118</v>
       </c>
       <c r="C44">
-        <v>33332</v>
+        <v>33106</v>
       </c>
       <c r="D44">
-        <v>2.046711340206186</v>
+        <v>2.310000000000001</v>
       </c>
       <c r="E44" t="s">
         <v>142</v>
@@ -2868,22 +2868,22 @@
         <v>2.3</v>
       </c>
       <c r="G44">
-        <v>4810740.062798683</v>
+        <v>4307544.049353574</v>
       </c>
       <c r="H44">
         <v>38785844.374162</v>
       </c>
       <c r="I44">
-        <v>79383427.52006964</v>
+        <v>89595300.50431426</v>
       </c>
       <c r="J44">
         <v>100</v>
       </c>
       <c r="K44">
-        <v>20.46711340206186</v>
+        <v>23.10000000000002</v>
       </c>
       <c r="L44">
-        <v>3471397.820165223</v>
+        <v>3379765.097364126</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -2894,10 +2894,10 @@
         <v>119</v>
       </c>
       <c r="C45">
-        <v>33609</v>
+        <v>33332</v>
       </c>
       <c r="D45">
-        <v>3.078</v>
+        <v>2.580000000000013</v>
       </c>
       <c r="E45" t="s">
         <v>142</v>
@@ -2906,22 +2906,22 @@
         <v>2.3</v>
       </c>
       <c r="G45">
-        <v>7232706.703717464</v>
+        <v>4810740.062798683</v>
       </c>
       <c r="H45">
         <v>38785844.374162</v>
       </c>
       <c r="I45">
-        <v>119382828.9836706</v>
+        <v>100067478.4853384</v>
       </c>
       <c r="J45">
         <v>100</v>
       </c>
       <c r="K45">
-        <v>30.78</v>
+        <v>25.80000000000013</v>
       </c>
       <c r="L45">
-        <v>3831684.085287054</v>
+        <v>3471397.820165223</v>
       </c>
     </row>
     <row r="46" spans="1:12">
@@ -2932,10 +2932,10 @@
         <v>120</v>
       </c>
       <c r="C46">
-        <v>38372</v>
+        <v>33609</v>
       </c>
       <c r="D46">
-        <v>3.546046391752578</v>
+        <v>3.879999999999999</v>
       </c>
       <c r="E46" t="s">
         <v>142</v>
@@ -2944,22 +2944,22 @@
         <v>2.3</v>
       </c>
       <c r="G46">
-        <v>8331454.23855985</v>
+        <v>7232706.703717464</v>
       </c>
       <c r="H46">
         <v>38785844.374162</v>
       </c>
       <c r="I46">
-        <v>137536403.4940742</v>
+        <v>150489076.1717485</v>
       </c>
       <c r="J46">
         <v>100</v>
       </c>
       <c r="K46">
-        <v>35.46046391752579</v>
+        <v>38.79999999999999</v>
       </c>
       <c r="L46">
-        <v>3965215.892681056</v>
+        <v>3831684.085287054</v>
       </c>
     </row>
     <row r="47" spans="1:12">
@@ -2970,10 +2970,10 @@
         <v>121</v>
       </c>
       <c r="C47">
-        <v>38723</v>
+        <v>38372</v>
       </c>
       <c r="D47">
-        <v>2.665484536082475</v>
+        <v>4.469999999999999</v>
       </c>
       <c r="E47" t="s">
         <v>142</v>
@@ -2982,22 +2982,22 @@
         <v>2.3</v>
       </c>
       <c r="G47">
-        <v>6264084.751326288</v>
+        <v>8331454.23855985</v>
       </c>
       <c r="H47">
         <v>38785844.374162</v>
       </c>
       <c r="I47">
-        <v>103383068.3982303</v>
+        <v>173372724.3525041</v>
       </c>
       <c r="J47">
         <v>100</v>
       </c>
       <c r="K47">
-        <v>26.65484536082475</v>
+        <v>44.69999999999999</v>
       </c>
       <c r="L47">
-        <v>3700552.097367561</v>
+        <v>3965215.892681056</v>
       </c>
     </row>
     <row r="48" spans="1:12">
@@ -3008,10 +3008,10 @@
         <v>122</v>
       </c>
       <c r="C48">
-        <v>39596</v>
+        <v>38723</v>
       </c>
       <c r="D48">
-        <v>11.52</v>
+        <v>3.360000000000013</v>
       </c>
       <c r="E48" t="s">
         <v>142</v>
@@ -3020,22 +3020,22 @@
         <v>2.3</v>
       </c>
       <c r="G48">
-        <v>27007138.60142434</v>
+        <v>6264084.751326288</v>
       </c>
       <c r="H48">
         <v>38785844.374162</v>
       </c>
       <c r="I48">
-        <v>446812927.1903462</v>
+        <v>130320437.0971848</v>
       </c>
       <c r="J48">
         <v>100</v>
       </c>
       <c r="K48">
-        <v>115.2</v>
+        <v>33.60000000000013</v>
       </c>
       <c r="L48">
-        <v>5273515.054654035</v>
+        <v>3700552.097367561</v>
       </c>
     </row>
     <row r="49" spans="1:12">
@@ -3046,34 +3046,34 @@
         <v>123</v>
       </c>
       <c r="C49">
-        <v>58710</v>
+        <v>39596</v>
       </c>
       <c r="D49">
-        <v>6.39398969072165</v>
+        <v>11.52000000000001</v>
       </c>
       <c r="E49" t="s">
         <v>142</v>
       </c>
       <c r="F49">
-        <v>2.5</v>
+        <v>2.3</v>
       </c>
       <c r="G49">
-        <v>15010968.32739887</v>
+        <v>27007138.60142434</v>
       </c>
       <c r="H49">
-        <v>39097761.98338025</v>
+        <v>38785844.374162</v>
       </c>
       <c r="I49">
-        <v>249990687.0520222</v>
+        <v>446812927.1903466</v>
       </c>
       <c r="J49">
         <v>100</v>
       </c>
       <c r="K49">
-        <v>63.9398969072165</v>
+        <v>115.2000000000001</v>
       </c>
       <c r="L49">
-        <v>4573255.840545377</v>
+        <v>5273515.054654035</v>
       </c>
     </row>
     <row r="50" spans="1:12">
@@ -3084,34 +3084,34 @@
         <v>124</v>
       </c>
       <c r="C50">
-        <v>37218</v>
+        <v>39326</v>
       </c>
       <c r="D50">
-        <v>2.966938144329897</v>
+        <v>2.55000000000001</v>
       </c>
       <c r="E50" t="s">
         <v>142</v>
       </c>
       <c r="F50">
-        <v>2.7</v>
+        <v>2.5</v>
       </c>
       <c r="G50">
-        <v>6971945.468368442</v>
+        <v>4754832.319820861</v>
       </c>
       <c r="H50">
-        <v>39380047.41901974</v>
+        <v>39097761.98338025</v>
       </c>
       <c r="I50">
-        <v>116838164.8130098</v>
+        <v>99699293.05762005</v>
       </c>
       <c r="J50">
         <v>100</v>
       </c>
       <c r="K50">
-        <v>29.66938144329897</v>
+        <v>25.50000000000011</v>
       </c>
       <c r="L50">
-        <v>3797758.507656866</v>
+        <v>3461586.123553794</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -3122,34 +3122,34 @@
         <v>125</v>
       </c>
       <c r="C51">
-        <v>37355</v>
+        <v>39418</v>
       </c>
       <c r="D51">
-        <v>8.091649484536084</v>
+        <v>1.960000000000008</v>
       </c>
       <c r="E51" t="s">
         <v>142</v>
       </c>
       <c r="F51">
-        <v>2.9</v>
+        <v>2.5</v>
       </c>
       <c r="G51">
-        <v>18987662.48066654</v>
+        <v>3655164.748267355</v>
       </c>
       <c r="H51">
-        <v>39635749.05499732</v>
+        <v>39097761.98338025</v>
       </c>
       <c r="I51">
-        <v>320718588.4100707</v>
+        <v>76631613.4874256</v>
       </c>
       <c r="J51">
         <v>100</v>
       </c>
       <c r="K51">
-        <v>80.91649484536084</v>
+        <v>19.60000000000008</v>
       </c>
       <c r="L51">
-        <v>4841430.024186624</v>
+        <v>3248017.696927753</v>
       </c>
     </row>
     <row r="52" spans="1:12">
@@ -3160,34 +3160,34 @@
         <v>126</v>
       </c>
       <c r="C52">
-        <v>45329</v>
+        <v>58710</v>
       </c>
       <c r="D52">
-        <v>4.910520618556701</v>
+        <v>8.060000000000002</v>
       </c>
       <c r="E52" t="s">
         <v>142</v>
       </c>
       <c r="F52">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="G52">
-        <v>11532970.80719121</v>
+        <v>15010968.32739887</v>
       </c>
       <c r="H52">
-        <v>39754521.5981693</v>
+        <v>39097761.98338025</v>
       </c>
       <c r="I52">
-        <v>195215397.988668</v>
+        <v>315127961.5860449</v>
       </c>
       <c r="J52">
         <v>100</v>
       </c>
       <c r="K52">
-        <v>49.10520618556701</v>
+        <v>80.60000000000002</v>
       </c>
       <c r="L52">
-        <v>4290239.673387973</v>
+        <v>4573255.840545377</v>
       </c>
     </row>
     <row r="53" spans="1:12">
@@ -3198,34 +3198,34 @@
         <v>127</v>
       </c>
       <c r="C53">
-        <v>45699</v>
+        <v>59075</v>
       </c>
       <c r="D53">
-        <v>5.307170103092785</v>
+        <v>2.55000000000001</v>
       </c>
       <c r="E53" t="s">
         <v>142</v>
       </c>
       <c r="F53">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="G53">
-        <v>12463194.18863161</v>
+        <v>4754832.319820861</v>
       </c>
       <c r="H53">
-        <v>39754521.5981693</v>
+        <v>39097761.98338025</v>
       </c>
       <c r="I53">
-        <v>210984008.4885605</v>
+        <v>99699293.05762005</v>
       </c>
       <c r="J53">
         <v>100</v>
       </c>
       <c r="K53">
-        <v>53.07170103092785</v>
+        <v>25.50000000000011</v>
       </c>
       <c r="L53">
-        <v>4371651.546027265</v>
+        <v>3461586.123553794</v>
       </c>
     </row>
     <row r="54" spans="1:12">
@@ -3236,34 +3236,34 @@
         <v>128</v>
       </c>
       <c r="C54">
-        <v>45772</v>
+        <v>37218</v>
       </c>
       <c r="D54">
-        <v>11.52</v>
+        <v>3.740000000000009</v>
       </c>
       <c r="E54" t="s">
         <v>142</v>
       </c>
       <c r="F54">
-        <v>3</v>
+        <v>2.7</v>
       </c>
       <c r="G54">
-        <v>27007138.60142434</v>
+        <v>6971945.468368442</v>
       </c>
       <c r="H54">
-        <v>39754521.5981693</v>
+        <v>39380047.41901974</v>
       </c>
       <c r="I54">
-        <v>457972088.8109103</v>
+        <v>147281377.3471342</v>
       </c>
       <c r="J54">
         <v>100</v>
       </c>
       <c r="K54">
-        <v>115.2</v>
+        <v>37.40000000000009</v>
       </c>
       <c r="L54">
-        <v>5273515.054654035</v>
+        <v>3797758.507656866</v>
       </c>
     </row>
     <row r="55" spans="1:12">
@@ -3274,34 +3274,34 @@
         <v>129</v>
       </c>
       <c r="C55">
-        <v>45896</v>
+        <v>37355</v>
       </c>
       <c r="D55">
-        <v>11.51999999999999</v>
+        <v>10.19999999999999</v>
       </c>
       <c r="E55" t="s">
         <v>142</v>
       </c>
       <c r="F55">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="G55">
-        <v>27007138.60142434</v>
+        <v>18987662.48066654</v>
       </c>
       <c r="H55">
-        <v>39754521.5981693</v>
+        <v>39635749.05499732</v>
       </c>
       <c r="I55">
-        <v>457972088.81091</v>
+        <v>404284640.3609723</v>
       </c>
       <c r="J55">
         <v>100</v>
       </c>
       <c r="K55">
-        <v>115.1999999999999</v>
+        <v>101.9999999999999</v>
       </c>
       <c r="L55">
-        <v>5273515.054654035</v>
+        <v>4841430.024186624</v>
       </c>
     </row>
     <row r="56" spans="1:12">
@@ -3312,10 +3312,10 @@
         <v>130</v>
       </c>
       <c r="C56">
-        <v>45899</v>
+        <v>45329</v>
       </c>
       <c r="D56">
-        <v>9.122938144329895</v>
+        <v>6.189999999999999</v>
       </c>
       <c r="E56" t="s">
         <v>142</v>
@@ -3324,22 +3324,22 @@
         <v>3</v>
       </c>
       <c r="G56">
-        <v>21401602.79478948</v>
+        <v>11532970.80719121</v>
       </c>
       <c r="H56">
         <v>39754521.5981693</v>
       </c>
       <c r="I56">
-        <v>362678041.4975253</v>
+        <v>246080488.6926679</v>
       </c>
       <c r="J56">
         <v>100</v>
       </c>
       <c r="K56">
-        <v>91.22938144329895</v>
+        <v>61.89999999999998</v>
       </c>
       <c r="L56">
-        <v>4984037.426968283</v>
+        <v>4290239.673387973</v>
       </c>
     </row>
     <row r="57" spans="1:12">
@@ -3350,10 +3350,10 @@
         <v>131</v>
       </c>
       <c r="C57">
-        <v>46049</v>
+        <v>45356</v>
       </c>
       <c r="D57">
-        <v>5.545159793814434</v>
+        <v>2.494919586501069</v>
       </c>
       <c r="E57" t="s">
         <v>142</v>
@@ -3362,22 +3362,22 @@
         <v>3</v>
       </c>
       <c r="G57">
-        <v>13021230.96247917</v>
+        <v>4997093.924883411</v>
       </c>
       <c r="H57">
         <v>39754521.5981693</v>
       </c>
       <c r="I57">
-        <v>220445174.7884959</v>
+        <v>99184334.58725238</v>
       </c>
       <c r="J57">
         <v>100</v>
       </c>
       <c r="K57">
-        <v>55.45159793814434</v>
+        <v>24.94919586501069</v>
       </c>
       <c r="L57">
-        <v>4418307.05254629</v>
+        <v>3503491.254460279</v>
       </c>
     </row>
     <row r="58" spans="1:12">
@@ -3388,10 +3388,10 @@
         <v>132</v>
       </c>
       <c r="C58">
-        <v>47053</v>
+        <v>45699</v>
       </c>
       <c r="D58">
-        <v>4.505938144329896</v>
+        <v>6.689999999999998</v>
       </c>
       <c r="E58" t="s">
         <v>142</v>
@@ -3400,22 +3400,22 @@
         <v>3</v>
       </c>
       <c r="G58">
-        <v>10583934.16780851</v>
+        <v>12463194.18863161</v>
       </c>
       <c r="H58">
         <v>39754521.5981693</v>
       </c>
       <c r="I58">
-        <v>179131415.2787777</v>
+        <v>265957749.4917525</v>
       </c>
       <c r="J58">
         <v>100</v>
       </c>
       <c r="K58">
-        <v>45.05938144329896</v>
+        <v>66.89999999999998</v>
       </c>
       <c r="L58">
-        <v>4201890.346963244</v>
+        <v>4371651.546027265</v>
       </c>
     </row>
     <row r="59" spans="1:12">
@@ -3426,10 +3426,10 @@
         <v>133</v>
       </c>
       <c r="C59">
-        <v>47166</v>
+        <v>45896</v>
       </c>
       <c r="D59">
-        <v>11.52</v>
+        <v>11.51999999999998</v>
       </c>
       <c r="E59" t="s">
         <v>142</v>
@@ -3444,13 +3444,13 @@
         <v>39754521.5981693</v>
       </c>
       <c r="I59">
-        <v>457972088.8109103</v>
+        <v>457972088.8109096</v>
       </c>
       <c r="J59">
         <v>100</v>
       </c>
       <c r="K59">
-        <v>115.2</v>
+        <v>115.1999999999998</v>
       </c>
       <c r="L59">
         <v>5273515.054654035</v>
@@ -3464,10 +3464,10 @@
         <v>134</v>
       </c>
       <c r="C60">
-        <v>47166</v>
+        <v>45899</v>
       </c>
       <c r="D60">
-        <v>11.52</v>
+        <v>11.50000000000002</v>
       </c>
       <c r="E60" t="s">
         <v>142</v>
@@ -3476,22 +3476,22 @@
         <v>3</v>
       </c>
       <c r="G60">
-        <v>27007138.60142434</v>
+        <v>21401602.79478948</v>
       </c>
       <c r="H60">
         <v>39754521.5981693</v>
       </c>
       <c r="I60">
-        <v>457972088.8109102</v>
+        <v>457176998.3789477</v>
       </c>
       <c r="J60">
         <v>100</v>
       </c>
       <c r="K60">
-        <v>115.2</v>
+        <v>115.0000000000002</v>
       </c>
       <c r="L60">
-        <v>5273515.054654035</v>
+        <v>4984037.426968283</v>
       </c>
     </row>
     <row r="61" spans="1:12">
@@ -3502,10 +3502,10 @@
         <v>135</v>
       </c>
       <c r="C61">
-        <v>47166</v>
+        <v>46049</v>
       </c>
       <c r="D61">
-        <v>10.07489690721649</v>
+        <v>6.99000000000001</v>
       </c>
       <c r="E61" t="s">
         <v>142</v>
@@ -3514,22 +3514,22 @@
         <v>3</v>
       </c>
       <c r="G61">
-        <v>23628643.36424644</v>
+        <v>13021230.96247917</v>
       </c>
       <c r="H61">
         <v>39754521.5981693</v>
       </c>
       <c r="I61">
-        <v>400522706.6972671</v>
+        <v>277884105.9712038</v>
       </c>
       <c r="J61">
         <v>100</v>
       </c>
       <c r="K61">
-        <v>100.7489690721649</v>
+        <v>69.90000000000011</v>
       </c>
       <c r="L61">
-        <v>5105201.851214484</v>
+        <v>4418307.05254629</v>
       </c>
     </row>
     <row r="62" spans="1:12">
@@ -3540,10 +3540,10 @@
         <v>136</v>
       </c>
       <c r="C62">
-        <v>47166</v>
+        <v>47053</v>
       </c>
       <c r="D62">
-        <v>7.528407216494845</v>
+        <v>5.680000000000001</v>
       </c>
       <c r="E62" t="s">
         <v>142</v>
@@ -3552,22 +3552,22 @@
         <v>3</v>
       </c>
       <c r="G62">
-        <v>17668702.74772677</v>
+        <v>10583934.16780851</v>
       </c>
       <c r="H62">
         <v>39754521.5981693</v>
       </c>
       <c r="I62">
-        <v>299288227.2879579</v>
+        <v>225805682.6776016</v>
       </c>
       <c r="J62">
         <v>100</v>
       </c>
       <c r="K62">
-        <v>75.28407216494844</v>
+        <v>56.8</v>
       </c>
       <c r="L62">
-        <v>4757631.938664145</v>
+        <v>4201890.346963244</v>
       </c>
     </row>
     <row r="63" spans="1:12">
@@ -3581,7 +3581,7 @@
         <v>47166</v>
       </c>
       <c r="D63">
-        <v>3.879231958762888</v>
+        <v>11.52000000000001</v>
       </c>
       <c r="E63" t="s">
         <v>142</v>
@@ -3590,22 +3590,22 @@
         <v>3</v>
       </c>
       <c r="G63">
-        <v>9113441.365831105</v>
+        <v>23628643.36424644</v>
       </c>
       <c r="H63">
         <v>39754521.5981693</v>
       </c>
       <c r="I63">
-        <v>154217010.6889478</v>
+        <v>457972088.8109106</v>
       </c>
       <c r="J63">
         <v>100</v>
       </c>
       <c r="K63">
-        <v>38.79231958762887</v>
+        <v>115.2000000000001</v>
       </c>
       <c r="L63">
-        <v>4052333.328712357</v>
+        <v>5105201.851214484</v>
       </c>
     </row>
     <row r="64" spans="1:12">
@@ -3616,10 +3616,10 @@
         <v>138</v>
       </c>
       <c r="C64">
-        <v>47259</v>
+        <v>47166</v>
       </c>
       <c r="D64">
-        <v>11.52</v>
+        <v>9.490000000000011</v>
       </c>
       <c r="E64" t="s">
         <v>142</v>
@@ -3628,22 +3628,22 @@
         <v>3</v>
       </c>
       <c r="G64">
-        <v>27007138.60142434</v>
+        <v>17668702.74772677</v>
       </c>
       <c r="H64">
         <v>39754521.5981693</v>
       </c>
       <c r="I64">
-        <v>457972088.8109103</v>
+        <v>377270409.9666271</v>
       </c>
       <c r="J64">
         <v>100</v>
       </c>
       <c r="K64">
-        <v>115.2</v>
+        <v>94.90000000000011</v>
       </c>
       <c r="L64">
-        <v>5273515.054654035</v>
+        <v>4757631.938664145</v>
       </c>
     </row>
     <row r="65" spans="1:12">
@@ -3654,10 +3654,10 @@
         <v>139</v>
       </c>
       <c r="C65">
-        <v>47495</v>
+        <v>47166</v>
       </c>
       <c r="D65">
-        <v>6.39398969072165</v>
+        <v>4.889999999999986</v>
       </c>
       <c r="E65" t="s">
         <v>142</v>
@@ -3666,22 +3666,22 @@
         <v>3</v>
       </c>
       <c r="G65">
-        <v>15010968.32739887</v>
+        <v>9113441.365831105</v>
       </c>
       <c r="H65">
         <v>39754521.5981693</v>
       </c>
       <c r="I65">
-        <v>254190001.2582656</v>
+        <v>194399610.6150473</v>
       </c>
       <c r="J65">
         <v>100</v>
       </c>
       <c r="K65">
-        <v>63.9398969072165</v>
+        <v>48.89999999999986</v>
       </c>
       <c r="L65">
-        <v>4573255.840545377</v>
+        <v>4052333.328712357</v>
       </c>
     </row>
     <row r="66" spans="1:12">
@@ -3692,34 +3692,34 @@
         <v>140</v>
       </c>
       <c r="C66">
-        <v>42489</v>
+        <v>47198</v>
       </c>
       <c r="D66">
-        <v>11.52</v>
+        <v>3.930000000000007</v>
       </c>
       <c r="E66" t="s">
         <v>142</v>
       </c>
       <c r="F66">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="G66">
-        <v>27007138.60142434</v>
+        <v>7325831.86001466</v>
       </c>
       <c r="H66">
-        <v>39975550.38970821</v>
+        <v>39754521.5981693</v>
       </c>
       <c r="I66">
-        <v>460518340.4894385</v>
+        <v>156235269.8808056</v>
       </c>
       <c r="J66">
         <v>100</v>
       </c>
       <c r="K66">
-        <v>115.2</v>
+        <v>39.30000000000007</v>
       </c>
       <c r="L66">
-        <v>5273515.054654035</v>
+        <v>3843575.485457812</v>
       </c>
     </row>
     <row r="67" spans="1:12">
@@ -3730,34 +3730,34 @@
         <v>141</v>
       </c>
       <c r="C67">
-        <v>15562</v>
+        <v>47495</v>
       </c>
       <c r="D67">
-        <v>11.4580484524807</v>
+        <v>8.060000000000002</v>
       </c>
       <c r="E67" t="s">
         <v>142</v>
       </c>
       <c r="F67">
-        <v>3.4</v>
+        <v>3</v>
       </c>
       <c r="G67">
-        <v>27007138.60142434</v>
+        <v>15010968.32739887</v>
       </c>
       <c r="H67">
-        <v>40176551.31533918</v>
+        <v>39754521.5981693</v>
       </c>
       <c r="I67">
-        <v>460344871.6247333</v>
+        <v>320421444.0812446</v>
       </c>
       <c r="J67">
         <v>100</v>
       </c>
       <c r="K67">
-        <v>114.580484524807</v>
+        <v>80.60000000000002</v>
       </c>
       <c r="L67">
-        <v>5273515.054654035</v>
+        <v>4573255.840545377</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented changing capex/K costs by process. Complete. Deleted old way,
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="204">
   <si>
     <t>Total Cost</t>
   </si>
@@ -194,24 +194,24 @@
     <t>MethaneHubUsage</t>
   </si>
   <si>
+    <t>tkm-N3Usage</t>
+  </si>
+  <si>
+    <t>tkm-SZMUsage</t>
+  </si>
+  <si>
     <t>pkmUsage</t>
   </si>
   <si>
+    <t>keroseneUsage</t>
+  </si>
+  <si>
+    <t>tkm-N1Usage</t>
+  </si>
+  <si>
     <t>tkm-N2Usage</t>
   </si>
   <si>
-    <t>tkm-N3Usage</t>
-  </si>
-  <si>
-    <t>tkm-N1Usage</t>
-  </si>
-  <si>
-    <t>tkm-SZMUsage</t>
-  </si>
-  <si>
-    <t>keroseneUsage</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -389,6 +389,12 @@
     <t>Zellstoff Stendal GmbH</t>
   </si>
   <si>
+    <t>Werk  Zielitz</t>
+  </si>
+  <si>
+    <t>CIECH Soda Deutschland GmbH &amp; Co. KG</t>
+  </si>
+  <si>
     <t>Rheinkalk GmbH Werk Hönnetal</t>
   </si>
   <si>
@@ -425,16 +431,202 @@
     <t>ThyssenKrupp Steel Europe AG Werk Bruckhausen</t>
   </si>
   <si>
-    <t>Hüttenwerke Krupp Mannesmann GmbH</t>
+    <t>Huntsman P&amp;A Germany GmbH ehemals Sachtleben Chemie GmbH</t>
   </si>
   <si>
     <t>Solvay Chemicals GmbH</t>
   </si>
   <si>
-    <t>Dow Olefinverbund GmbH Werk Böhlen</t>
+    <t>BSR / MHKW</t>
+  </si>
+  <si>
+    <t>RWE Power AG-Fabrik Ville/Berrenrath</t>
+  </si>
+  <si>
+    <t>MtG</t>
   </si>
   <si>
     <t>PtF-FT1</t>
+  </si>
+  <si>
+    <t>{'Meth': 3487393.97800187, 'MtG': 4444727.840108303, 'FT': 4879006.727884552}</t>
+  </si>
+  <si>
+    <t>{'Meth': 3095903.241680239, 'MtG': 3945587.280523948, 'FT': 4331096.881437624}</t>
+  </si>
+  <si>
+    <t>{'Meth': 15940434.284553453, 'MtG': 20345919.952581324, 'FT': 22333848.978979554}</t>
+  </si>
+  <si>
+    <t>{'Meth': 18114593.910633203, 'MtG': 23126845.927408446, 'FT': 25386489.552041017}</t>
+  </si>
+  <si>
+    <t>{'Meth': 2741666.4448316456, 'MtG': 3493983.9170904844, 'FT': 3835368.9251284986}</t>
+  </si>
+  <si>
+    <t>{'Meth': 21772856.99976025, 'MtG': 27809259.748271197, 'FT': 30526405.730614576}</t>
+  </si>
+  <si>
+    <t>{'Meth': 5537474.182711428, 'MtG': 7059273.628407304, 'FT': 7749010.6854637}</t>
+  </si>
+  <si>
+    <t>{'Meth': 2368753.8965786793, 'MtG': 3018611.9555815747, 'FT': 3313550.0237504714}</t>
+  </si>
+  <si>
+    <t>{'Meth': 5313876.844978522, 'MtG': 6774050.451501959, 'FT': 7435919.344636883}</t>
+  </si>
+  <si>
+    <t>{'Meth': 5071633.194829957, 'MtG': 6465058.676521169, 'FT': 7096737.058741168}</t>
+  </si>
+  <si>
+    <t>{'Meth': 7456203.6692092875, 'MtG': 9507439.23017819, 'FT': 10436378.027560541}</t>
+  </si>
+  <si>
+    <t>{'Meth': 2853533.867243568, 'MtG': 3636595.5055431565, 'FT': 3991914.5955419056}</t>
+  </si>
+  <si>
+    <t>{'Meth': 3189118.573443136, 'MtG': 4064430.2709011757, 'FT': 4461551.60678213}</t>
+  </si>
+  <si>
+    <t>{'Meth': 14341627.495048827, 'MtG': 18301820.518093012, 'FT': 20090027.70305404}</t>
+  </si>
+  <si>
+    <t>{'Meth': 6003264.40165077, 'MtG': 7653488.580293442, 'FT': 8401284.312186236}</t>
+  </si>
+  <si>
+    <t>{'Meth': 4158437.5577930594, 'MtG': 5300397.37082434, 'FT': 5818280.750365}</t>
+  </si>
+  <si>
+    <t>{'Meth': 6021894.954526041, 'MtG': 7677257.178368888, 'FT': 8427375.257255137}</t>
+  </si>
+  <si>
+    <t>{'Meth': 4195714.668279373, 'MtG': 5347934.566975232, 'FT': 5870462.640502805}</t>
+  </si>
+  <si>
+    <t>{'Meth': 11104999.999200322, 'MtG': 14166084.452965502, 'FT': 15550203.261065204}</t>
+  </si>
+  <si>
+    <t>{'Meth': 7716935.3545670165, 'MtG': 9840199.603234423, 'FT': 10801651.25852516}</t>
+  </si>
+  <si>
+    <t>{'Meth': 9113441.365831105, 'MtG': 11622844.458892835, 'FT': 12758472.13869276}</t>
+  </si>
+  <si>
+    <t>{'Meth': 2443339.008220378, 'MtG': 3113686.3478833577, 'FT': 3417913.8040260775}</t>
+  </si>
+  <si>
+    <t>{'Meth': 27007138.60142434, 'MtG': 34515896.339734614, 'FT': 37888324.4415765}</t>
+  </si>
+  <si>
+    <t>{'Meth': 10230317.574675746, 'MtG': 13048960.343419567, 'FT': 14323928.842826845}</t>
+  </si>
+  <si>
+    <t>{'Meth': 5015728.864236233, 'MtG': 6393752.882294831, 'FT': 7018464.223534462}</t>
+  </si>
+  <si>
+    <t>{'Meth': 21958471.983473293, 'MtG': 28046945.729025654, 'FT': 30787315.18130359}</t>
+  </si>
+  <si>
+    <t>{'Meth': 3077259.9314400596, 'MtG': 3921818.6824485026, 'FT': 4305005.936368723}</t>
+  </si>
+  <si>
+    <t>{'Meth': 4587104.703249776, 'MtG': 5847075.126559586, 'FT': 6418372.486949732}</t>
+  </si>
+  <si>
+    <t>{'Meth': 2051752.656756106, 'MtG': 2614545.7882990018, 'FT': 2870003.957579148}</t>
+  </si>
+  <si>
+    <t>{'Meth': 2723021.589861078, 'MtG': 3470215.3190150387, 'FT': 3809277.9800595967}</t>
+  </si>
+  <si>
+    <t>{'Meth': 18801918.172355607, 'MtG': 24006284.056199927, 'FT': 26351854.519590363}</t>
+  </si>
+  <si>
+    <t>{'Meth': 2778955.9108548313, 'MtG': 3541521.1132413754, 'FT': 3887550.815266301}</t>
+  </si>
+  <si>
+    <t>{'Meth': 21215963.57252571, 'MtG': 27096201.806007836, 'FT': 29743677.37854753}</t>
+  </si>
+  <si>
+    <t>{'Meth': 7176830.63573128, 'MtG': 9150910.259046506, 'FT': 10045013.85152702}</t>
+  </si>
+  <si>
+    <t>{'Meth': 2984042.160773337, 'MtG': 3802975.692071275, 'FT': 4174551.211024216}</t>
+  </si>
+  <si>
+    <t>{'Meth': 2256873.78961794, 'MtG': 2876000.3671289016, 'FT': 3157004.353337063}</t>
+  </si>
+  <si>
+    <t>{'Meth': 3058616.539902832, 'MtG': 3898050.084373057, 'FT': 4278914.991299821}</t>
+  </si>
+  <si>
+    <t>{'Meth': 11495757.656832574, 'MtG': 14665225.012549855, 'FT': 16098113.107512131}</t>
+  </si>
+  <si>
+    <t>{'Meth': 7754181.439418147, 'MtG': 9887736.799385315, 'FT': 10853833.14866296}</t>
+  </si>
+  <si>
+    <t>{'Meth': 6170936.453752637, 'MtG': 7867405.96297245, 'FT': 8636102.817806346}</t>
+  </si>
+  <si>
+    <t>{'Meth': 4307544.049353574, 'MtG': 5490546.155427906, 'FT': 6027008.310916212}</t>
+  </si>
+  <si>
+    <t>{'Meth': 4810740.062798683, 'MtG': 6132298.3034649305, 'FT': 6731463.8277765475}</t>
+  </si>
+  <si>
+    <t>{'Meth': 7232706.703717464, 'MtG': 9222216.053272843, 'FT': 10123286.686733723}</t>
+  </si>
+  <si>
+    <t>{'Meth': 8331454.2385598505, 'MtG': 10624563.339724127, 'FT': 11662652.445798906}</t>
+  </si>
+  <si>
+    <t>{'Meth': 6264084.751326288, 'MtG': 7986248.953349681, 'FT': 8766557.543150855}</t>
+  </si>
+  <si>
+    <t>{'Meth': 4754832.319820861, 'MtG': 6060992.509238595, 'FT': 6653190.992569845}</t>
+  </si>
+  <si>
+    <t>{'Meth': 3655164.7482673554, 'MtG': 4658645.222787313, 'FT': 5113825.233504665}</t>
+  </si>
+  <si>
+    <t>{'Meth': 15010968.327398868, 'MtG': 19157490.04880905, 'FT': 21029301.725534488}</t>
+  </si>
+  <si>
+    <t>{'Meth': 6971945.468368442, 'MtG': 8889455.680216607, 'FT': 9758013.455769105}</t>
+  </si>
+  <si>
+    <t>{'Meth': 18987662.48066654, 'MtG': 24243970.03695438, 'FT': 26612763.97027938}</t>
+  </si>
+  <si>
+    <t>{'Meth': 11532970.807191214, 'MtG': 14712762.208700748, 'FT': 16150294.997649936}</t>
+  </si>
+  <si>
+    <t>{'Meth': 12463194.188631605, 'MtG': 15901192.112473022, 'FT': 17454842.251095004}</t>
+  </si>
+  <si>
+    <t>{'Meth': 21401602.794789482, 'MtG': 27333887.786762293, 'FT': 30004586.829236556}</t>
+  </si>
+  <si>
+    <t>{'Meth': 13021230.962479174, 'MtG': 16614250.054736383, 'FT': 18237570.603162043}</t>
+  </si>
+  <si>
+    <t>{'Meth': 10583934.167808509, 'MtG': 13500563.706853025, 'FT': 14819656.799135963}</t>
+  </si>
+  <si>
+    <t>{'Meth': 23628643.364246435, 'MtG': 30186119.555815745, 'FT': 33135500.23750471}</t>
+  </si>
+  <si>
+    <t>{'Meth': 17668702.747726772, 'MtG': 22556399.573597748, 'FT': 24760306.870387375}</t>
+  </si>
+  <si>
+    <t>{'Meth': 7325831.86001466, 'MtG': 9341059.04365007, 'FT': 10253741.41207823}</t>
+  </si>
+  <si>
+    <t>{'Meth': 7418954.986766862, 'MtG': 9459902.034027299, 'FT': 10384196.137422739}</t>
+  </si>
+  <si>
+    <t>{'Meth': 20101958.5303517, 'MtG': 25670085.921481106, 'FT': 28178220.674413458}</t>
   </si>
 </sst>
 </file>
@@ -1000,10 +1192,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>13267039228.84912</v>
+        <v>13506690818.90995</v>
       </c>
       <c r="C2">
-        <v>95.99999999999999</v>
+        <v>96</v>
       </c>
       <c r="D2">
         <v>1190.511948111309</v>
@@ -1015,10 +1207,10 @@
         <v>400</v>
       </c>
       <c r="G2">
-        <v>330.4949195865012</v>
+        <v>331.0757941250727</v>
       </c>
       <c r="H2">
-        <v>33.82257948984662</v>
+        <v>30.15963365760841</v>
       </c>
       <c r="I2">
         <v>858.4615384615383</v>
@@ -1036,7 +1228,7 @@
         <v>248.7145732819791</v>
       </c>
       <c r="N2">
-        <v>80.88278805918019</v>
+        <v>80.8827880591802</v>
       </c>
       <c r="O2">
         <v>167.8317852227989</v>
@@ -1066,31 +1258,31 @@
         <v>0</v>
       </c>
       <c r="X2">
-        <v>0</v>
+        <v>141.9507589561625</v>
       </c>
       <c r="Y2">
-        <v>0</v>
+        <v>141.9507589561625</v>
       </c>
       <c r="Z2">
-        <v>278.3115112307378</v>
+        <v>141.6084210526316</v>
       </c>
       <c r="AA2">
-        <v>86.00598784560997</v>
+        <v>43.76093567251463</v>
       </c>
       <c r="AB2">
-        <v>192.3055233851278</v>
+        <v>97.84748538011695</v>
       </c>
       <c r="AC2">
-        <v>0</v>
+        <v>-6.564332929285719e-18</v>
       </c>
       <c r="AD2">
-        <v>0</v>
+        <v>-1.608261567675001e-18</v>
       </c>
       <c r="AE2">
-        <v>0</v>
+        <v>-1.969299878785716e-19</v>
       </c>
       <c r="AF2">
-        <v>0</v>
+        <v>-4.759141373732146e-18</v>
       </c>
       <c r="AG2">
         <v>0</v>
@@ -1099,16 +1291,16 @@
         <v>0</v>
       </c>
       <c r="AI2">
-        <v>321.227980977466</v>
+        <v>399.9430126483085</v>
       </c>
       <c r="AJ2">
-        <v>321.227980977466</v>
+        <v>399.9430126483085</v>
       </c>
       <c r="AK2">
-        <v>450.772019022534</v>
+        <v>372.0569873516916</v>
       </c>
       <c r="AL2">
-        <v>450.772019022534</v>
+        <v>372.0569873516916</v>
       </c>
       <c r="AM2">
         <v>6.75</v>
@@ -1165,10 +1357,10 @@
         <v>41.45</v>
       </c>
       <c r="BE2">
-        <v>406.8887759047903</v>
+        <v>506.5944826878574</v>
       </c>
       <c r="BF2">
-        <v>1074.598847069465</v>
+        <v>980.1408090644542</v>
       </c>
       <c r="BG2">
         <v>120</v>
@@ -1177,22 +1369,22 @@
         <v>154.0911111111111</v>
       </c>
       <c r="BI2">
+        <v>130.3</v>
+      </c>
+      <c r="BJ2">
+        <v>414.5</v>
+      </c>
+      <c r="BK2">
         <v>858</v>
       </c>
-      <c r="BJ2">
+      <c r="BL2">
+        <v>120</v>
+      </c>
+      <c r="BM2">
+        <v>7.5</v>
+      </c>
+      <c r="BN2">
         <v>24.2</v>
-      </c>
-      <c r="BK2">
-        <v>130.3</v>
-      </c>
-      <c r="BL2">
-        <v>7.5</v>
-      </c>
-      <c r="BM2">
-        <v>414.5</v>
-      </c>
-      <c r="BN2">
-        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1202,7 +1394,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L64"/>
+  <dimension ref="A1:L67"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1254,28 +1446,28 @@
         <v>25541</v>
       </c>
       <c r="D2">
-        <v>1.870000000000002</v>
+        <v>1.870000000000001</v>
       </c>
       <c r="E2" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
-      <c r="G2">
-        <v>3487393.97800187</v>
+      <c r="G2" t="s">
+        <v>144</v>
       </c>
       <c r="H2">
         <v>33331633.33333333</v>
       </c>
       <c r="I2">
-        <v>62330154.33333339</v>
+        <v>62330154.33333338</v>
       </c>
       <c r="J2">
         <v>100</v>
       </c>
       <c r="K2">
-        <v>18.70000000000002</v>
+        <v>18.70000000000001</v>
       </c>
       <c r="L2">
         <v>3211279.34822684</v>
@@ -1292,28 +1484,28 @@
         <v>25541</v>
       </c>
       <c r="D3">
-        <v>1.66</v>
+        <v>1.660000000000003</v>
       </c>
       <c r="E3" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
-      <c r="G3">
-        <v>3095903.241680239</v>
+      <c r="G3" t="s">
+        <v>145</v>
       </c>
       <c r="H3">
         <v>33331633.33333333</v>
       </c>
       <c r="I3">
-        <v>55330511.33333334</v>
+        <v>55330511.33333343</v>
       </c>
       <c r="J3">
         <v>100</v>
       </c>
       <c r="K3">
-        <v>16.6</v>
+        <v>16.60000000000003</v>
       </c>
       <c r="L3">
         <v>3120028.598903444</v>
@@ -1330,28 +1522,28 @@
         <v>25572</v>
       </c>
       <c r="D4">
-        <v>8.560000000000004</v>
+        <v>8.560000000000009</v>
       </c>
       <c r="E4" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F4">
         <v>0.1</v>
       </c>
-      <c r="G4">
-        <v>15940434.28455345</v>
+      <c r="G4" t="s">
+        <v>146</v>
       </c>
       <c r="H4">
         <v>33429264.21745752</v>
       </c>
       <c r="I4">
-        <v>286154501.7014365</v>
+        <v>286154501.7014366</v>
       </c>
       <c r="J4">
         <v>100</v>
       </c>
       <c r="K4">
-        <v>85.60000000000004</v>
+        <v>85.60000000000009</v>
       </c>
       <c r="L4">
         <v>4640353.526253123</v>
@@ -1368,28 +1560,28 @@
         <v>25734</v>
       </c>
       <c r="D5">
-        <v>9.729999999999993</v>
+        <v>9.729999999999999</v>
       </c>
       <c r="E5" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F5">
         <v>0.1</v>
       </c>
-      <c r="G5">
-        <v>18114593.9106332</v>
+      <c r="G5" t="s">
+        <v>147</v>
       </c>
       <c r="H5">
         <v>33429264.21745752</v>
       </c>
       <c r="I5">
-        <v>325266740.8358614</v>
+        <v>325266740.8358616</v>
       </c>
       <c r="J5">
         <v>100</v>
       </c>
       <c r="K5">
-        <v>97.29999999999993</v>
+        <v>97.29999999999998</v>
       </c>
       <c r="L5">
         <v>4786474.22858194</v>
@@ -1406,28 +1598,28 @@
         <v>26388</v>
       </c>
       <c r="D6">
-        <v>1.469999999999999</v>
+        <v>1.47</v>
       </c>
       <c r="E6" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F6">
         <v>0.1</v>
       </c>
-      <c r="G6">
-        <v>2741666.444831646</v>
+      <c r="G6" t="s">
+        <v>148</v>
       </c>
       <c r="H6">
         <v>33429264.21745752</v>
       </c>
       <c r="I6">
-        <v>49141018.39966252</v>
+        <v>49141018.39966254</v>
       </c>
       <c r="J6">
         <v>100</v>
       </c>
       <c r="K6">
-        <v>14.69999999999999</v>
+        <v>14.7</v>
       </c>
       <c r="L6">
         <v>3029585.493423196</v>
@@ -1447,19 +1639,19 @@
         <v>11.52</v>
       </c>
       <c r="E7" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F7">
         <v>0.2</v>
       </c>
-      <c r="G7">
-        <v>21772856.99976025</v>
+      <c r="G7" t="s">
+        <v>149</v>
       </c>
       <c r="H7">
         <v>33609222.38641504</v>
       </c>
       <c r="I7">
-        <v>387178241.8915013</v>
+        <v>387178241.8915014</v>
       </c>
       <c r="J7">
         <v>100</v>
@@ -1482,28 +1674,28 @@
         <v>26316</v>
       </c>
       <c r="D8">
-        <v>2.969999999999996</v>
+        <v>2.969999999999998</v>
       </c>
       <c r="E8" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F8">
         <v>0.2</v>
       </c>
-      <c r="G8">
-        <v>5537474.182711428</v>
+      <c r="G8" t="s">
+        <v>150</v>
       </c>
       <c r="H8">
         <v>33609222.38641504</v>
       </c>
       <c r="I8">
-        <v>99819390.48765253</v>
+        <v>99819390.48765258</v>
       </c>
       <c r="J8">
         <v>100</v>
       </c>
       <c r="K8">
-        <v>29.69999999999996</v>
+        <v>29.69999999999997</v>
       </c>
       <c r="L8">
         <v>3591695.233391508</v>
@@ -1520,28 +1712,28 @@
         <v>26954</v>
       </c>
       <c r="D9">
-        <v>1.27</v>
+        <v>1.269999999999999</v>
       </c>
       <c r="E9" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F9">
         <v>0.2</v>
       </c>
-      <c r="G9">
-        <v>2368753.896578679</v>
+      <c r="G9" t="s">
+        <v>151</v>
       </c>
       <c r="H9">
         <v>33609222.38641504</v>
       </c>
       <c r="I9">
-        <v>42683712.4307471</v>
+        <v>42683712.43074708</v>
       </c>
       <c r="J9">
         <v>100</v>
       </c>
       <c r="K9">
-        <v>12.7</v>
+        <v>12.69999999999999</v>
       </c>
       <c r="L9">
         <v>2924239.357757165</v>
@@ -1558,28 +1750,28 @@
         <v>27570</v>
       </c>
       <c r="D10">
-        <v>2.849999999999997</v>
+        <v>2.850000000000002</v>
       </c>
       <c r="E10" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F10">
         <v>0.2</v>
       </c>
-      <c r="G10">
-        <v>5313876.844978522</v>
+      <c r="G10" t="s">
+        <v>152</v>
       </c>
       <c r="H10">
         <v>33609222.38641504</v>
       </c>
       <c r="I10">
-        <v>95786283.80128276</v>
+        <v>95786283.80128293</v>
       </c>
       <c r="J10">
         <v>100</v>
       </c>
       <c r="K10">
-        <v>28.49999999999997</v>
+        <v>28.50000000000002</v>
       </c>
       <c r="L10">
         <v>3556025.558079649</v>
@@ -1596,28 +1788,28 @@
         <v>26892</v>
       </c>
       <c r="D11">
-        <v>2.719999999999999</v>
+        <v>2.720000000000004</v>
       </c>
       <c r="E11" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F11">
         <v>0.5</v>
       </c>
-      <c r="G11">
-        <v>5071633.194829957</v>
+      <c r="G11" t="s">
+        <v>153</v>
       </c>
       <c r="H11">
         <v>34374076.88937075</v>
       </c>
       <c r="I11">
-        <v>93497489.13908842</v>
+        <v>93497489.1390886</v>
       </c>
       <c r="J11">
         <v>100</v>
       </c>
       <c r="K11">
-        <v>27.19999999999999</v>
+        <v>27.20000000000004</v>
       </c>
       <c r="L11">
         <v>3516074.693055412</v>
@@ -1637,13 +1829,13 @@
         <v>4</v>
       </c>
       <c r="E12" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F12">
         <v>0.7</v>
       </c>
-      <c r="G12">
-        <v>7456203.669209288</v>
+      <c r="G12" t="s">
+        <v>154</v>
       </c>
       <c r="H12">
         <v>34962685.86338257</v>
@@ -1672,28 +1864,28 @@
         <v>20457</v>
       </c>
       <c r="D13">
-        <v>1.529999999999999</v>
+        <v>1.530000000000001</v>
       </c>
       <c r="E13" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F13">
         <v>0.75</v>
       </c>
-      <c r="G13">
-        <v>2853533.867243568</v>
+      <c r="G13" t="s">
+        <v>155</v>
       </c>
       <c r="H13">
         <v>35112131.13005736</v>
       </c>
       <c r="I13">
-        <v>53721560.62898773</v>
+        <v>53721560.62898779</v>
       </c>
       <c r="J13">
         <v>100</v>
       </c>
       <c r="K13">
-        <v>15.29999999999999</v>
+        <v>15.30000000000001</v>
       </c>
       <c r="L13">
         <v>3059058.228987825</v>
@@ -1713,19 +1905,19 @@
         <v>1.710000000000002</v>
       </c>
       <c r="E14" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F14">
         <v>0.75</v>
       </c>
-      <c r="G14">
-        <v>3189118.573443136</v>
+      <c r="G14" t="s">
+        <v>156</v>
       </c>
       <c r="H14">
         <v>35112131.13005736</v>
       </c>
       <c r="I14">
-        <v>60041744.23239815</v>
+        <v>60041744.23239816</v>
       </c>
       <c r="J14">
         <v>100</v>
@@ -1748,28 +1940,28 @@
         <v>21079</v>
       </c>
       <c r="D15">
-        <v>7.7</v>
+        <v>7.700000000000006</v>
       </c>
       <c r="E15" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F15">
         <v>0.75</v>
       </c>
-      <c r="G15">
-        <v>14341627.49504883</v>
+      <c r="G15" t="s">
+        <v>157</v>
       </c>
       <c r="H15">
         <v>35112131.13005736</v>
       </c>
       <c r="I15">
-        <v>270363409.7014417</v>
+        <v>270363409.7014419</v>
       </c>
       <c r="J15">
         <v>100</v>
       </c>
       <c r="K15">
-        <v>77</v>
+        <v>77.00000000000006</v>
       </c>
       <c r="L15">
         <v>4522964.437644095</v>
@@ -1786,16 +1978,16 @@
         <v>21107</v>
       </c>
       <c r="D16">
-        <v>3.219999999999999</v>
+        <v>3.219999999999998</v>
       </c>
       <c r="E16" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F16">
         <v>0.75</v>
       </c>
-      <c r="G16">
-        <v>6003264.40165077</v>
+      <c r="G16" t="s">
+        <v>158</v>
       </c>
       <c r="H16">
         <v>35112131.13005736</v>
@@ -1807,7 +1999,7 @@
         <v>100</v>
       </c>
       <c r="K16">
-        <v>32.19999999999999</v>
+        <v>32.19999999999998</v>
       </c>
       <c r="L16">
         <v>3662634.134160224</v>
@@ -1824,28 +2016,28 @@
         <v>21107</v>
       </c>
       <c r="D17">
-        <v>2.230000000000001</v>
+        <v>2.23</v>
       </c>
       <c r="E17" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F17">
         <v>0.75</v>
       </c>
-      <c r="G17">
-        <v>4158437.557793059</v>
+      <c r="G17" t="s">
+        <v>159</v>
       </c>
       <c r="H17">
         <v>35112131.13005736</v>
       </c>
       <c r="I17">
-        <v>78300052.42002796</v>
+        <v>78300052.42002793</v>
       </c>
       <c r="J17">
         <v>100</v>
       </c>
       <c r="K17">
-        <v>22.30000000000001</v>
+        <v>22.3</v>
       </c>
       <c r="L17">
         <v>3351059.927308201</v>
@@ -1862,28 +2054,28 @@
         <v>21119</v>
       </c>
       <c r="D18">
-        <v>3.229999999999997</v>
+        <v>3.23</v>
       </c>
       <c r="E18" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F18">
         <v>0.75</v>
       </c>
-      <c r="G18">
-        <v>6021894.954526041</v>
+      <c r="G18" t="s">
+        <v>160</v>
       </c>
       <c r="H18">
         <v>35112131.13005736</v>
       </c>
       <c r="I18">
-        <v>113412183.5500852</v>
+        <v>113412183.5500853</v>
       </c>
       <c r="J18">
         <v>100</v>
       </c>
       <c r="K18">
-        <v>32.29999999999998</v>
+        <v>32.3</v>
       </c>
       <c r="L18">
         <v>3665383.563029062</v>
@@ -1900,28 +2092,28 @@
         <v>21129</v>
       </c>
       <c r="D19">
-        <v>2.249999999999999</v>
+        <v>2.25</v>
       </c>
       <c r="E19" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F19">
         <v>0.75</v>
       </c>
-      <c r="G19">
-        <v>4195714.668279373</v>
+      <c r="G19" t="s">
+        <v>161</v>
       </c>
       <c r="H19">
         <v>35112131.13005736</v>
       </c>
       <c r="I19">
-        <v>79002295.04262903</v>
+        <v>79002295.04262909</v>
       </c>
       <c r="J19">
         <v>100</v>
       </c>
       <c r="K19">
-        <v>22.49999999999999</v>
+        <v>22.5</v>
       </c>
       <c r="L19">
         <v>3358308.48673273</v>
@@ -1938,28 +2130,28 @@
         <v>21683</v>
       </c>
       <c r="D20">
-        <v>5.960000000000008</v>
+        <v>5.960000000000003</v>
       </c>
       <c r="E20" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F20">
         <v>0.75</v>
       </c>
-      <c r="G20">
-        <v>11104999.99920032</v>
+      <c r="G20" t="s">
+        <v>162</v>
       </c>
       <c r="H20">
         <v>35112131.13005736</v>
       </c>
       <c r="I20">
-        <v>209268301.5351422</v>
+        <v>209268301.535142</v>
       </c>
       <c r="J20">
         <v>100</v>
       </c>
       <c r="K20">
-        <v>59.60000000000008</v>
+        <v>59.60000000000002</v>
       </c>
       <c r="L20">
         <v>4251106.766759329</v>
@@ -1976,28 +2168,28 @@
         <v>21683</v>
       </c>
       <c r="D21">
-        <v>4.140000000000001</v>
+        <v>4.140000000000014</v>
       </c>
       <c r="E21" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F21">
         <v>0.75</v>
       </c>
-      <c r="G21">
-        <v>7716935.354567016</v>
+      <c r="G21" t="s">
+        <v>163</v>
       </c>
       <c r="H21">
         <v>35112131.13005736</v>
       </c>
       <c r="I21">
-        <v>145364222.8784375</v>
+        <v>145364222.878438</v>
       </c>
       <c r="J21">
         <v>100</v>
       </c>
       <c r="K21">
-        <v>41.40000000000001</v>
+        <v>41.40000000000014</v>
       </c>
       <c r="L21">
         <v>3892301.737650325</v>
@@ -2017,13 +2209,13 @@
         <v>4.890000000000001</v>
       </c>
       <c r="E22" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F22">
         <v>0.75</v>
       </c>
-      <c r="G22">
-        <v>9113441.365831105</v>
+      <c r="G22" t="s">
+        <v>164</v>
       </c>
       <c r="H22">
         <v>35112131.13005736</v>
@@ -2052,28 +2244,28 @@
         <v>22145</v>
       </c>
       <c r="D23">
-        <v>3.229999999999997</v>
+        <v>3.230000000000002</v>
       </c>
       <c r="E23" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F23">
         <v>0.8</v>
       </c>
-      <c r="G23">
-        <v>6021894.954526041</v>
+      <c r="G23" t="s">
+        <v>160</v>
       </c>
       <c r="H23">
         <v>35261419.93911113</v>
       </c>
       <c r="I23">
-        <v>113894386.4033289</v>
+        <v>113894386.403329</v>
       </c>
       <c r="J23">
         <v>100</v>
       </c>
       <c r="K23">
-        <v>32.29999999999998</v>
+        <v>32.30000000000003</v>
       </c>
       <c r="L23">
         <v>3665383.563029062</v>
@@ -2093,19 +2285,19 @@
         <v>1.309999999999999</v>
       </c>
       <c r="E24" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F24">
         <v>0.8</v>
       </c>
-      <c r="G24">
-        <v>2443339.008220378</v>
+      <c r="G24" t="s">
+        <v>165</v>
       </c>
       <c r="H24">
         <v>35261419.93911113</v>
       </c>
       <c r="I24">
-        <v>46192460.12023554</v>
+        <v>46192460.12023553</v>
       </c>
       <c r="J24">
         <v>100</v>
@@ -2131,19 +2323,19 @@
         <v>11.52</v>
       </c>
       <c r="E25" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F25">
         <v>0.8</v>
       </c>
-      <c r="G25">
-        <v>27007138.60142434</v>
+      <c r="G25" t="s">
+        <v>166</v>
       </c>
       <c r="H25">
         <v>35261419.93911113</v>
       </c>
       <c r="I25">
-        <v>406211557.6985603</v>
+        <v>406211557.6985604</v>
       </c>
       <c r="J25">
         <v>100</v>
@@ -2166,16 +2358,16 @@
         <v>28237</v>
       </c>
       <c r="D26">
-        <v>5.489999999999999</v>
+        <v>5.490000000000001</v>
       </c>
       <c r="E26" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F26">
         <v>0.8</v>
       </c>
-      <c r="G26">
-        <v>10230317.57467575</v>
+      <c r="G26" t="s">
+        <v>167</v>
       </c>
       <c r="H26">
         <v>35261419.93911113</v>
@@ -2187,7 +2379,7 @@
         <v>100</v>
       </c>
       <c r="K26">
-        <v>54.89999999999999</v>
+        <v>54.90000000000001</v>
       </c>
       <c r="L26">
         <v>4167435.864813926</v>
@@ -2204,28 +2396,28 @@
         <v>28237</v>
       </c>
       <c r="D27">
-        <v>2.690000000000004</v>
+        <v>2.690000000000001</v>
       </c>
       <c r="E27" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F27">
         <v>0.8</v>
       </c>
-      <c r="G27">
-        <v>5015728.864236233</v>
+      <c r="G27" t="s">
+        <v>168</v>
       </c>
       <c r="H27">
         <v>35261419.93911113</v>
       </c>
       <c r="I27">
-        <v>94853219.63620909</v>
+        <v>94853219.63620897</v>
       </c>
       <c r="J27">
         <v>100</v>
       </c>
       <c r="K27">
-        <v>26.90000000000004</v>
+        <v>26.90000000000001</v>
       </c>
       <c r="L27">
         <v>3506650.390632065</v>
@@ -2245,13 +2437,13 @@
         <v>11.52</v>
       </c>
       <c r="E28" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F28">
         <v>1</v>
       </c>
-      <c r="G28">
-        <v>21958471.98347329</v>
+      <c r="G28" t="s">
+        <v>169</v>
       </c>
       <c r="H28">
         <v>35849408.31499194</v>
@@ -2280,28 +2472,28 @@
         <v>29525</v>
       </c>
       <c r="D29">
-        <v>1.649999999999996</v>
+        <v>1.649999999999998</v>
       </c>
       <c r="E29" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F29">
         <v>1.4</v>
       </c>
-      <c r="G29">
-        <v>3077259.93144006</v>
+      <c r="G29" t="s">
+        <v>170</v>
       </c>
       <c r="H29">
         <v>36933299.30390043</v>
       </c>
       <c r="I29">
-        <v>60939943.85143556</v>
+        <v>60939943.85143565</v>
       </c>
       <c r="J29">
         <v>100</v>
       </c>
       <c r="K29">
-        <v>16.49999999999996</v>
+        <v>16.49999999999998</v>
       </c>
       <c r="L29">
         <v>3115469.701891457</v>
@@ -2318,28 +2510,28 @@
         <v>30659</v>
       </c>
       <c r="D30">
-        <v>2.460000000000001</v>
+        <v>2.460000000000003</v>
       </c>
       <c r="E30" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F30">
         <v>1.7</v>
       </c>
-      <c r="G30">
-        <v>4587104.703249776</v>
+      <c r="G30" t="s">
+        <v>171</v>
       </c>
       <c r="H30">
         <v>37640511.58399763</v>
       </c>
       <c r="I30">
-        <v>92595658.4966342</v>
+        <v>92595658.49663429</v>
       </c>
       <c r="J30">
         <v>100</v>
       </c>
       <c r="K30">
-        <v>24.60000000000001</v>
+        <v>24.60000000000003</v>
       </c>
       <c r="L30">
         <v>3431616.232505888</v>
@@ -2359,13 +2551,13 @@
         <v>1.100000000000001</v>
       </c>
       <c r="E31" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F31">
         <v>1.8</v>
       </c>
-      <c r="G31">
-        <v>2051752.656756106</v>
+      <c r="G31" t="s">
+        <v>172</v>
       </c>
       <c r="H31">
         <v>37855437.77268496</v>
@@ -2397,19 +2589,19 @@
         <v>1.460000000000003</v>
       </c>
       <c r="E32" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F32">
         <v>1.8</v>
       </c>
-      <c r="G32">
-        <v>2723021.589861078</v>
+      <c r="G32" t="s">
+        <v>173</v>
       </c>
       <c r="H32">
         <v>37855437.77268496</v>
       </c>
       <c r="I32">
-        <v>55268939.14812016</v>
+        <v>55268939.14812015</v>
       </c>
       <c r="J32">
         <v>100</v>
@@ -2435,19 +2627,19 @@
         <v>10.1</v>
       </c>
       <c r="E33" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F33">
         <v>1.8</v>
       </c>
-      <c r="G33">
-        <v>18801918.17235561</v>
+      <c r="G33" t="s">
+        <v>174</v>
       </c>
       <c r="H33">
         <v>37855437.77268496</v>
       </c>
       <c r="I33">
-        <v>382339921.5041181</v>
+        <v>382339921.5041182</v>
       </c>
       <c r="J33">
         <v>100</v>
@@ -2470,28 +2662,28 @@
         <v>49536</v>
       </c>
       <c r="D34">
-        <v>1.489999999999998</v>
+        <v>1.489999999999995</v>
       </c>
       <c r="E34" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F34">
         <v>1.8</v>
       </c>
-      <c r="G34">
-        <v>2778955.910854831</v>
+      <c r="G34" t="s">
+        <v>175</v>
       </c>
       <c r="H34">
         <v>37855437.77268496</v>
       </c>
       <c r="I34">
-        <v>56404602.28130051</v>
+        <v>56404602.2813004</v>
       </c>
       <c r="J34">
         <v>100</v>
       </c>
       <c r="K34">
-        <v>14.89999999999998</v>
+        <v>14.89999999999995</v>
       </c>
       <c r="L34">
         <v>3039509.425943215</v>
@@ -2508,28 +2700,28 @@
         <v>49808</v>
       </c>
       <c r="D35">
-        <v>11.40000000000002</v>
+        <v>11.39999999999998</v>
       </c>
       <c r="E35" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F35">
         <v>1.8</v>
       </c>
-      <c r="G35">
-        <v>21215963.57252571</v>
+      <c r="G35" t="s">
+        <v>176</v>
       </c>
       <c r="H35">
         <v>37855437.77268496</v>
       </c>
       <c r="I35">
-        <v>431551990.6086094</v>
+        <v>431551990.6086079</v>
       </c>
       <c r="J35">
         <v>100</v>
       </c>
       <c r="K35">
-        <v>114.0000000000002</v>
+        <v>113.9999999999998</v>
       </c>
       <c r="L35">
         <v>4973514.536159209</v>
@@ -2546,28 +2738,28 @@
         <v>49824</v>
       </c>
       <c r="D36">
-        <v>3.850000000000001</v>
+        <v>3.850000000000002</v>
       </c>
       <c r="E36" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F36">
         <v>1.8</v>
       </c>
-      <c r="G36">
-        <v>7176830.63573128</v>
+      <c r="G36" t="s">
+        <v>177</v>
       </c>
       <c r="H36">
         <v>37855437.77268496</v>
       </c>
       <c r="I36">
-        <v>145743435.4248371</v>
+        <v>145743435.4248372</v>
       </c>
       <c r="J36">
         <v>100</v>
       </c>
       <c r="K36">
-        <v>38.50000000000001</v>
+        <v>38.50000000000002</v>
       </c>
       <c r="L36">
         <v>3824493.385265881</v>
@@ -2584,28 +2776,28 @@
         <v>49824</v>
       </c>
       <c r="D37">
-        <v>1.599999999999992</v>
+        <v>1.600000000000003</v>
       </c>
       <c r="E37" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F37">
         <v>1.8</v>
       </c>
-      <c r="G37">
-        <v>2984042.160773337</v>
+      <c r="G37" t="s">
+        <v>178</v>
       </c>
       <c r="H37">
         <v>37855437.77268496</v>
       </c>
       <c r="I37">
-        <v>60568700.43629565</v>
+        <v>60568700.43629605</v>
       </c>
       <c r="J37">
         <v>100</v>
       </c>
       <c r="K37">
-        <v>15.99999999999992</v>
+        <v>16.00000000000003</v>
       </c>
       <c r="L37">
         <v>3092355.773228031</v>
@@ -2625,13 +2817,13 @@
         <v>1.210000000000001</v>
       </c>
       <c r="E38" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F38">
         <v>1.9</v>
       </c>
-      <c r="G38">
-        <v>2256873.78961794</v>
+      <c r="G38" t="s">
+        <v>179</v>
       </c>
       <c r="H38">
         <v>38060293.37896816</v>
@@ -2660,28 +2852,28 @@
         <v>31226</v>
       </c>
       <c r="D39">
-        <v>1.640000000000002</v>
+        <v>1.640000000000001</v>
       </c>
       <c r="E39" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F39">
         <v>1.9</v>
       </c>
-      <c r="G39">
-        <v>3058616.539902832</v>
+      <c r="G39" t="s">
+        <v>180</v>
       </c>
       <c r="H39">
         <v>38060293.37896816</v>
       </c>
       <c r="I39">
-        <v>62418881.14150786</v>
+        <v>62418881.14150781</v>
       </c>
       <c r="J39">
         <v>100</v>
       </c>
       <c r="K39">
-        <v>16.40000000000002</v>
+        <v>16.40000000000001</v>
       </c>
       <c r="L39">
         <v>3110889.813225406</v>
@@ -2698,28 +2890,28 @@
         <v>31319</v>
       </c>
       <c r="D40">
-        <v>6.170000000000002</v>
+        <v>6.17</v>
       </c>
       <c r="E40" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F40">
         <v>1.9</v>
       </c>
-      <c r="G40">
-        <v>11495757.65683257</v>
+      <c r="G40" t="s">
+        <v>181</v>
       </c>
       <c r="H40">
         <v>38060293.37896816</v>
       </c>
       <c r="I40">
-        <v>234832010.1482337</v>
+        <v>234832010.1482336</v>
       </c>
       <c r="J40">
         <v>100</v>
       </c>
       <c r="K40">
-        <v>61.70000000000002</v>
+        <v>61.7</v>
       </c>
       <c r="L40">
         <v>4286880.992309345</v>
@@ -2736,28 +2928,28 @@
         <v>31789</v>
       </c>
       <c r="D41">
-        <v>4.16</v>
+        <v>4.159999999999991</v>
       </c>
       <c r="E41" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F41">
         <v>1.9</v>
       </c>
-      <c r="G41">
-        <v>7754181.439418147</v>
+      <c r="G41" t="s">
+        <v>182</v>
       </c>
       <c r="H41">
         <v>38060293.37896816</v>
       </c>
       <c r="I41">
-        <v>158330820.4565076</v>
+        <v>158330820.4565072</v>
       </c>
       <c r="J41">
         <v>100</v>
       </c>
       <c r="K41">
-        <v>41.6</v>
+        <v>41.59999999999991</v>
       </c>
       <c r="L41">
         <v>3896843.850100604</v>
@@ -2774,28 +2966,28 @@
         <v>38239</v>
       </c>
       <c r="D42">
-        <v>11.51999999999999</v>
+        <v>11.52</v>
       </c>
       <c r="E42" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F42">
         <v>2</v>
       </c>
-      <c r="G42">
-        <v>27007138.60142434</v>
+      <c r="G42" t="s">
+        <v>166</v>
       </c>
       <c r="H42">
         <v>38255392.02166688</v>
       </c>
       <c r="I42">
-        <v>440702116.0896021</v>
+        <v>440702116.0896024</v>
       </c>
       <c r="J42">
         <v>100</v>
       </c>
       <c r="K42">
-        <v>115.1999999999999</v>
+        <v>115.2</v>
       </c>
       <c r="L42">
         <v>5273515.054654035</v>
@@ -2812,28 +3004,28 @@
         <v>31061</v>
       </c>
       <c r="D43">
-        <v>3.309999999999999</v>
+        <v>3.310000000000006</v>
       </c>
       <c r="E43" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F43">
         <v>2.1</v>
       </c>
-      <c r="G43">
-        <v>6170936.453752637</v>
+      <c r="G43" t="s">
+        <v>183</v>
       </c>
       <c r="H43">
         <v>38441090.93970785</v>
       </c>
       <c r="I43">
-        <v>127240011.0104329</v>
+        <v>127240011.0104332</v>
       </c>
       <c r="J43">
         <v>100</v>
       </c>
       <c r="K43">
-        <v>33.09999999999999</v>
+        <v>33.10000000000006</v>
       </c>
       <c r="L43">
         <v>3687149.882920415</v>
@@ -2850,28 +3042,28 @@
         <v>33106</v>
       </c>
       <c r="D44">
-        <v>2.309999999999997</v>
+        <v>2.309999999999998</v>
       </c>
       <c r="E44" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F44">
         <v>2.3</v>
       </c>
-      <c r="G44">
-        <v>4307544.049353574</v>
+      <c r="G44" t="s">
+        <v>184</v>
       </c>
       <c r="H44">
         <v>38785844.374162</v>
       </c>
       <c r="I44">
-        <v>89595300.50431411</v>
+        <v>89595300.50431414</v>
       </c>
       <c r="J44">
         <v>100</v>
       </c>
       <c r="K44">
-        <v>23.09999999999997</v>
+        <v>23.09999999999998</v>
       </c>
       <c r="L44">
         <v>3379765.097364126</v>
@@ -2891,13 +3083,13 @@
         <v>2.579999999999999</v>
       </c>
       <c r="E45" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F45">
         <v>2.3</v>
       </c>
-      <c r="G45">
-        <v>4810740.062798683</v>
+      <c r="G45" t="s">
+        <v>185</v>
       </c>
       <c r="H45">
         <v>38785844.374162</v>
@@ -2926,16 +3118,16 @@
         <v>33609</v>
       </c>
       <c r="D46">
-        <v>3.879999999999999</v>
+        <v>3.879999999999998</v>
       </c>
       <c r="E46" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F46">
         <v>2.3</v>
       </c>
-      <c r="G46">
-        <v>7232706.703717464</v>
+      <c r="G46" t="s">
+        <v>186</v>
       </c>
       <c r="H46">
         <v>38785844.374162</v>
@@ -2964,28 +3156,28 @@
         <v>38372</v>
       </c>
       <c r="D47">
-        <v>4.469999999999999</v>
+        <v>4.469999999999998</v>
       </c>
       <c r="E47" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F47">
         <v>2.3</v>
       </c>
-      <c r="G47">
-        <v>8331454.23855985</v>
+      <c r="G47" t="s">
+        <v>187</v>
       </c>
       <c r="H47">
         <v>38785844.374162</v>
       </c>
       <c r="I47">
-        <v>173372724.3525041</v>
+        <v>173372724.352504</v>
       </c>
       <c r="J47">
         <v>100</v>
       </c>
       <c r="K47">
-        <v>44.69999999999999</v>
+        <v>44.69999999999998</v>
       </c>
       <c r="L47">
         <v>3965215.892681056</v>
@@ -3002,28 +3194,28 @@
         <v>38723</v>
       </c>
       <c r="D48">
-        <v>3.360000000000001</v>
+        <v>3.359999999999998</v>
       </c>
       <c r="E48" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F48">
         <v>2.3</v>
       </c>
-      <c r="G48">
-        <v>6264084.751326288</v>
+      <c r="G48" t="s">
+        <v>188</v>
       </c>
       <c r="H48">
         <v>38785844.374162</v>
       </c>
       <c r="I48">
-        <v>130320437.0971844</v>
+        <v>130320437.0971842</v>
       </c>
       <c r="J48">
         <v>100</v>
       </c>
       <c r="K48">
-        <v>33.60000000000001</v>
+        <v>33.59999999999998</v>
       </c>
       <c r="L48">
         <v>3700552.097367561</v>
@@ -3040,28 +3232,28 @@
         <v>39596</v>
       </c>
       <c r="D49">
-        <v>11.52000000000001</v>
+        <v>11.52</v>
       </c>
       <c r="E49" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F49">
         <v>2.3</v>
       </c>
-      <c r="G49">
-        <v>27007138.60142434</v>
+      <c r="G49" t="s">
+        <v>166</v>
       </c>
       <c r="H49">
         <v>38785844.374162</v>
       </c>
       <c r="I49">
-        <v>446812927.1903465</v>
+        <v>446812927.1903463</v>
       </c>
       <c r="J49">
         <v>100</v>
       </c>
       <c r="K49">
-        <v>115.2000000000001</v>
+        <v>115.2</v>
       </c>
       <c r="L49">
         <v>5273515.054654035</v>
@@ -3075,34 +3267,34 @@
         <v>124</v>
       </c>
       <c r="C50">
-        <v>58710</v>
+        <v>39326</v>
       </c>
       <c r="D50">
-        <v>8.060000000000009</v>
+        <v>2.550000000000001</v>
       </c>
       <c r="E50" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F50">
         <v>2.5</v>
       </c>
-      <c r="G50">
-        <v>15010968.32739887</v>
+      <c r="G50" t="s">
+        <v>189</v>
       </c>
       <c r="H50">
         <v>39097761.98338025</v>
       </c>
       <c r="I50">
-        <v>315127961.5860452</v>
+        <v>99699293.05761966</v>
       </c>
       <c r="J50">
         <v>100</v>
       </c>
       <c r="K50">
-        <v>80.60000000000009</v>
+        <v>25.50000000000001</v>
       </c>
       <c r="L50">
-        <v>4573255.840545377</v>
+        <v>3461586.123553794</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -3113,34 +3305,34 @@
         <v>125</v>
       </c>
       <c r="C51">
-        <v>59075</v>
+        <v>39418</v>
       </c>
       <c r="D51">
-        <v>2.550000000000002</v>
+        <v>1.960000000000001</v>
       </c>
       <c r="E51" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F51">
         <v>2.5</v>
       </c>
-      <c r="G51">
-        <v>4754832.319820861</v>
+      <c r="G51" t="s">
+        <v>190</v>
       </c>
       <c r="H51">
         <v>39097761.98338025</v>
       </c>
       <c r="I51">
-        <v>99699293.05761971</v>
+        <v>76631613.48742531</v>
       </c>
       <c r="J51">
         <v>100</v>
       </c>
       <c r="K51">
-        <v>25.50000000000001</v>
+        <v>19.6</v>
       </c>
       <c r="L51">
-        <v>3461586.123553794</v>
+        <v>3248017.696927753</v>
       </c>
     </row>
     <row r="52" spans="1:12">
@@ -3151,34 +3343,34 @@
         <v>126</v>
       </c>
       <c r="C52">
-        <v>37218</v>
+        <v>58710</v>
       </c>
       <c r="D52">
-        <v>3.740000000000001</v>
+        <v>8.059999999999999</v>
       </c>
       <c r="E52" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F52">
-        <v>2.7</v>
-      </c>
-      <c r="G52">
-        <v>6971945.468368442</v>
+        <v>2.5</v>
+      </c>
+      <c r="G52" t="s">
+        <v>191</v>
       </c>
       <c r="H52">
-        <v>39380047.41901974</v>
+        <v>39097761.98338025</v>
       </c>
       <c r="I52">
-        <v>147281377.3471339</v>
+        <v>315127961.5860448</v>
       </c>
       <c r="J52">
         <v>100</v>
       </c>
       <c r="K52">
-        <v>37.40000000000001</v>
+        <v>80.59999999999999</v>
       </c>
       <c r="L52">
-        <v>3797758.507656866</v>
+        <v>4573255.840545377</v>
       </c>
     </row>
     <row r="53" spans="1:12">
@@ -3189,34 +3381,34 @@
         <v>127</v>
       </c>
       <c r="C53">
-        <v>37355</v>
+        <v>59075</v>
       </c>
       <c r="D53">
-        <v>10.2</v>
+        <v>2.550000000000001</v>
       </c>
       <c r="E53" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F53">
-        <v>2.9</v>
-      </c>
-      <c r="G53">
-        <v>18987662.48066654</v>
+        <v>2.5</v>
+      </c>
+      <c r="G53" t="s">
+        <v>189</v>
       </c>
       <c r="H53">
-        <v>39635749.05499732</v>
+        <v>39097761.98338025</v>
       </c>
       <c r="I53">
-        <v>404284640.3609725</v>
+        <v>99699293.05761966</v>
       </c>
       <c r="J53">
         <v>100</v>
       </c>
       <c r="K53">
-        <v>102</v>
+        <v>25.50000000000001</v>
       </c>
       <c r="L53">
-        <v>4841430.024186624</v>
+        <v>3461586.123553794</v>
       </c>
     </row>
     <row r="54" spans="1:12">
@@ -3227,34 +3419,34 @@
         <v>128</v>
       </c>
       <c r="C54">
-        <v>45329</v>
+        <v>37218</v>
       </c>
       <c r="D54">
-        <v>6.19</v>
+        <v>3.740000000000002</v>
       </c>
       <c r="E54" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F54">
-        <v>3</v>
-      </c>
-      <c r="G54">
-        <v>11532970.80719121</v>
+        <v>2.7</v>
+      </c>
+      <c r="G54" t="s">
+        <v>192</v>
       </c>
       <c r="H54">
-        <v>39754521.5981693</v>
+        <v>39380047.41901974</v>
       </c>
       <c r="I54">
-        <v>246080488.6926679</v>
+        <v>147281377.3471339</v>
       </c>
       <c r="J54">
         <v>100</v>
       </c>
       <c r="K54">
-        <v>61.89999999999999</v>
+        <v>37.40000000000003</v>
       </c>
       <c r="L54">
-        <v>4290239.673387973</v>
+        <v>3797758.507656866</v>
       </c>
     </row>
     <row r="55" spans="1:12">
@@ -3265,34 +3457,34 @@
         <v>129</v>
       </c>
       <c r="C55">
-        <v>45699</v>
+        <v>37355</v>
       </c>
       <c r="D55">
-        <v>6.690000000000076</v>
+        <v>10.19999999999999</v>
       </c>
       <c r="E55" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F55">
-        <v>3</v>
-      </c>
-      <c r="G55">
-        <v>12463194.18863161</v>
+        <v>2.9</v>
+      </c>
+      <c r="G55" t="s">
+        <v>193</v>
       </c>
       <c r="H55">
-        <v>39754521.5981693</v>
+        <v>39635749.05499732</v>
       </c>
       <c r="I55">
-        <v>265957749.4917556</v>
+        <v>404284640.3609722</v>
       </c>
       <c r="J55">
         <v>100</v>
       </c>
       <c r="K55">
-        <v>66.90000000000076</v>
+        <v>101.9999999999999</v>
       </c>
       <c r="L55">
-        <v>4371651.546027265</v>
+        <v>4841430.024186624</v>
       </c>
     </row>
     <row r="56" spans="1:12">
@@ -3303,34 +3495,34 @@
         <v>130</v>
       </c>
       <c r="C56">
-        <v>45899</v>
+        <v>45329</v>
       </c>
       <c r="D56">
-        <v>11.5</v>
+        <v>6.190000000000005</v>
       </c>
       <c r="E56" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F56">
         <v>3</v>
       </c>
-      <c r="G56">
-        <v>21401602.79478948</v>
+      <c r="G56" t="s">
+        <v>194</v>
       </c>
       <c r="H56">
         <v>39754521.5981693</v>
       </c>
       <c r="I56">
-        <v>457176998.3789469</v>
+        <v>246080488.6926681</v>
       </c>
       <c r="J56">
         <v>100</v>
       </c>
       <c r="K56">
-        <v>115</v>
+        <v>61.90000000000005</v>
       </c>
       <c r="L56">
-        <v>4984037.426968283</v>
+        <v>4290239.673387973</v>
       </c>
     </row>
     <row r="57" spans="1:12">
@@ -3341,34 +3533,34 @@
         <v>131</v>
       </c>
       <c r="C57">
-        <v>46049</v>
+        <v>45699</v>
       </c>
       <c r="D57">
-        <v>6.990000000000002</v>
+        <v>6.690000000000002</v>
       </c>
       <c r="E57" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F57">
         <v>3</v>
       </c>
-      <c r="G57">
-        <v>13021230.96247917</v>
+      <c r="G57" t="s">
+        <v>195</v>
       </c>
       <c r="H57">
         <v>39754521.5981693</v>
       </c>
       <c r="I57">
-        <v>277884105.9712034</v>
+        <v>265957749.4917527</v>
       </c>
       <c r="J57">
         <v>100</v>
       </c>
       <c r="K57">
-        <v>69.90000000000002</v>
+        <v>66.90000000000002</v>
       </c>
       <c r="L57">
-        <v>4418307.05254629</v>
+        <v>4371651.546027265</v>
       </c>
     </row>
     <row r="58" spans="1:12">
@@ -3379,34 +3571,34 @@
         <v>132</v>
       </c>
       <c r="C58">
-        <v>47053</v>
+        <v>45899</v>
       </c>
       <c r="D58">
-        <v>5.679999999999998</v>
+        <v>11.5</v>
       </c>
       <c r="E58" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F58">
         <v>3</v>
       </c>
-      <c r="G58">
-        <v>10583934.16780851</v>
+      <c r="G58" t="s">
+        <v>196</v>
       </c>
       <c r="H58">
         <v>39754521.5981693</v>
       </c>
       <c r="I58">
-        <v>225805682.6776015</v>
+        <v>457176998.3789468</v>
       </c>
       <c r="J58">
         <v>100</v>
       </c>
       <c r="K58">
-        <v>56.79999999999998</v>
+        <v>115</v>
       </c>
       <c r="L58">
-        <v>4201890.346963244</v>
+        <v>4984037.426968283</v>
       </c>
     </row>
     <row r="59" spans="1:12">
@@ -3417,34 +3609,34 @@
         <v>133</v>
       </c>
       <c r="C59">
-        <v>47166</v>
+        <v>46049</v>
       </c>
       <c r="D59">
-        <v>11.52</v>
+        <v>6.990000000000005</v>
       </c>
       <c r="E59" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F59">
         <v>3</v>
       </c>
-      <c r="G59">
-        <v>23628643.36424644</v>
+      <c r="G59" t="s">
+        <v>197</v>
       </c>
       <c r="H59">
         <v>39754521.5981693</v>
       </c>
       <c r="I59">
-        <v>457972088.8109104</v>
+        <v>277884105.9712036</v>
       </c>
       <c r="J59">
         <v>100</v>
       </c>
       <c r="K59">
-        <v>115.2</v>
+        <v>69.90000000000005</v>
       </c>
       <c r="L59">
-        <v>5105201.851214484</v>
+        <v>4418307.05254629</v>
       </c>
     </row>
     <row r="60" spans="1:12">
@@ -3455,34 +3647,34 @@
         <v>134</v>
       </c>
       <c r="C60">
-        <v>47166</v>
+        <v>47053</v>
       </c>
       <c r="D60">
-        <v>9.490000000000002</v>
+        <v>5.680000000000002</v>
       </c>
       <c r="E60" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F60">
         <v>3</v>
       </c>
-      <c r="G60">
-        <v>17668702.74772677</v>
+      <c r="G60" t="s">
+        <v>198</v>
       </c>
       <c r="H60">
         <v>39754521.5981693</v>
       </c>
       <c r="I60">
-        <v>377270409.9666267</v>
+        <v>225805682.6776017</v>
       </c>
       <c r="J60">
         <v>100</v>
       </c>
       <c r="K60">
-        <v>94.90000000000002</v>
+        <v>56.80000000000003</v>
       </c>
       <c r="L60">
-        <v>4757631.938664145</v>
+        <v>4201890.346963244</v>
       </c>
     </row>
     <row r="61" spans="1:12">
@@ -3496,31 +3688,31 @@
         <v>47166</v>
       </c>
       <c r="D61">
-        <v>4.890000000000001</v>
+        <v>11.52</v>
       </c>
       <c r="E61" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F61">
         <v>3</v>
       </c>
-      <c r="G61">
-        <v>9113441.365831105</v>
+      <c r="G61" t="s">
+        <v>199</v>
       </c>
       <c r="H61">
         <v>39754521.5981693</v>
       </c>
       <c r="I61">
-        <v>194399610.6150479</v>
+        <v>457972088.8109104</v>
       </c>
       <c r="J61">
         <v>100</v>
       </c>
       <c r="K61">
-        <v>48.90000000000001</v>
+        <v>115.2</v>
       </c>
       <c r="L61">
-        <v>4052333.328712357</v>
+        <v>5105201.851214484</v>
       </c>
     </row>
     <row r="62" spans="1:12">
@@ -3531,34 +3723,34 @@
         <v>136</v>
       </c>
       <c r="C62">
-        <v>47259</v>
+        <v>47166</v>
       </c>
       <c r="D62">
-        <v>11.52</v>
+        <v>9.490000000000038</v>
       </c>
       <c r="E62" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F62">
         <v>3</v>
       </c>
-      <c r="G62">
-        <v>27007138.60142434</v>
+      <c r="G62" t="s">
+        <v>200</v>
       </c>
       <c r="H62">
         <v>39754521.5981693</v>
       </c>
       <c r="I62">
-        <v>457972088.8109105</v>
+        <v>377270409.9666281</v>
       </c>
       <c r="J62">
         <v>100</v>
       </c>
       <c r="K62">
-        <v>115.2</v>
+        <v>94.90000000000038</v>
       </c>
       <c r="L62">
-        <v>5273515.054654035</v>
+        <v>4757631.938664145</v>
       </c>
     </row>
     <row r="63" spans="1:12">
@@ -3569,34 +3761,34 @@
         <v>137</v>
       </c>
       <c r="C63">
-        <v>47495</v>
+        <v>47166</v>
       </c>
       <c r="D63">
-        <v>8.059999999999997</v>
+        <v>4.889999999999994</v>
       </c>
       <c r="E63" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F63">
         <v>3</v>
       </c>
-      <c r="G63">
-        <v>15010968.32739887</v>
+      <c r="G63" t="s">
+        <v>164</v>
       </c>
       <c r="H63">
         <v>39754521.5981693</v>
       </c>
       <c r="I63">
-        <v>320421444.0812444</v>
+        <v>194399610.6150476</v>
       </c>
       <c r="J63">
         <v>100</v>
       </c>
       <c r="K63">
-        <v>80.59999999999997</v>
+        <v>48.89999999999994</v>
       </c>
       <c r="L63">
-        <v>4573255.840545377</v>
+        <v>4052333.328712357</v>
       </c>
     </row>
     <row r="64" spans="1:12">
@@ -3607,34 +3799,148 @@
         <v>138</v>
       </c>
       <c r="C64">
-        <v>4564</v>
+        <v>47198</v>
       </c>
       <c r="D64">
-        <v>10.93491958650111</v>
+        <v>3.93</v>
       </c>
       <c r="E64" t="s">
+        <v>143</v>
+      </c>
+      <c r="F64">
+        <v>3</v>
+      </c>
+      <c r="G64" t="s">
+        <v>201</v>
+      </c>
+      <c r="H64">
+        <v>39754521.5981693</v>
+      </c>
+      <c r="I64">
+        <v>156235269.8808053</v>
+      </c>
+      <c r="J64">
+        <v>100</v>
+      </c>
+      <c r="K64">
+        <v>39.3</v>
+      </c>
+      <c r="L64">
+        <v>3843575.485457812</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
+      <c r="A65" s="1">
+        <v>63</v>
+      </c>
+      <c r="B65" t="s">
         <v>139</v>
       </c>
-      <c r="F64">
+      <c r="C65">
+        <v>47495</v>
+      </c>
+      <c r="D65">
+        <v>8.060000000000004</v>
+      </c>
+      <c r="E65" t="s">
+        <v>143</v>
+      </c>
+      <c r="F65">
+        <v>3</v>
+      </c>
+      <c r="G65" t="s">
+        <v>191</v>
+      </c>
+      <c r="H65">
+        <v>39754521.5981693</v>
+      </c>
+      <c r="I65">
+        <v>320421444.0812447</v>
+      </c>
+      <c r="J65">
+        <v>100</v>
+      </c>
+      <c r="K65">
+        <v>80.60000000000004</v>
+      </c>
+      <c r="L65">
+        <v>4573255.840545377</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12">
+      <c r="A66" s="1">
+        <v>64</v>
+      </c>
+      <c r="B66" t="s">
+        <v>140</v>
+      </c>
+      <c r="C66">
+        <v>13597</v>
+      </c>
+      <c r="D66">
+        <v>3.98</v>
+      </c>
+      <c r="E66" t="s">
+        <v>142</v>
+      </c>
+      <c r="F66">
+        <v>3.1</v>
+      </c>
+      <c r="G66" t="s">
+        <v>202</v>
+      </c>
+      <c r="H66">
+        <v>39867684.89458863</v>
+      </c>
+      <c r="I66">
+        <v>158673385.8804628</v>
+      </c>
+      <c r="J66">
+        <v>100</v>
+      </c>
+      <c r="K66">
+        <v>39.8</v>
+      </c>
+      <c r="L66">
+        <v>3855352.754713441</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12">
+      <c r="A67" s="1">
+        <v>65</v>
+      </c>
+      <c r="B67" t="s">
+        <v>141</v>
+      </c>
+      <c r="C67">
+        <v>50354</v>
+      </c>
+      <c r="D67">
+        <v>10.61579412507253</v>
+      </c>
+      <c r="E67" t="s">
+        <v>142</v>
+      </c>
+      <c r="F67">
         <v>3.5</v>
       </c>
-      <c r="G64">
-        <v>21030316.26973897</v>
-      </c>
-      <c r="H64">
+      <c r="G67" t="s">
+        <v>203</v>
+      </c>
+      <c r="H67">
         <v>40270228.28044015</v>
       </c>
-      <c r="I64">
-        <v>440351707.9766559</v>
-      </c>
-      <c r="J64">
-        <v>100</v>
-      </c>
-      <c r="K64">
-        <v>109.3491958650111</v>
-      </c>
-      <c r="L64">
-        <v>4962921.442981876</v>
+      <c r="I67">
+        <v>427500452.7948263</v>
+      </c>
+      <c r="J67">
+        <v>100</v>
+      </c>
+      <c r="K67">
+        <v>106.1579412507253</v>
+      </c>
+      <c r="L67">
+        <v>4908863.618608388</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Can now name input file
Also started work on porting in some new data
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -194,24 +194,24 @@
     <t>MethaneHubUsage</t>
   </si>
   <si>
+    <t>tkm-SZMUsage</t>
+  </si>
+  <si>
+    <t>pkmUsage</t>
+  </si>
+  <si>
+    <t>tkm-N2Usage</t>
+  </si>
+  <si>
     <t>tkm-N3Usage</t>
   </si>
   <si>
-    <t>tkm-SZMUsage</t>
-  </si>
-  <si>
-    <t>pkmUsage</t>
-  </si>
-  <si>
     <t>keroseneUsage</t>
   </si>
   <si>
     <t>tkm-N1Usage</t>
   </si>
   <si>
-    <t>tkm-N2Usage</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -419,6 +419,9 @@
     <t>GMVA Gemeinschafts-Müllverbrennungsanlage Niederrhein GmbH</t>
   </si>
   <si>
+    <t>ArcelorMittal Bremen GmbH Kokerei Prosper</t>
+  </si>
+  <si>
     <t>DK Recycling und Roheisen GmbH</t>
   </si>
   <si>
@@ -437,18 +440,15 @@
     <t>Solvay Chemicals GmbH</t>
   </si>
   <si>
-    <t>BSR / MHKW</t>
-  </si>
-  <si>
     <t>RWE Power AG-Fabrik Ville/Berrenrath</t>
   </si>
   <si>
+    <t>PtF-FT1</t>
+  </si>
+  <si>
     <t>MtG</t>
   </si>
   <si>
-    <t>PtF-FT1</t>
-  </si>
-  <si>
     <t>{'Meth': 3487393.97800187, 'MtG': 4444727.840108303, 'FT': 4879006.727884552}</t>
   </si>
   <si>
@@ -611,6 +611,9 @@
     <t>{'Meth': 13021230.962479174, 'MtG': 16614250.054736383, 'FT': 18237570.603162043}</t>
   </si>
   <si>
+    <t>{'Meth': 7046450.302235504, 'MtG': 8984530.072518388, 'FT': 9862377.23604471}</t>
+  </si>
+  <si>
     <t>{'Meth': 10583934.167808509, 'MtG': 13500563.706853025, 'FT': 14819656.799135963}</t>
   </si>
   <si>
@@ -621,9 +624,6 @@
   </si>
   <si>
     <t>{'Meth': 7325831.86001466, 'MtG': 9341059.04365007, 'FT': 10253741.41207823}</t>
-  </si>
-  <si>
-    <t>{'Meth': 7418954.986766862, 'MtG': 9459902.034027299, 'FT': 10384196.137422739}</t>
   </si>
   <si>
     <t>{'Meth': 20101958.5303517, 'MtG': 25670085.921481106, 'FT': 28178220.674413458}</t>
@@ -1192,7 +1192,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>13506690818.90995</v>
+        <v>13506213488.67132</v>
       </c>
       <c r="C2">
         <v>96</v>
@@ -1204,34 +1204,34 @@
         <v>157.5538327091136</v>
       </c>
       <c r="F2">
-        <v>400</v>
+        <v>399.9999999999999</v>
       </c>
       <c r="G2">
-        <v>331.0757941250727</v>
+        <v>331.0598351407165</v>
       </c>
       <c r="H2">
-        <v>30.15963365760841</v>
+        <v>30.26026966650523</v>
       </c>
       <c r="I2">
-        <v>858.4615384615383</v>
+        <v>858.4615384615339</v>
       </c>
       <c r="J2">
-        <v>240</v>
+        <v>239.9999999999987</v>
       </c>
       <c r="K2">
-        <v>498.4615384615384</v>
+        <v>498.4615384615358</v>
       </c>
       <c r="L2">
-        <v>120</v>
+        <v>119.9999999999994</v>
       </c>
       <c r="M2">
-        <v>248.7145732819791</v>
+        <v>248.7145732819835</v>
       </c>
       <c r="N2">
-        <v>80.8827880591802</v>
+        <v>80.88278805918165</v>
       </c>
       <c r="O2">
-        <v>167.8317852227989</v>
+        <v>167.8317852228019</v>
       </c>
       <c r="P2">
         <v>154.0911111111111</v>
@@ -1240,10 +1240,10 @@
         <v>154.0911111111111</v>
       </c>
       <c r="R2">
-        <v>216</v>
+        <v>215.9999999999999</v>
       </c>
       <c r="S2">
-        <v>216</v>
+        <v>215.9999999999999</v>
       </c>
       <c r="T2">
         <v>0</v>
@@ -1258,31 +1258,31 @@
         <v>0</v>
       </c>
       <c r="X2">
-        <v>141.9507589561625</v>
+        <v>138.0507946936537</v>
       </c>
       <c r="Y2">
-        <v>141.9507589561625</v>
+        <v>138.0507946936537</v>
       </c>
       <c r="Z2">
-        <v>141.6084210526316</v>
+        <v>145.3642105263158</v>
       </c>
       <c r="AA2">
-        <v>43.76093567251463</v>
+        <v>44.92157894736842</v>
       </c>
       <c r="AB2">
-        <v>97.84748538011695</v>
+        <v>100.4426315789473</v>
       </c>
       <c r="AC2">
-        <v>-6.564332929285719e-18</v>
+        <v>0</v>
       </c>
       <c r="AD2">
-        <v>-1.608261567675001e-18</v>
+        <v>0</v>
       </c>
       <c r="AE2">
-        <v>-1.969299878785716e-19</v>
+        <v>0</v>
       </c>
       <c r="AF2">
-        <v>-4.759141373732146e-18</v>
+        <v>0</v>
       </c>
       <c r="AG2">
         <v>0</v>
@@ -1291,16 +1291,16 @@
         <v>0</v>
       </c>
       <c r="AI2">
-        <v>399.9430126483085</v>
+        <v>397.7803908159494</v>
       </c>
       <c r="AJ2">
-        <v>399.9430126483085</v>
+        <v>397.7803908159494</v>
       </c>
       <c r="AK2">
-        <v>372.0569873516916</v>
+        <v>374.2196091840507</v>
       </c>
       <c r="AL2">
-        <v>372.0569873516916</v>
+        <v>374.2196091840507</v>
       </c>
       <c r="AM2">
         <v>6.75</v>
@@ -1357,10 +1357,10 @@
         <v>41.45</v>
       </c>
       <c r="BE2">
-        <v>506.5944826878574</v>
+        <v>503.8551617002026</v>
       </c>
       <c r="BF2">
-        <v>980.1408090644542</v>
+        <v>982.7359552632849</v>
       </c>
       <c r="BG2">
         <v>120</v>
@@ -1369,22 +1369,22 @@
         <v>154.0911111111111</v>
       </c>
       <c r="BI2">
+        <v>414.5</v>
+      </c>
+      <c r="BJ2">
+        <v>858.0000000000001</v>
+      </c>
+      <c r="BK2">
+        <v>24.2</v>
+      </c>
+      <c r="BL2">
         <v>130.3</v>
       </c>
-      <c r="BJ2">
-        <v>414.5</v>
-      </c>
-      <c r="BK2">
-        <v>858</v>
-      </c>
-      <c r="BL2">
+      <c r="BM2">
         <v>120</v>
       </c>
-      <c r="BM2">
+      <c r="BN2">
         <v>7.5</v>
-      </c>
-      <c r="BN2">
-        <v>24.2</v>
       </c>
     </row>
   </sheetData>
@@ -1461,7 +1461,7 @@
         <v>33331633.33333333</v>
       </c>
       <c r="I2">
-        <v>62330154.33333338</v>
+        <v>62330154.33333337</v>
       </c>
       <c r="J2">
         <v>100</v>
@@ -1484,10 +1484,10 @@
         <v>25541</v>
       </c>
       <c r="D3">
-        <v>1.660000000000003</v>
+        <v>1.66</v>
       </c>
       <c r="E3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1499,13 +1499,13 @@
         <v>33331633.33333333</v>
       </c>
       <c r="I3">
-        <v>55330511.33333343</v>
+        <v>55330511.33333334</v>
       </c>
       <c r="J3">
         <v>100</v>
       </c>
       <c r="K3">
-        <v>16.60000000000003</v>
+        <v>16.6</v>
       </c>
       <c r="L3">
         <v>3120028.598903444</v>
@@ -1522,10 +1522,10 @@
         <v>25572</v>
       </c>
       <c r="D4">
-        <v>8.560000000000009</v>
+        <v>8.559999999999995</v>
       </c>
       <c r="E4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F4">
         <v>0.1</v>
@@ -1537,13 +1537,13 @@
         <v>33429264.21745752</v>
       </c>
       <c r="I4">
-        <v>286154501.7014366</v>
+        <v>286154501.7014362</v>
       </c>
       <c r="J4">
         <v>100</v>
       </c>
       <c r="K4">
-        <v>85.60000000000009</v>
+        <v>85.59999999999995</v>
       </c>
       <c r="L4">
         <v>4640353.526253123</v>
@@ -1560,7 +1560,7 @@
         <v>25734</v>
       </c>
       <c r="D5">
-        <v>9.729999999999999</v>
+        <v>9.729999999999997</v>
       </c>
       <c r="E5" t="s">
         <v>142</v>
@@ -1581,7 +1581,7 @@
         <v>100</v>
       </c>
       <c r="K5">
-        <v>97.29999999999998</v>
+        <v>97.29999999999997</v>
       </c>
       <c r="L5">
         <v>4786474.22858194</v>
@@ -1598,7 +1598,7 @@
         <v>26388</v>
       </c>
       <c r="D6">
-        <v>1.47</v>
+        <v>1.469999999999999</v>
       </c>
       <c r="E6" t="s">
         <v>142</v>
@@ -1613,13 +1613,13 @@
         <v>33429264.21745752</v>
       </c>
       <c r="I6">
-        <v>49141018.39966254</v>
+        <v>49141018.39966252</v>
       </c>
       <c r="J6">
         <v>100</v>
       </c>
       <c r="K6">
-        <v>14.7</v>
+        <v>14.69999999999999</v>
       </c>
       <c r="L6">
         <v>3029585.493423196</v>
@@ -1639,7 +1639,7 @@
         <v>11.52</v>
       </c>
       <c r="E7" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F7">
         <v>0.2</v>
@@ -1651,7 +1651,7 @@
         <v>33609222.38641504</v>
       </c>
       <c r="I7">
-        <v>387178241.8915014</v>
+        <v>387178241.8915013</v>
       </c>
       <c r="J7">
         <v>100</v>
@@ -1674,10 +1674,10 @@
         <v>26316</v>
       </c>
       <c r="D8">
-        <v>2.969999999999998</v>
+        <v>2.969999999999999</v>
       </c>
       <c r="E8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F8">
         <v>0.2</v>
@@ -1689,13 +1689,13 @@
         <v>33609222.38641504</v>
       </c>
       <c r="I8">
-        <v>99819390.48765258</v>
+        <v>99819390.48765263</v>
       </c>
       <c r="J8">
         <v>100</v>
       </c>
       <c r="K8">
-        <v>29.69999999999997</v>
+        <v>29.69999999999999</v>
       </c>
       <c r="L8">
         <v>3591695.233391508</v>
@@ -1712,10 +1712,10 @@
         <v>26954</v>
       </c>
       <c r="D9">
-        <v>1.269999999999999</v>
+        <v>1.27</v>
       </c>
       <c r="E9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F9">
         <v>0.2</v>
@@ -1727,13 +1727,13 @@
         <v>33609222.38641504</v>
       </c>
       <c r="I9">
-        <v>42683712.43074708</v>
+        <v>42683712.43074709</v>
       </c>
       <c r="J9">
         <v>100</v>
       </c>
       <c r="K9">
-        <v>12.69999999999999</v>
+        <v>12.7</v>
       </c>
       <c r="L9">
         <v>2924239.357757165</v>
@@ -1750,10 +1750,10 @@
         <v>27570</v>
       </c>
       <c r="D10">
-        <v>2.850000000000002</v>
+        <v>2.850000000000001</v>
       </c>
       <c r="E10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F10">
         <v>0.2</v>
@@ -1765,13 +1765,13 @@
         <v>33609222.38641504</v>
       </c>
       <c r="I10">
-        <v>95786283.80128293</v>
+        <v>95786283.80128291</v>
       </c>
       <c r="J10">
         <v>100</v>
       </c>
       <c r="K10">
-        <v>28.50000000000002</v>
+        <v>28.50000000000001</v>
       </c>
       <c r="L10">
         <v>3556025.558079649</v>
@@ -1788,7 +1788,7 @@
         <v>26892</v>
       </c>
       <c r="D11">
-        <v>2.720000000000004</v>
+        <v>2.719999999999999</v>
       </c>
       <c r="E11" t="s">
         <v>143</v>
@@ -1803,13 +1803,13 @@
         <v>34374076.88937075</v>
       </c>
       <c r="I11">
-        <v>93497489.1390886</v>
+        <v>93497489.13908841</v>
       </c>
       <c r="J11">
         <v>100</v>
       </c>
       <c r="K11">
-        <v>27.20000000000004</v>
+        <v>27.19999999999999</v>
       </c>
       <c r="L11">
         <v>3516074.693055412</v>
@@ -1826,10 +1826,10 @@
         <v>24534</v>
       </c>
       <c r="D12">
-        <v>4</v>
+        <v>3.999999999999998</v>
       </c>
       <c r="E12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F12">
         <v>0.7</v>
@@ -1841,13 +1841,13 @@
         <v>34962685.86338257</v>
       </c>
       <c r="I12">
-        <v>139850743.4535303</v>
+        <v>139850743.4535302</v>
       </c>
       <c r="J12">
         <v>100</v>
       </c>
       <c r="K12">
-        <v>40</v>
+        <v>39.99999999999999</v>
       </c>
       <c r="L12">
         <v>3860032.27064468</v>
@@ -1879,7 +1879,7 @@
         <v>35112131.13005736</v>
       </c>
       <c r="I13">
-        <v>53721560.62898779</v>
+        <v>53721560.62898781</v>
       </c>
       <c r="J13">
         <v>100</v>
@@ -1902,10 +1902,10 @@
         <v>20539</v>
       </c>
       <c r="D14">
-        <v>1.710000000000002</v>
+        <v>1.710000000000001</v>
       </c>
       <c r="E14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F14">
         <v>0.75</v>
@@ -1917,13 +1917,13 @@
         <v>35112131.13005736</v>
       </c>
       <c r="I14">
-        <v>60041744.23239816</v>
+        <v>60041744.23239812</v>
       </c>
       <c r="J14">
         <v>100</v>
       </c>
       <c r="K14">
-        <v>17.10000000000002</v>
+        <v>17.10000000000001</v>
       </c>
       <c r="L14">
         <v>3142515.846107772</v>
@@ -1940,7 +1940,7 @@
         <v>21079</v>
       </c>
       <c r="D15">
-        <v>7.700000000000006</v>
+        <v>7.699999999999998</v>
       </c>
       <c r="E15" t="s">
         <v>143</v>
@@ -1955,13 +1955,13 @@
         <v>35112131.13005736</v>
       </c>
       <c r="I15">
-        <v>270363409.7014419</v>
+        <v>270363409.7014416</v>
       </c>
       <c r="J15">
         <v>100</v>
       </c>
       <c r="K15">
-        <v>77.00000000000006</v>
+        <v>76.99999999999999</v>
       </c>
       <c r="L15">
         <v>4522964.437644095</v>
@@ -1978,7 +1978,7 @@
         <v>21107</v>
       </c>
       <c r="D16">
-        <v>3.219999999999998</v>
+        <v>3.219999999999999</v>
       </c>
       <c r="E16" t="s">
         <v>142</v>
@@ -1999,7 +1999,7 @@
         <v>100</v>
       </c>
       <c r="K16">
-        <v>32.19999999999998</v>
+        <v>32.19999999999999</v>
       </c>
       <c r="L16">
         <v>3662634.134160224</v>
@@ -2019,7 +2019,7 @@
         <v>2.23</v>
       </c>
       <c r="E17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F17">
         <v>0.75</v>
@@ -2057,7 +2057,7 @@
         <v>3.23</v>
       </c>
       <c r="E18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F18">
         <v>0.75</v>
@@ -2095,7 +2095,7 @@
         <v>2.25</v>
       </c>
       <c r="E19" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F19">
         <v>0.75</v>
@@ -2107,7 +2107,7 @@
         <v>35112131.13005736</v>
       </c>
       <c r="I19">
-        <v>79002295.04262909</v>
+        <v>79002295.04262906</v>
       </c>
       <c r="J19">
         <v>100</v>
@@ -2130,10 +2130,10 @@
         <v>21683</v>
       </c>
       <c r="D20">
-        <v>5.960000000000003</v>
+        <v>5.960000000000001</v>
       </c>
       <c r="E20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F20">
         <v>0.75</v>
@@ -2145,13 +2145,13 @@
         <v>35112131.13005736</v>
       </c>
       <c r="I20">
-        <v>209268301.535142</v>
+        <v>209268301.5351419</v>
       </c>
       <c r="J20">
         <v>100</v>
       </c>
       <c r="K20">
-        <v>59.60000000000002</v>
+        <v>59.60000000000001</v>
       </c>
       <c r="L20">
         <v>4251106.766759329</v>
@@ -2168,10 +2168,10 @@
         <v>21683</v>
       </c>
       <c r="D21">
-        <v>4.140000000000014</v>
+        <v>4.140000000000001</v>
       </c>
       <c r="E21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F21">
         <v>0.75</v>
@@ -2183,13 +2183,13 @@
         <v>35112131.13005736</v>
       </c>
       <c r="I21">
-        <v>145364222.878438</v>
+        <v>145364222.8784375</v>
       </c>
       <c r="J21">
         <v>100</v>
       </c>
       <c r="K21">
-        <v>41.40000000000014</v>
+        <v>41.40000000000001</v>
       </c>
       <c r="L21">
         <v>3892301.737650325</v>
@@ -2209,7 +2209,7 @@
         <v>4.890000000000001</v>
       </c>
       <c r="E22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F22">
         <v>0.75</v>
@@ -2244,10 +2244,10 @@
         <v>22145</v>
       </c>
       <c r="D23">
-        <v>3.230000000000002</v>
+        <v>3.23</v>
       </c>
       <c r="E23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F23">
         <v>0.8</v>
@@ -2265,7 +2265,7 @@
         <v>100</v>
       </c>
       <c r="K23">
-        <v>32.30000000000003</v>
+        <v>32.3</v>
       </c>
       <c r="L23">
         <v>3665383.563029062</v>
@@ -2285,7 +2285,7 @@
         <v>1.309999999999999</v>
       </c>
       <c r="E24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F24">
         <v>0.8</v>
@@ -2323,7 +2323,7 @@
         <v>11.52</v>
       </c>
       <c r="E25" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F25">
         <v>0.8</v>
@@ -2335,7 +2335,7 @@
         <v>35261419.93911113</v>
       </c>
       <c r="I25">
-        <v>406211557.6985604</v>
+        <v>406211557.6985603</v>
       </c>
       <c r="J25">
         <v>100</v>
@@ -2358,7 +2358,7 @@
         <v>28237</v>
       </c>
       <c r="D26">
-        <v>5.490000000000001</v>
+        <v>5.490000000000002</v>
       </c>
       <c r="E26" t="s">
         <v>142</v>
@@ -2373,13 +2373,13 @@
         <v>35261419.93911113</v>
       </c>
       <c r="I26">
-        <v>193585195.4657201</v>
+        <v>193585195.4657202</v>
       </c>
       <c r="J26">
         <v>100</v>
       </c>
       <c r="K26">
-        <v>54.90000000000001</v>
+        <v>54.90000000000002</v>
       </c>
       <c r="L26">
         <v>4167435.864813926</v>
@@ -2411,7 +2411,7 @@
         <v>35261419.93911113</v>
       </c>
       <c r="I27">
-        <v>94853219.63620897</v>
+        <v>94853219.63620898</v>
       </c>
       <c r="J27">
         <v>100</v>
@@ -2437,7 +2437,7 @@
         <v>11.52</v>
       </c>
       <c r="E28" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F28">
         <v>1</v>
@@ -2472,7 +2472,7 @@
         <v>29525</v>
       </c>
       <c r="D29">
-        <v>1.649999999999998</v>
+        <v>1.649999999999999</v>
       </c>
       <c r="E29" t="s">
         <v>142</v>
@@ -2493,7 +2493,7 @@
         <v>100</v>
       </c>
       <c r="K29">
-        <v>16.49999999999998</v>
+        <v>16.49999999999999</v>
       </c>
       <c r="L29">
         <v>3115469.701891457</v>
@@ -2510,10 +2510,10 @@
         <v>30659</v>
       </c>
       <c r="D30">
-        <v>2.460000000000003</v>
+        <v>2.460000000000001</v>
       </c>
       <c r="E30" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F30">
         <v>1.7</v>
@@ -2525,13 +2525,13 @@
         <v>37640511.58399763</v>
       </c>
       <c r="I30">
-        <v>92595658.49663429</v>
+        <v>92595658.4966342</v>
       </c>
       <c r="J30">
         <v>100</v>
       </c>
       <c r="K30">
-        <v>24.60000000000003</v>
+        <v>24.60000000000001</v>
       </c>
       <c r="L30">
         <v>3431616.232505888</v>
@@ -2551,7 +2551,7 @@
         <v>1.100000000000001</v>
       </c>
       <c r="E31" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F31">
         <v>1.8</v>
@@ -2586,10 +2586,10 @@
         <v>49124</v>
       </c>
       <c r="D32">
-        <v>1.460000000000003</v>
+        <v>1.460000000000001</v>
       </c>
       <c r="E32" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F32">
         <v>1.8</v>
@@ -2601,13 +2601,13 @@
         <v>37855437.77268496</v>
       </c>
       <c r="I32">
-        <v>55268939.14812015</v>
+        <v>55268939.14812008</v>
       </c>
       <c r="J32">
         <v>100</v>
       </c>
       <c r="K32">
-        <v>14.60000000000003</v>
+        <v>14.60000000000001</v>
       </c>
       <c r="L32">
         <v>3024585.102161352</v>
@@ -2627,7 +2627,7 @@
         <v>10.1</v>
       </c>
       <c r="E33" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F33">
         <v>1.8</v>
@@ -2639,7 +2639,7 @@
         <v>37855437.77268496</v>
       </c>
       <c r="I33">
-        <v>382339921.5041182</v>
+        <v>382339921.5041181</v>
       </c>
       <c r="J33">
         <v>100</v>
@@ -2662,7 +2662,7 @@
         <v>49536</v>
       </c>
       <c r="D34">
-        <v>1.489999999999995</v>
+        <v>1.489999999999998</v>
       </c>
       <c r="E34" t="s">
         <v>143</v>
@@ -2677,13 +2677,13 @@
         <v>37855437.77268496</v>
       </c>
       <c r="I34">
-        <v>56404602.2813004</v>
+        <v>56404602.28130053</v>
       </c>
       <c r="J34">
         <v>100</v>
       </c>
       <c r="K34">
-        <v>14.89999999999995</v>
+        <v>14.89999999999998</v>
       </c>
       <c r="L34">
         <v>3039509.425943215</v>
@@ -2700,10 +2700,10 @@
         <v>49808</v>
       </c>
       <c r="D35">
-        <v>11.39999999999998</v>
+        <v>11.4</v>
       </c>
       <c r="E35" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F35">
         <v>1.8</v>
@@ -2715,13 +2715,13 @@
         <v>37855437.77268496</v>
       </c>
       <c r="I35">
-        <v>431551990.6086079</v>
+        <v>431551990.6086085</v>
       </c>
       <c r="J35">
         <v>100</v>
       </c>
       <c r="K35">
-        <v>113.9999999999998</v>
+        <v>114</v>
       </c>
       <c r="L35">
         <v>4973514.536159209</v>
@@ -2738,7 +2738,7 @@
         <v>49824</v>
       </c>
       <c r="D36">
-        <v>3.850000000000002</v>
+        <v>3.850000000000001</v>
       </c>
       <c r="E36" t="s">
         <v>143</v>
@@ -2753,13 +2753,13 @@
         <v>37855437.77268496</v>
       </c>
       <c r="I36">
-        <v>145743435.4248372</v>
+        <v>145743435.4248371</v>
       </c>
       <c r="J36">
         <v>100</v>
       </c>
       <c r="K36">
-        <v>38.50000000000002</v>
+        <v>38.50000000000001</v>
       </c>
       <c r="L36">
         <v>3824493.385265881</v>
@@ -2776,10 +2776,10 @@
         <v>49824</v>
       </c>
       <c r="D37">
-        <v>1.600000000000003</v>
+        <v>1.600000000000001</v>
       </c>
       <c r="E37" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F37">
         <v>1.8</v>
@@ -2791,13 +2791,13 @@
         <v>37855437.77268496</v>
       </c>
       <c r="I37">
-        <v>60568700.43629605</v>
+        <v>60568700.43629599</v>
       </c>
       <c r="J37">
         <v>100</v>
       </c>
       <c r="K37">
-        <v>16.00000000000003</v>
+        <v>16.00000000000001</v>
       </c>
       <c r="L37">
         <v>3092355.773228031</v>
@@ -2814,10 +2814,10 @@
         <v>31171</v>
       </c>
       <c r="D38">
-        <v>1.210000000000001</v>
+        <v>1.21</v>
       </c>
       <c r="E38" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F38">
         <v>1.9</v>
@@ -2829,13 +2829,13 @@
         <v>38060293.37896816</v>
       </c>
       <c r="I38">
-        <v>46052954.98855151</v>
+        <v>46052954.9885515</v>
       </c>
       <c r="J38">
         <v>100</v>
       </c>
       <c r="K38">
-        <v>12.10000000000001</v>
+        <v>12.1</v>
       </c>
       <c r="L38">
         <v>2890190.553294488</v>
@@ -2855,7 +2855,7 @@
         <v>1.640000000000001</v>
       </c>
       <c r="E39" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F39">
         <v>1.9</v>
@@ -2890,10 +2890,10 @@
         <v>31319</v>
       </c>
       <c r="D40">
-        <v>6.17</v>
+        <v>6.170000000000002</v>
       </c>
       <c r="E40" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F40">
         <v>1.9</v>
@@ -2905,13 +2905,13 @@
         <v>38060293.37896816</v>
       </c>
       <c r="I40">
-        <v>234832010.1482336</v>
+        <v>234832010.1482337</v>
       </c>
       <c r="J40">
         <v>100</v>
       </c>
       <c r="K40">
-        <v>61.7</v>
+        <v>61.70000000000002</v>
       </c>
       <c r="L40">
         <v>4286880.992309345</v>
@@ -2928,10 +2928,10 @@
         <v>31789</v>
       </c>
       <c r="D41">
-        <v>4.159999999999991</v>
+        <v>4.16</v>
       </c>
       <c r="E41" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F41">
         <v>1.9</v>
@@ -2943,13 +2943,13 @@
         <v>38060293.37896816</v>
       </c>
       <c r="I41">
-        <v>158330820.4565072</v>
+        <v>158330820.4565076</v>
       </c>
       <c r="J41">
         <v>100</v>
       </c>
       <c r="K41">
-        <v>41.59999999999991</v>
+        <v>41.6</v>
       </c>
       <c r="L41">
         <v>3896843.850100604</v>
@@ -2969,7 +2969,7 @@
         <v>11.52</v>
       </c>
       <c r="E42" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F42">
         <v>2</v>
@@ -2981,7 +2981,7 @@
         <v>38255392.02166688</v>
       </c>
       <c r="I42">
-        <v>440702116.0896024</v>
+        <v>440702116.0896025</v>
       </c>
       <c r="J42">
         <v>100</v>
@@ -3004,10 +3004,10 @@
         <v>31061</v>
       </c>
       <c r="D43">
-        <v>3.310000000000006</v>
+        <v>3.309999999999998</v>
       </c>
       <c r="E43" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F43">
         <v>2.1</v>
@@ -3019,13 +3019,13 @@
         <v>38441090.93970785</v>
       </c>
       <c r="I43">
-        <v>127240011.0104332</v>
+        <v>127240011.0104329</v>
       </c>
       <c r="J43">
         <v>100</v>
       </c>
       <c r="K43">
-        <v>33.10000000000006</v>
+        <v>33.09999999999998</v>
       </c>
       <c r="L43">
         <v>3687149.882920415</v>
@@ -3042,10 +3042,10 @@
         <v>33106</v>
       </c>
       <c r="D44">
-        <v>2.309999999999998</v>
+        <v>2.309999999999999</v>
       </c>
       <c r="E44" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F44">
         <v>2.3</v>
@@ -3057,13 +3057,13 @@
         <v>38785844.374162</v>
       </c>
       <c r="I44">
-        <v>89595300.50431414</v>
+        <v>89595300.50431415</v>
       </c>
       <c r="J44">
         <v>100</v>
       </c>
       <c r="K44">
-        <v>23.09999999999998</v>
+        <v>23.09999999999999</v>
       </c>
       <c r="L44">
         <v>3379765.097364126</v>
@@ -3080,7 +3080,7 @@
         <v>33332</v>
       </c>
       <c r="D45">
-        <v>2.579999999999999</v>
+        <v>2.579999999999998</v>
       </c>
       <c r="E45" t="s">
         <v>143</v>
@@ -3101,7 +3101,7 @@
         <v>100</v>
       </c>
       <c r="K45">
-        <v>25.79999999999999</v>
+        <v>25.79999999999998</v>
       </c>
       <c r="L45">
         <v>3471397.820165223</v>
@@ -3118,10 +3118,10 @@
         <v>33609</v>
       </c>
       <c r="D46">
-        <v>3.879999999999998</v>
+        <v>3.879999999999999</v>
       </c>
       <c r="E46" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F46">
         <v>2.3</v>
@@ -3139,7 +3139,7 @@
         <v>100</v>
       </c>
       <c r="K46">
-        <v>38.79999999999998</v>
+        <v>38.79999999999999</v>
       </c>
       <c r="L46">
         <v>3831684.085287054</v>
@@ -3156,10 +3156,10 @@
         <v>38372</v>
       </c>
       <c r="D47">
-        <v>4.469999999999998</v>
+        <v>4.469999999999999</v>
       </c>
       <c r="E47" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F47">
         <v>2.3</v>
@@ -3171,13 +3171,13 @@
         <v>38785844.374162</v>
       </c>
       <c r="I47">
-        <v>173372724.352504</v>
+        <v>173372724.3525041</v>
       </c>
       <c r="J47">
         <v>100</v>
       </c>
       <c r="K47">
-        <v>44.69999999999998</v>
+        <v>44.69999999999999</v>
       </c>
       <c r="L47">
         <v>3965215.892681056</v>
@@ -3194,10 +3194,10 @@
         <v>38723</v>
       </c>
       <c r="D48">
-        <v>3.359999999999998</v>
+        <v>3.359999999999999</v>
       </c>
       <c r="E48" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F48">
         <v>2.3</v>
@@ -3209,13 +3209,13 @@
         <v>38785844.374162</v>
       </c>
       <c r="I48">
-        <v>130320437.0971842</v>
+        <v>130320437.0971843</v>
       </c>
       <c r="J48">
         <v>100</v>
       </c>
       <c r="K48">
-        <v>33.59999999999998</v>
+        <v>33.59999999999999</v>
       </c>
       <c r="L48">
         <v>3700552.097367561</v>
@@ -3235,7 +3235,7 @@
         <v>11.52</v>
       </c>
       <c r="E49" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F49">
         <v>2.3</v>
@@ -3273,7 +3273,7 @@
         <v>2.550000000000001</v>
       </c>
       <c r="E50" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F50">
         <v>2.5</v>
@@ -3323,13 +3323,13 @@
         <v>39097761.98338025</v>
       </c>
       <c r="I51">
-        <v>76631613.48742531</v>
+        <v>76631613.48742533</v>
       </c>
       <c r="J51">
         <v>100</v>
       </c>
       <c r="K51">
-        <v>19.6</v>
+        <v>19.60000000000001</v>
       </c>
       <c r="L51">
         <v>3248017.696927753</v>
@@ -3346,10 +3346,10 @@
         <v>58710</v>
       </c>
       <c r="D52">
-        <v>8.059999999999999</v>
+        <v>8.060000000000002</v>
       </c>
       <c r="E52" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F52">
         <v>2.5</v>
@@ -3361,13 +3361,13 @@
         <v>39097761.98338025</v>
       </c>
       <c r="I52">
-        <v>315127961.5860448</v>
+        <v>315127961.5860449</v>
       </c>
       <c r="J52">
         <v>100</v>
       </c>
       <c r="K52">
-        <v>80.59999999999999</v>
+        <v>80.60000000000002</v>
       </c>
       <c r="L52">
         <v>4573255.840545377</v>
@@ -3387,7 +3387,7 @@
         <v>2.550000000000001</v>
       </c>
       <c r="E53" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F53">
         <v>2.5</v>
@@ -3443,7 +3443,7 @@
         <v>100</v>
       </c>
       <c r="K54">
-        <v>37.40000000000003</v>
+        <v>37.40000000000002</v>
       </c>
       <c r="L54">
         <v>3797758.507656866</v>
@@ -3460,7 +3460,7 @@
         <v>37355</v>
       </c>
       <c r="D55">
-        <v>10.19999999999999</v>
+        <v>10.2</v>
       </c>
       <c r="E55" t="s">
         <v>143</v>
@@ -3475,13 +3475,13 @@
         <v>39635749.05499732</v>
       </c>
       <c r="I55">
-        <v>404284640.3609722</v>
+        <v>404284640.3609725</v>
       </c>
       <c r="J55">
         <v>100</v>
       </c>
       <c r="K55">
-        <v>101.9999999999999</v>
+        <v>102</v>
       </c>
       <c r="L55">
         <v>4841430.024186624</v>
@@ -3498,7 +3498,7 @@
         <v>45329</v>
       </c>
       <c r="D56">
-        <v>6.190000000000005</v>
+        <v>6.190000000000001</v>
       </c>
       <c r="E56" t="s">
         <v>143</v>
@@ -3513,13 +3513,13 @@
         <v>39754521.5981693</v>
       </c>
       <c r="I56">
-        <v>246080488.6926681</v>
+        <v>246080488.692668</v>
       </c>
       <c r="J56">
         <v>100</v>
       </c>
       <c r="K56">
-        <v>61.90000000000005</v>
+        <v>61.90000000000001</v>
       </c>
       <c r="L56">
         <v>4290239.673387973</v>
@@ -3536,10 +3536,10 @@
         <v>45699</v>
       </c>
       <c r="D57">
-        <v>6.690000000000002</v>
+        <v>6.690000000000001</v>
       </c>
       <c r="E57" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F57">
         <v>3</v>
@@ -3557,7 +3557,7 @@
         <v>100</v>
       </c>
       <c r="K57">
-        <v>66.90000000000002</v>
+        <v>66.90000000000001</v>
       </c>
       <c r="L57">
         <v>4371651.546027265</v>
@@ -3589,7 +3589,7 @@
         <v>39754521.5981693</v>
       </c>
       <c r="I58">
-        <v>457176998.3789468</v>
+        <v>457176998.3789469</v>
       </c>
       <c r="J58">
         <v>100</v>
@@ -3612,10 +3612,10 @@
         <v>46049</v>
       </c>
       <c r="D59">
-        <v>6.990000000000005</v>
+        <v>6.990000000000002</v>
       </c>
       <c r="E59" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F59">
         <v>3</v>
@@ -3627,13 +3627,13 @@
         <v>39754521.5981693</v>
       </c>
       <c r="I59">
-        <v>277884105.9712036</v>
+        <v>277884105.9712034</v>
       </c>
       <c r="J59">
         <v>100</v>
       </c>
       <c r="K59">
-        <v>69.90000000000005</v>
+        <v>69.90000000000002</v>
       </c>
       <c r="L59">
         <v>4418307.05254629</v>
@@ -3647,13 +3647,13 @@
         <v>134</v>
       </c>
       <c r="C60">
-        <v>47053</v>
+        <v>46236</v>
       </c>
       <c r="D60">
-        <v>5.680000000000002</v>
+        <v>3.780000000000001</v>
       </c>
       <c r="E60" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F60">
         <v>3</v>
@@ -3665,16 +3665,16 @@
         <v>39754521.5981693</v>
       </c>
       <c r="I60">
-        <v>225805682.6776017</v>
+        <v>150272091.64108</v>
       </c>
       <c r="J60">
         <v>100</v>
       </c>
       <c r="K60">
-        <v>56.80000000000003</v>
+        <v>37.80000000000001</v>
       </c>
       <c r="L60">
-        <v>4201890.346963244</v>
+        <v>3807548.40454141</v>
       </c>
     </row>
     <row r="61" spans="1:12">
@@ -3685,13 +3685,13 @@
         <v>135</v>
       </c>
       <c r="C61">
-        <v>47166</v>
+        <v>47053</v>
       </c>
       <c r="D61">
-        <v>11.52</v>
+        <v>5.68</v>
       </c>
       <c r="E61" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F61">
         <v>3</v>
@@ -3703,16 +3703,16 @@
         <v>39754521.5981693</v>
       </c>
       <c r="I61">
-        <v>457972088.8109104</v>
+        <v>225805682.6776016</v>
       </c>
       <c r="J61">
         <v>100</v>
       </c>
       <c r="K61">
-        <v>115.2</v>
+        <v>56.8</v>
       </c>
       <c r="L61">
-        <v>5105201.851214484</v>
+        <v>4201890.346963244</v>
       </c>
     </row>
     <row r="62" spans="1:12">
@@ -3726,10 +3726,10 @@
         <v>47166</v>
       </c>
       <c r="D62">
-        <v>9.490000000000038</v>
+        <v>11.52</v>
       </c>
       <c r="E62" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F62">
         <v>3</v>
@@ -3741,16 +3741,16 @@
         <v>39754521.5981693</v>
       </c>
       <c r="I62">
-        <v>377270409.9666281</v>
+        <v>457972088.8109104</v>
       </c>
       <c r="J62">
         <v>100</v>
       </c>
       <c r="K62">
-        <v>94.90000000000038</v>
+        <v>115.2</v>
       </c>
       <c r="L62">
-        <v>4757631.938664145</v>
+        <v>5105201.851214484</v>
       </c>
     </row>
     <row r="63" spans="1:12">
@@ -3764,31 +3764,31 @@
         <v>47166</v>
       </c>
       <c r="D63">
-        <v>4.889999999999994</v>
+        <v>9.490000000000002</v>
       </c>
       <c r="E63" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F63">
         <v>3</v>
       </c>
       <c r="G63" t="s">
-        <v>164</v>
+        <v>201</v>
       </c>
       <c r="H63">
         <v>39754521.5981693</v>
       </c>
       <c r="I63">
-        <v>194399610.6150476</v>
+        <v>377270409.9666267</v>
       </c>
       <c r="J63">
         <v>100</v>
       </c>
       <c r="K63">
-        <v>48.89999999999994</v>
+        <v>94.90000000000002</v>
       </c>
       <c r="L63">
-        <v>4052333.328712357</v>
+        <v>4757631.938664145</v>
       </c>
     </row>
     <row r="64" spans="1:12">
@@ -3799,10 +3799,10 @@
         <v>138</v>
       </c>
       <c r="C64">
-        <v>47198</v>
+        <v>47166</v>
       </c>
       <c r="D64">
-        <v>3.93</v>
+        <v>4.890000000000001</v>
       </c>
       <c r="E64" t="s">
         <v>143</v>
@@ -3811,22 +3811,22 @@
         <v>3</v>
       </c>
       <c r="G64" t="s">
-        <v>201</v>
+        <v>164</v>
       </c>
       <c r="H64">
         <v>39754521.5981693</v>
       </c>
       <c r="I64">
-        <v>156235269.8808053</v>
+        <v>194399610.6150479</v>
       </c>
       <c r="J64">
         <v>100</v>
       </c>
       <c r="K64">
-        <v>39.3</v>
+        <v>48.90000000000001</v>
       </c>
       <c r="L64">
-        <v>3843575.485457812</v>
+        <v>4052333.328712357</v>
       </c>
     </row>
     <row r="65" spans="1:12">
@@ -3837,34 +3837,34 @@
         <v>139</v>
       </c>
       <c r="C65">
-        <v>47495</v>
+        <v>47198</v>
       </c>
       <c r="D65">
-        <v>8.060000000000004</v>
+        <v>3.93</v>
       </c>
       <c r="E65" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F65">
         <v>3</v>
       </c>
       <c r="G65" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
       <c r="H65">
         <v>39754521.5981693</v>
       </c>
       <c r="I65">
-        <v>320421444.0812447</v>
+        <v>156235269.8808053</v>
       </c>
       <c r="J65">
         <v>100</v>
       </c>
       <c r="K65">
-        <v>80.60000000000004</v>
+        <v>39.3</v>
       </c>
       <c r="L65">
-        <v>4573255.840545377</v>
+        <v>3843575.485457812</v>
       </c>
     </row>
     <row r="66" spans="1:12">
@@ -3875,34 +3875,34 @@
         <v>140</v>
       </c>
       <c r="C66">
-        <v>13597</v>
+        <v>47495</v>
       </c>
       <c r="D66">
-        <v>3.98</v>
+        <v>8.06</v>
       </c>
       <c r="E66" t="s">
         <v>142</v>
       </c>
       <c r="F66">
-        <v>3.1</v>
+        <v>3</v>
       </c>
       <c r="G66" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="H66">
-        <v>39867684.89458863</v>
+        <v>39754521.5981693</v>
       </c>
       <c r="I66">
-        <v>158673385.8804628</v>
+        <v>320421444.0812445</v>
       </c>
       <c r="J66">
         <v>100</v>
       </c>
       <c r="K66">
-        <v>39.8</v>
+        <v>80.60000000000001</v>
       </c>
       <c r="L66">
-        <v>3855352.754713441</v>
+        <v>4573255.840545377</v>
       </c>
     </row>
     <row r="67" spans="1:12">
@@ -3916,10 +3916,10 @@
         <v>50354</v>
       </c>
       <c r="D67">
-        <v>10.61579412507253</v>
+        <v>10.79983514071649</v>
       </c>
       <c r="E67" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F67">
         <v>3.5</v>
@@ -3931,13 +3931,13 @@
         <v>40270228.28044015</v>
       </c>
       <c r="I67">
-        <v>427500452.7948263</v>
+        <v>434911826.5077725</v>
       </c>
       <c r="J67">
         <v>100</v>
       </c>
       <c r="K67">
-        <v>106.1579412507253</v>
+        <v>107.9983514071649</v>
       </c>
       <c r="L67">
         <v>4908863.618608388</v>

</xml_diff>

<commit_message>
Made CO2 Plant Size Bounds Site Dependent
These values are now no longer directly input, but instead are
calculated from the plant's capacity in kg of CO2
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="141">
   <si>
     <t>Total Cost</t>
   </si>
@@ -224,18 +224,18 @@
     <t>tkm-N3Usage</t>
   </si>
   <si>
+    <t>tkm-SZMUsage</t>
+  </si>
+  <si>
+    <t>tkm-N1Usage</t>
+  </si>
+  <si>
+    <t>tkm-N2Usage</t>
+  </si>
+  <si>
     <t>pkmUsage</t>
   </si>
   <si>
-    <t>tkm-N2Usage</t>
-  </si>
-  <si>
-    <t>tkm-N1Usage</t>
-  </si>
-  <si>
-    <t>tkm-SZMUsage</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -356,9 +356,15 @@
     <t>EEW Energy from Waste Hannover GmbH</t>
   </si>
   <si>
+    <t>Schoeller Technocell GmbH &amp; Co. KG</t>
+  </si>
+  <si>
     <t>Georgsmarienhütte GmbH</t>
   </si>
   <si>
+    <t>RAG Anthrazit Ibbenbüren GmbH</t>
+  </si>
+  <si>
     <t>Dyckerhoff GmbH, werk Lengerich</t>
   </si>
   <si>
@@ -374,6 +380,9 @@
     <t>EBE Holzheizkraftwerk GmbH</t>
   </si>
   <si>
+    <t>Nordzucker AG Werk Nordstemmen</t>
+  </si>
+  <si>
     <t>Peiner Träger GmbH</t>
   </si>
   <si>
@@ -392,6 +401,9 @@
     <t>Heidelberg Cement AG Zementwerk Paderborn</t>
   </si>
   <si>
+    <t>Pfleiderer Gütersloh GmbH (Werk 2)</t>
+  </si>
+  <si>
     <t>MVA Bielefeld-Herford GmbH</t>
   </si>
   <si>
@@ -404,13 +416,22 @@
     <t>Zellstoff Stendal GmbH</t>
   </si>
   <si>
-    <t>Rheinkalk GmbH Werk Hönnetal</t>
+    <t>Werk  Zielitz</t>
+  </si>
+  <si>
+    <t>Deuna Zement GmbH</t>
+  </si>
+  <si>
+    <t>Hagener Entsorgungsbetrieb HEB GmbH</t>
   </si>
   <si>
     <t>MtG</t>
   </si>
   <si>
     <t>PtF-MeOH</t>
+  </si>
+  <si>
+    <t>PtF-FT2</t>
   </si>
   <si>
     <t>PtF-DME</t>
@@ -1006,7 +1027,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>10261084987.95488</v>
+        <v>10395451552.85602</v>
       </c>
       <c r="C2">
         <v>96</v>
@@ -1021,31 +1042,31 @@
         <v>400</v>
       </c>
       <c r="G2">
-        <v>277.8056350617557</v>
+        <v>278.8279158149577</v>
       </c>
       <c r="H2">
-        <v>20.26196192689025</v>
+        <v>20.54999089349133</v>
       </c>
       <c r="I2">
-        <v>865.6153846153844</v>
+        <v>818.8317901721812</v>
       </c>
       <c r="J2">
-        <v>242</v>
+        <v>228.9207155320077</v>
       </c>
       <c r="K2">
-        <v>502.6153846153845</v>
+        <v>475.4507168741698</v>
       </c>
       <c r="L2">
-        <v>121</v>
+        <v>114.4603577660039</v>
       </c>
       <c r="M2">
-        <v>225.5180670115592</v>
+        <v>272.3016614547624</v>
       </c>
       <c r="N2">
-        <v>73.33920878424689</v>
+        <v>88.55338583894712</v>
       </c>
       <c r="O2">
-        <v>152.1788582273123</v>
+        <v>183.7482756158153</v>
       </c>
       <c r="P2">
         <v>176.2915151515151</v>
@@ -1084,31 +1105,31 @@
         <v>50.00000000000001</v>
       </c>
       <c r="AB2">
-        <v>114.7892669495623</v>
+        <v>109.7589866399234</v>
       </c>
       <c r="AC2">
-        <v>114.7892669495623</v>
+        <v>109.7589866399234</v>
       </c>
       <c r="AD2">
-        <v>29.10315789473685</v>
+        <v>25.77779706999457</v>
       </c>
       <c r="AE2">
-        <v>8.993684210526318</v>
+        <v>7.966055344546936</v>
       </c>
       <c r="AF2">
-        <v>20.10947368421052</v>
+        <v>17.81174172544764</v>
       </c>
       <c r="AG2">
-        <v>0</v>
+        <v>9.020196184822272</v>
       </c>
       <c r="AH2">
-        <v>0</v>
+        <v>2.209948065281456</v>
       </c>
       <c r="AI2">
-        <v>0</v>
+        <v>0.2706058855446682</v>
       </c>
       <c r="AJ2">
-        <v>0</v>
+        <v>6.539642233996148</v>
       </c>
       <c r="AK2">
         <v>0</v>
@@ -1117,10 +1138,10 @@
         <v>0</v>
       </c>
       <c r="AM2">
-        <v>49.99566329486784</v>
+        <v>49.19901804586726</v>
       </c>
       <c r="AN2">
-        <v>49.99566329486784</v>
+        <v>49.19901804586726</v>
       </c>
       <c r="AO2">
         <v>50</v>
@@ -1129,16 +1150,16 @@
         <v>50</v>
       </c>
       <c r="AQ2">
-        <v>386.1456499256868</v>
+        <v>384.1642969472952</v>
       </c>
       <c r="AR2">
-        <v>386.1456499256868</v>
+        <v>384.1642969472952</v>
       </c>
       <c r="AS2">
-        <v>368.7743500743131</v>
+        <v>370.7557030527048</v>
       </c>
       <c r="AT2">
-        <v>368.7743500743131</v>
+        <v>370.7557030527048</v>
       </c>
       <c r="AU2">
         <v>7.2</v>
@@ -1195,10 +1216,10 @@
         <v>38.85</v>
       </c>
       <c r="BM2">
-        <v>489.1178232392033</v>
+        <v>486.6081094665739</v>
       </c>
       <c r="BN2">
-        <v>941.723038270994</v>
+        <v>944.100661845064</v>
       </c>
       <c r="BO2">
         <v>121</v>
@@ -1213,16 +1234,16 @@
         <v>123.8</v>
       </c>
       <c r="BS2">
+        <v>388.5</v>
+      </c>
+      <c r="BT2">
+        <v>8</v>
+      </c>
+      <c r="BU2">
+        <v>26.2</v>
+      </c>
+      <c r="BV2">
         <v>838.8</v>
-      </c>
-      <c r="BT2">
-        <v>26.2</v>
-      </c>
-      <c r="BU2">
-        <v>8</v>
-      </c>
-      <c r="BV2">
-        <v>388.5</v>
       </c>
     </row>
   </sheetData>
@@ -1232,7 +1253,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L47"/>
+  <dimension ref="A1:L53"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1287,7 +1308,7 @@
         <v>2.762499999999999</v>
       </c>
       <c r="E2" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -1308,7 +1329,7 @@
         <v>18.7</v>
       </c>
       <c r="L2">
-        <v>3211279.34822684</v>
+        <v>3732706.505062939</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1325,7 +1346,7 @@
         <v>2.452272727272728</v>
       </c>
       <c r="E3" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1346,7 +1367,7 @@
         <v>16.6</v>
       </c>
       <c r="L3">
-        <v>3120028.598903444</v>
+        <v>3626639.03828233</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1363,7 +1384,7 @@
         <v>11.52</v>
       </c>
       <c r="E4" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="F4">
         <v>10</v>
@@ -1384,7 +1405,7 @@
         <v>79.30854271356787</v>
       </c>
       <c r="L4">
-        <v>5594639.70924738</v>
+        <v>6476561.045924471</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1398,31 +1419,31 @@
         <v>25734</v>
       </c>
       <c r="D5">
-        <v>11.52</v>
+        <v>7.222268041237111</v>
       </c>
       <c r="E5" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="F5">
         <v>10</v>
       </c>
       <c r="G5">
-        <v>612153.4459508199</v>
+        <v>471955.2073590848</v>
       </c>
       <c r="H5">
         <v>33429264.21745752</v>
       </c>
       <c r="I5">
-        <v>385105123.7851107</v>
+        <v>241435106.5998148</v>
       </c>
       <c r="J5">
         <v>100</v>
       </c>
       <c r="K5">
-        <v>79.30854271356787</v>
+        <v>97.3</v>
       </c>
       <c r="L5">
-        <v>5770810.054667593</v>
+        <v>4710073.692228228</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1436,31 +1457,31 @@
         <v>26388</v>
       </c>
       <c r="D6">
-        <v>2.171590909090909</v>
+        <v>2.135255474452553</v>
       </c>
       <c r="E6" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="F6">
         <v>10</v>
       </c>
       <c r="G6">
-        <v>151482.1833090819</v>
+        <v>120505.3208392468</v>
       </c>
       <c r="H6">
         <v>33429264.21745752</v>
       </c>
       <c r="I6">
-        <v>72594686.27222878</v>
+        <v>71380019.427247</v>
       </c>
       <c r="J6">
         <v>100</v>
       </c>
       <c r="K6">
-        <v>14.7</v>
+        <v>14.69999999999999</v>
       </c>
       <c r="L6">
-        <v>3029585.493423196</v>
+        <v>4228405.28873365</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1477,13 +1498,13 @@
         <v>11.52</v>
       </c>
       <c r="E7" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="F7">
         <v>20</v>
       </c>
       <c r="G7">
-        <v>768114.7751442149</v>
+        <v>612153.4459508199</v>
       </c>
       <c r="H7">
         <v>33609222.38641504</v>
@@ -1495,10 +1516,10 @@
         <v>100</v>
       </c>
       <c r="K7">
-        <v>77.98153846153848</v>
+        <v>79.30854271356787</v>
       </c>
       <c r="L7">
-        <v>5004876.854845014</v>
+        <v>6985327.79762394</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1515,7 +1536,7 @@
         <v>4.387499999999999</v>
       </c>
       <c r="E8" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="F8">
         <v>20</v>
@@ -1536,7 +1557,7 @@
         <v>29.7</v>
       </c>
       <c r="L8">
-        <v>3591695.233391508</v>
+        <v>4174891.906955022</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -1553,7 +1574,7 @@
         <v>1.876136363636363</v>
       </c>
       <c r="E9" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="F9">
         <v>20</v>
@@ -1565,16 +1586,16 @@
         <v>33609222.38641504</v>
       </c>
       <c r="I9">
-        <v>63055484.27269458</v>
+        <v>63055484.27269455</v>
       </c>
       <c r="J9">
         <v>100</v>
       </c>
       <c r="K9">
-        <v>12.7</v>
+        <v>12.69999999999999</v>
       </c>
       <c r="L9">
-        <v>2924239.357757165</v>
+        <v>3399058.782939054</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1588,22 +1609,22 @@
         <v>27570</v>
       </c>
       <c r="D10">
-        <v>4.210227272727273</v>
+        <v>4.258756476683939</v>
       </c>
       <c r="E10" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="F10">
         <v>20</v>
       </c>
       <c r="G10">
-        <v>290717.7264693647</v>
+        <v>239232.4574537762</v>
       </c>
       <c r="H10">
         <v>33609222.38641504</v>
       </c>
       <c r="I10">
-        <v>141502464.7064406</v>
+        <v>143133493.5144559</v>
       </c>
       <c r="J10">
         <v>100</v>
@@ -1612,7 +1633,7 @@
         <v>28.5</v>
       </c>
       <c r="L10">
-        <v>3556025.558079649</v>
+        <v>4568335.589196196</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1626,31 +1647,31 @@
         <v>26892</v>
       </c>
       <c r="D11">
-        <v>4.018181818181819</v>
+        <v>4.064497409326425</v>
       </c>
       <c r="E11" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="F11">
         <v>50</v>
       </c>
       <c r="G11">
-        <v>277720.7385821831</v>
+        <v>228612.3322807539</v>
       </c>
       <c r="H11">
         <v>34374076.88937075</v>
       </c>
       <c r="I11">
-        <v>138121290.7736534</v>
+        <v>139713346.4648347</v>
       </c>
       <c r="J11">
         <v>100</v>
       </c>
       <c r="K11">
-        <v>27.20000000000001</v>
+        <v>27.2</v>
       </c>
       <c r="L11">
-        <v>3516074.693055412</v>
+        <v>4517011.72902463</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -1664,31 +1685,31 @@
         <v>24534</v>
       </c>
       <c r="D12">
-        <v>5.90909090909091</v>
+        <v>5.977202072538859</v>
       </c>
       <c r="E12" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="F12">
         <v>70</v>
       </c>
       <c r="G12">
-        <v>404637.3354885659</v>
+        <v>332009.530752334</v>
       </c>
       <c r="H12">
         <v>34962685.86338257</v>
       </c>
       <c r="I12">
-        <v>206597689.1927152</v>
+        <v>208979038.4041353</v>
       </c>
       <c r="J12">
         <v>100</v>
       </c>
       <c r="K12">
-        <v>40.00000000000001</v>
+        <v>39.99999999999999</v>
       </c>
       <c r="L12">
-        <v>3860032.27064468</v>
+        <v>4958885.280609371</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1702,31 +1723,31 @@
         <v>20457</v>
       </c>
       <c r="D13">
-        <v>2.260227272727274</v>
+        <v>2.222408759124086</v>
       </c>
       <c r="E13" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="F13">
         <v>75</v>
       </c>
       <c r="G13">
-        <v>157594.8154876857</v>
+        <v>125351.7400645756</v>
       </c>
       <c r="H13">
         <v>35112131.13005736</v>
       </c>
       <c r="I13">
-        <v>79361396.38373198</v>
+        <v>78033507.77495298</v>
       </c>
       <c r="J13">
         <v>100</v>
       </c>
       <c r="K13">
-        <v>15.30000000000001</v>
+        <v>15.29999999999999</v>
       </c>
       <c r="L13">
-        <v>3059058.228987825</v>
+        <v>4269540.510434923</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1743,7 +1764,7 @@
         <v>2.526136363636365</v>
       </c>
       <c r="E14" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="F14">
         <v>75</v>
@@ -1764,7 +1785,7 @@
         <v>17.10000000000001</v>
       </c>
       <c r="L14">
-        <v>3142515.846107772</v>
+        <v>3652777.621948962</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1778,31 +1799,31 @@
         <v>21079</v>
       </c>
       <c r="D15">
-        <v>11.50611398963731</v>
+        <v>11.18467153284671</v>
       </c>
       <c r="E15" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="F15">
         <v>75</v>
       </c>
       <c r="G15">
-        <v>616913.5402400541</v>
+        <v>595578.0818916217</v>
       </c>
       <c r="H15">
         <v>35112131.13005736</v>
       </c>
       <c r="I15">
-        <v>404004183.2015327</v>
+        <v>392717653.5079336</v>
       </c>
       <c r="J15">
         <v>100</v>
       </c>
       <c r="K15">
-        <v>77.00000000000001</v>
+        <v>77</v>
       </c>
       <c r="L15">
-        <v>4985010.106808093</v>
+        <v>6312720.59838088</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1816,22 +1837,22 @@
         <v>21107</v>
       </c>
       <c r="D16">
-        <v>4.756818181818183</v>
+        <v>4.811647668393782</v>
       </c>
       <c r="E16" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="F16">
         <v>75</v>
       </c>
       <c r="G16">
-        <v>327575.6525297191</v>
+        <v>269310.7866974464</v>
       </c>
       <c r="H16">
         <v>35112131.13005736</v>
       </c>
       <c r="I16">
-        <v>167022023.7618411</v>
+        <v>168947203.8842773</v>
       </c>
       <c r="J16">
         <v>100</v>
@@ -1840,7 +1861,7 @@
         <v>32.2</v>
       </c>
       <c r="L16">
-        <v>3662634.134160224</v>
+        <v>4705292.915364972</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1857,7 +1878,7 @@
         <v>3.294318181818181</v>
       </c>
       <c r="E17" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="F17">
         <v>75</v>
@@ -1878,7 +1899,7 @@
         <v>22.29999999999999</v>
       </c>
       <c r="L17">
-        <v>3351059.927308201</v>
+        <v>3895183.767312502</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1892,10 +1913,10 @@
         <v>21119</v>
       </c>
       <c r="D18">
-        <v>4.771590909090912</v>
+        <v>4.771590909090911</v>
       </c>
       <c r="E18" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="F18">
         <v>75</v>
@@ -1913,10 +1934,10 @@
         <v>100</v>
       </c>
       <c r="K18">
-        <v>32.30000000000002</v>
+        <v>32.30000000000001</v>
       </c>
       <c r="L18">
-        <v>3665383.563029062</v>
+        <v>4260545.279819391</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1930,22 +1951,22 @@
         <v>21129</v>
       </c>
       <c r="D19">
-        <v>3.323863636363637</v>
+        <v>3.268248175182482</v>
       </c>
       <c r="E19" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="F19">
         <v>75</v>
       </c>
       <c r="G19">
-        <v>230526.0827522533</v>
+        <v>183076.4265540964</v>
       </c>
       <c r="H19">
         <v>35112131.13005736</v>
       </c>
       <c r="I19">
-        <v>116707935.8584293</v>
+        <v>114755158.492578</v>
       </c>
       <c r="J19">
         <v>100</v>
@@ -1954,7 +1975,7 @@
         <v>22.5</v>
       </c>
       <c r="L19">
-        <v>3358308.48673273</v>
+        <v>4687205.361039192</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1968,31 +1989,31 @@
         <v>21683</v>
       </c>
       <c r="D20">
-        <v>8.906031088082898</v>
+        <v>4.423917525773195</v>
       </c>
       <c r="E20" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="F20">
         <v>75</v>
       </c>
       <c r="G20">
-        <v>485437.7520006373</v>
+        <v>292473.7751894842</v>
       </c>
       <c r="H20">
         <v>35112131.13005736</v>
       </c>
       <c r="I20">
-        <v>312709731.4131342</v>
+        <v>155333172.2735074</v>
       </c>
       <c r="J20">
         <v>100</v>
       </c>
       <c r="K20">
-        <v>59.59999999999998</v>
+        <v>59.6</v>
       </c>
       <c r="L20">
-        <v>4685380.681094596</v>
+        <v>4183251.635494259</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -2009,7 +2030,7 @@
         <v>6.18640414507772</v>
       </c>
       <c r="E21" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="F21">
         <v>75</v>
@@ -2030,7 +2051,7 @@
         <v>41.4</v>
       </c>
       <c r="L21">
-        <v>4289921.74677372</v>
+        <v>5000341.044117969</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -2044,22 +2065,22 @@
         <v>22113</v>
       </c>
       <c r="D22">
-        <v>7.307129533678759</v>
+        <v>7.223863636363639</v>
       </c>
       <c r="E22" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="F22">
         <v>75</v>
       </c>
       <c r="G22">
-        <v>402397.6292133929</v>
+        <v>491530.2935203245</v>
       </c>
       <c r="H22">
         <v>35112131.13005736</v>
       </c>
       <c r="I22">
-        <v>256568890.3708435</v>
+        <v>253645247.2656531</v>
       </c>
       <c r="J22">
         <v>100</v>
@@ -2068,7 +2089,7 @@
         <v>48.90000000000001</v>
       </c>
       <c r="L22">
-        <v>4466301.444171549</v>
+        <v>4710325.492274638</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -2085,7 +2106,7 @@
         <v>4.771590909090911</v>
       </c>
       <c r="E23" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="F23">
         <v>80</v>
@@ -2106,7 +2127,7 @@
         <v>32.30000000000001</v>
       </c>
       <c r="L23">
-        <v>3665383.563029062</v>
+        <v>4260545.279819391</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -2123,7 +2144,7 @@
         <v>1.935227272727271</v>
       </c>
       <c r="E24" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="F24">
         <v>80</v>
@@ -2135,7 +2156,7 @@
         <v>35261419.93911113</v>
       </c>
       <c r="I24">
-        <v>68238861.54125704</v>
+        <v>68238861.54125705</v>
       </c>
       <c r="J24">
         <v>100</v>
@@ -2144,7 +2165,7 @@
         <v>13.09999999999999</v>
       </c>
       <c r="L24">
-        <v>2946266.794435292</v>
+        <v>3424662.894964906</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -2161,13 +2182,13 @@
         <v>11.52</v>
       </c>
       <c r="E25" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="F25">
         <v>80</v>
       </c>
       <c r="G25">
-        <v>801035.0141948109</v>
+        <v>617604.1836526247</v>
       </c>
       <c r="H25">
         <v>35261419.93911113</v>
@@ -2179,10 +2200,10 @@
         <v>100</v>
       </c>
       <c r="K25">
-        <v>155.2000000000001</v>
+        <v>77.09292649098477</v>
       </c>
       <c r="L25">
-        <v>5273515.054654035</v>
+        <v>8022471.696007755</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -2196,10 +2217,10 @@
         <v>28237</v>
       </c>
       <c r="D26">
-        <v>8.203709844559583</v>
+        <v>8.203709844559585</v>
       </c>
       <c r="E26" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="F26">
         <v>80</v>
@@ -2211,16 +2232,16 @@
         <v>35261419.93911113</v>
       </c>
       <c r="I26">
-        <v>289274457.8876355</v>
+        <v>289274457.8876356</v>
       </c>
       <c r="J26">
         <v>100</v>
       </c>
       <c r="K26">
-        <v>54.89999999999998</v>
+        <v>54.9</v>
       </c>
       <c r="L26">
-        <v>4593162.336777735</v>
+        <v>5353798.859421938</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -2237,7 +2258,7 @@
         <v>3.973863636363635</v>
       </c>
       <c r="E27" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="F27">
         <v>80</v>
@@ -2258,7 +2279,7 @@
         <v>26.89999999999999</v>
       </c>
       <c r="L27">
-        <v>3506650.390632065</v>
+        <v>4076038.022453973</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -2275,13 +2296,13 @@
         <v>11.52</v>
       </c>
       <c r="E28" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="F28">
         <v>100</v>
       </c>
       <c r="G28">
-        <v>612153.4459508199</v>
+        <v>768114.7751442149</v>
       </c>
       <c r="H28">
         <v>35849408.31499194</v>
@@ -2293,10 +2314,10 @@
         <v>100</v>
       </c>
       <c r="K28">
-        <v>79.30854271356787</v>
+        <v>77.98153846153848</v>
       </c>
       <c r="L28">
-        <v>6046567.678346199</v>
+        <v>5829531.060018688</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -2313,7 +2334,7 @@
         <v>2.4375</v>
       </c>
       <c r="E29" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="F29">
         <v>140</v>
@@ -2325,7 +2346,7 @@
         <v>36933299.30390043</v>
       </c>
       <c r="I29">
-        <v>90024917.05325732</v>
+        <v>90024917.05325729</v>
       </c>
       <c r="J29">
         <v>100</v>
@@ -2334,7 +2355,7 @@
         <v>16.5</v>
       </c>
       <c r="L29">
-        <v>3115469.701891457</v>
+        <v>3621339.896511324</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -2348,10 +2369,10 @@
         <v>30659</v>
       </c>
       <c r="D30">
-        <v>3.634090909090903</v>
+        <v>3.634090909090908</v>
       </c>
       <c r="E30" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="F30">
         <v>170</v>
@@ -2363,16 +2384,16 @@
         <v>37640511.58399763</v>
       </c>
       <c r="I30">
-        <v>136789040.9609366</v>
+        <v>136789040.9609368</v>
       </c>
       <c r="J30">
         <v>100</v>
       </c>
       <c r="K30">
-        <v>24.59999999999996</v>
+        <v>24.59999999999999</v>
       </c>
       <c r="L30">
-        <v>3431616.232505888</v>
+        <v>3988820.294013698</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -2383,34 +2404,34 @@
         <v>113</v>
       </c>
       <c r="C31">
-        <v>49124</v>
+        <v>49086</v>
       </c>
       <c r="D31">
-        <v>2.156818181818181</v>
+        <v>1.624999999999999</v>
       </c>
       <c r="E31" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="F31">
         <v>180</v>
       </c>
       <c r="G31">
-        <v>150462.8831150383</v>
+        <v>113667.1290495303</v>
       </c>
       <c r="H31">
         <v>37855437.77268496</v>
       </c>
       <c r="I31">
-        <v>81647296.46881369</v>
+        <v>61515086.38061304</v>
       </c>
       <c r="J31">
         <v>100</v>
       </c>
       <c r="K31">
-        <v>14.6</v>
+        <v>10.99999999999999</v>
       </c>
       <c r="L31">
-        <v>3024585.102161352</v>
+        <v>3282881.485281148</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -2421,34 +2442,34 @@
         <v>114</v>
       </c>
       <c r="C32">
-        <v>49525</v>
+        <v>49124</v>
       </c>
       <c r="D32">
-        <v>11.52</v>
+        <v>2.156818181818181</v>
       </c>
       <c r="E32" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="F32">
         <v>180</v>
       </c>
       <c r="G32">
-        <v>612153.4459508199</v>
+        <v>150462.8831150383</v>
       </c>
       <c r="H32">
         <v>37855437.77268496</v>
       </c>
       <c r="I32">
-        <v>436094643.1413309</v>
+        <v>81647296.46881369</v>
       </c>
       <c r="J32">
         <v>100</v>
       </c>
       <c r="K32">
-        <v>79.30854271356787</v>
+        <v>14.6</v>
       </c>
       <c r="L32">
-        <v>5823166.995898143</v>
+        <v>3515698.032370814</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -2459,34 +2480,34 @@
         <v>115</v>
       </c>
       <c r="C33">
-        <v>49536</v>
+        <v>49477</v>
       </c>
       <c r="D33">
-        <v>2.201136363636365</v>
+        <v>1.595454545454544</v>
       </c>
       <c r="E33" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="F33">
         <v>180</v>
       </c>
       <c r="G33">
-        <v>153520.3307989783</v>
+        <v>111617.1376495814</v>
       </c>
       <c r="H33">
         <v>37855437.77268496</v>
       </c>
       <c r="I33">
-        <v>83324980.64283049</v>
+        <v>60396630.26460185</v>
       </c>
       <c r="J33">
         <v>100</v>
       </c>
       <c r="K33">
-        <v>14.90000000000001</v>
+        <v>10.79999999999999</v>
       </c>
       <c r="L33">
-        <v>3039509.425943215</v>
+        <v>3268336.19577872</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -2497,13 +2518,13 @@
         <v>116</v>
       </c>
       <c r="C34">
-        <v>49808</v>
+        <v>49525</v>
       </c>
       <c r="D34">
         <v>11.52</v>
       </c>
       <c r="E34" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="F34">
         <v>180</v>
@@ -2524,7 +2545,7 @@
         <v>77.98153846153848</v>
       </c>
       <c r="L34">
-        <v>4973514.536159209</v>
+        <v>5614149.162975817</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -2535,34 +2556,34 @@
         <v>117</v>
       </c>
       <c r="C35">
-        <v>49824</v>
+        <v>49536</v>
       </c>
       <c r="D35">
-        <v>5.687500000000001</v>
+        <v>2.201136363636365</v>
       </c>
       <c r="E35" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="F35">
         <v>180</v>
       </c>
       <c r="G35">
-        <v>389884.387080091</v>
+        <v>153520.3307989783</v>
       </c>
       <c r="H35">
         <v>37855437.77268496</v>
       </c>
       <c r="I35">
-        <v>215302802.3321458</v>
+        <v>83324980.64283049</v>
       </c>
       <c r="J35">
         <v>100</v>
       </c>
       <c r="K35">
-        <v>38.50000000000001</v>
+        <v>14.90000000000001</v>
       </c>
       <c r="L35">
-        <v>3824493.385265881</v>
+        <v>3533045.673115612</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -2573,34 +2594,34 @@
         <v>118</v>
       </c>
       <c r="C36">
-        <v>49824</v>
+        <v>49808</v>
       </c>
       <c r="D36">
-        <v>2.363636363636363</v>
+        <v>11.52</v>
       </c>
       <c r="E36" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="F36">
         <v>180</v>
       </c>
       <c r="G36">
-        <v>164719.3634241114</v>
+        <v>612153.4459508199</v>
       </c>
       <c r="H36">
         <v>37855437.77268496</v>
       </c>
       <c r="I36">
-        <v>89476489.2808917</v>
+        <v>436094643.1413309</v>
       </c>
       <c r="J36">
         <v>100</v>
       </c>
       <c r="K36">
-        <v>15.99999999999999</v>
+        <v>79.30854271356787</v>
       </c>
       <c r="L36">
-        <v>3092355.773228031</v>
+        <v>6941555.276767245</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -2611,34 +2632,34 @@
         <v>119</v>
       </c>
       <c r="C37">
-        <v>31226</v>
+        <v>49824</v>
       </c>
       <c r="D37">
-        <v>2.422727272727272</v>
+        <v>5.6875</v>
       </c>
       <c r="E37" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="F37">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="G37">
-        <v>168787.2243370978</v>
+        <v>389884.387080091</v>
       </c>
       <c r="H37">
-        <v>38060293.37896816</v>
+        <v>37855437.77268496</v>
       </c>
       <c r="I37">
-        <v>92209710.7772274</v>
+        <v>215302802.3321457</v>
       </c>
       <c r="J37">
         <v>100</v>
       </c>
       <c r="K37">
-        <v>16.4</v>
+        <v>38.5</v>
       </c>
       <c r="L37">
-        <v>3110889.813225406</v>
+        <v>4445490.345034822</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -2649,34 +2670,34 @@
         <v>120</v>
       </c>
       <c r="C38">
-        <v>31319</v>
+        <v>49824</v>
       </c>
       <c r="D38">
-        <v>9.114772727272728</v>
+        <v>2.324087591240875</v>
       </c>
       <c r="E38" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="F38">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="G38">
-        <v>614621.4706630026</v>
+        <v>130998.8478980427</v>
       </c>
       <c r="H38">
-        <v>38060293.37896816</v>
+        <v>37855437.77268496</v>
       </c>
       <c r="I38">
-        <v>346910924.0826178</v>
+        <v>87979353.18848825</v>
       </c>
       <c r="J38">
         <v>100</v>
       </c>
       <c r="K38">
-        <v>61.7</v>
+        <v>16</v>
       </c>
       <c r="L38">
-        <v>4286880.992309345</v>
+        <v>4316014.033784165</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -2687,34 +2708,34 @@
         <v>121</v>
       </c>
       <c r="C39">
-        <v>31789</v>
+        <v>31171</v>
       </c>
       <c r="D39">
-        <v>6.216290155440415</v>
+        <v>1.787500000000001</v>
       </c>
       <c r="E39" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="F39">
         <v>190</v>
       </c>
       <c r="G39">
-        <v>344753.3335028072</v>
+        <v>124931.1729695994</v>
       </c>
       <c r="H39">
         <v>38060293.37896816</v>
       </c>
       <c r="I39">
-        <v>236593827.0448538</v>
+        <v>68032774.41490564</v>
       </c>
       <c r="J39">
         <v>100</v>
       </c>
       <c r="K39">
-        <v>41.6</v>
+        <v>12.10000000000001</v>
       </c>
       <c r="L39">
-        <v>4294927.860967864</v>
+        <v>3359481.349733927</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -2725,34 +2746,34 @@
         <v>122</v>
       </c>
       <c r="C40">
-        <v>38239</v>
+        <v>31226</v>
       </c>
       <c r="D40">
-        <v>11.52</v>
+        <v>2.422727272727272</v>
       </c>
       <c r="E40" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="F40">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="G40">
-        <v>801035.0141948109</v>
+        <v>168787.2243370978</v>
       </c>
       <c r="H40">
-        <v>38255392.02166688</v>
+        <v>38060293.37896816</v>
       </c>
       <c r="I40">
-        <v>440702116.0896025</v>
+        <v>92209710.7772274</v>
       </c>
       <c r="J40">
         <v>100</v>
       </c>
       <c r="K40">
-        <v>155.2000000000001</v>
+        <v>16.4</v>
       </c>
       <c r="L40">
-        <v>5273515.054654035</v>
+        <v>3616016.354594713</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -2763,34 +2784,34 @@
         <v>123</v>
       </c>
       <c r="C41">
-        <v>31061</v>
+        <v>31319</v>
       </c>
       <c r="D41">
-        <v>4.889772727272737</v>
+        <v>9.114772727272729</v>
       </c>
       <c r="E41" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="F41">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="G41">
-        <v>336511.4001062157</v>
+        <v>614621.4706630026</v>
       </c>
       <c r="H41">
-        <v>38441090.93970785</v>
+        <v>38060293.37896816</v>
       </c>
       <c r="I41">
-        <v>187968198.0835945</v>
+        <v>346910924.0826179</v>
       </c>
       <c r="J41">
         <v>100</v>
       </c>
       <c r="K41">
-        <v>33.10000000000007</v>
+        <v>61.70000000000002</v>
       </c>
       <c r="L41">
-        <v>3687149.882920415</v>
+        <v>4982957.516685472</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -2801,34 +2822,34 @@
         <v>124</v>
       </c>
       <c r="C42">
-        <v>33106</v>
+        <v>31789</v>
       </c>
       <c r="D42">
-        <v>3.412500000000001</v>
+        <v>6.145454545454548</v>
       </c>
       <c r="E42" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="F42">
-        <v>230</v>
+        <v>190</v>
       </c>
       <c r="G42">
-        <v>236568.9630487722</v>
+        <v>420339.1934723008</v>
       </c>
       <c r="H42">
-        <v>38785844.374162</v>
+        <v>38060293.37896816</v>
       </c>
       <c r="I42">
-        <v>132356693.9268279</v>
+        <v>233897802.9471135</v>
       </c>
       <c r="J42">
         <v>100</v>
       </c>
       <c r="K42">
-        <v>23.10000000000001</v>
+        <v>41.60000000000002</v>
       </c>
       <c r="L42">
-        <v>3379765.097364126</v>
+        <v>4529588.61910183</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -2839,34 +2860,34 @@
         <v>125</v>
       </c>
       <c r="C43">
-        <v>33609</v>
+        <v>38239</v>
       </c>
       <c r="D43">
-        <v>5.635912408759122</v>
+        <v>11.52</v>
       </c>
       <c r="E43" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="F43">
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="G43">
-        <v>310874.993281192</v>
+        <v>801035.0141948109</v>
       </c>
       <c r="H43">
-        <v>38785844.374162</v>
+        <v>38255392.02166688</v>
       </c>
       <c r="I43">
-        <v>218593621.5925398</v>
+        <v>440702116.0896025</v>
       </c>
       <c r="J43">
         <v>100</v>
       </c>
       <c r="K43">
-        <v>38.79999999999999</v>
+        <v>155.2000000000001</v>
       </c>
       <c r="L43">
-        <v>4619667.836848523</v>
+        <v>7703421.965571916</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -2877,34 +2898,34 @@
         <v>126</v>
       </c>
       <c r="C44">
-        <v>38372</v>
+        <v>31061</v>
       </c>
       <c r="D44">
-        <v>6.580701271262555</v>
+        <v>4.946134715025906</v>
       </c>
       <c r="E44" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="F44">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="G44">
-        <v>369332.0210697243</v>
+        <v>276594.1657165497</v>
       </c>
       <c r="H44">
-        <v>38785844.374162</v>
+        <v>38441090.93970785</v>
       </c>
       <c r="I44">
-        <v>255238055.3800395</v>
+        <v>190134814.3803568</v>
       </c>
       <c r="J44">
         <v>100</v>
       </c>
       <c r="K44">
-        <v>44.03867355595261</v>
+        <v>33.09999999999999</v>
       </c>
       <c r="L44">
-        <v>4370284.483374606</v>
+        <v>4736787.674254571</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -2915,34 +2936,34 @@
         <v>127</v>
       </c>
       <c r="C45">
-        <v>38723</v>
+        <v>33106</v>
       </c>
       <c r="D45">
-        <v>4.880583941605832</v>
+        <v>3.412499999999952</v>
       </c>
       <c r="E45" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="F45">
         <v>230</v>
       </c>
       <c r="G45">
-        <v>270532.0601478429</v>
+        <v>236568.9630487722</v>
       </c>
       <c r="H45">
         <v>38785844.374162</v>
       </c>
       <c r="I45">
-        <v>189297569.2141579</v>
+        <v>132356693.9268259</v>
       </c>
       <c r="J45">
         <v>100</v>
       </c>
       <c r="K45">
-        <v>33.59999999999995</v>
+        <v>23.09999999999967</v>
       </c>
       <c r="L45">
-        <v>4461568.626817144</v>
+        <v>3928549.900674851</v>
       </c>
     </row>
     <row r="46" spans="1:12">
@@ -2953,34 +2974,34 @@
         <v>128</v>
       </c>
       <c r="C46">
-        <v>39596</v>
+        <v>33332</v>
       </c>
       <c r="D46">
-        <v>11.52</v>
+        <v>3.811363636363637</v>
       </c>
       <c r="E46" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="F46">
         <v>230</v>
       </c>
       <c r="G46">
-        <v>801035.0141948109</v>
+        <v>263696.5242697849</v>
       </c>
       <c r="H46">
         <v>38785844.374162</v>
       </c>
       <c r="I46">
-        <v>446812927.1903462</v>
+        <v>147826956.8533402</v>
       </c>
       <c r="J46">
         <v>100</v>
       </c>
       <c r="K46">
-        <v>155.2</v>
+        <v>25.80000000000001</v>
       </c>
       <c r="L46">
-        <v>5273515.054654035</v>
+        <v>4035061.363361877</v>
       </c>
     </row>
     <row r="47" spans="1:12">
@@ -2991,34 +3012,262 @@
         <v>129</v>
       </c>
       <c r="C47">
-        <v>58710</v>
+        <v>33609</v>
       </c>
       <c r="D47">
-        <v>10.98116777456054</v>
+        <v>5.731818181818184</v>
       </c>
       <c r="E47" t="s">
+        <v>136</v>
+      </c>
+      <c r="F47">
+        <v>230</v>
+      </c>
+      <c r="G47">
+        <v>392837.4968233245</v>
+      </c>
+      <c r="H47">
+        <v>38785844.374162</v>
+      </c>
+      <c r="I47">
+        <v>222313407.9809923</v>
+      </c>
+      <c r="J47">
+        <v>100</v>
+      </c>
+      <c r="K47">
+        <v>38.80000000000002</v>
+      </c>
+      <c r="L47">
+        <v>4453848.625282167</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
         <v>130</v>
       </c>
-      <c r="F47">
+      <c r="C48">
+        <v>38372</v>
+      </c>
+      <c r="D48">
+        <v>6.603409090909089</v>
+      </c>
+      <c r="E48" t="s">
+        <v>136</v>
+      </c>
+      <c r="F48">
+        <v>230</v>
+      </c>
+      <c r="G48">
+        <v>450660.4973793401</v>
+      </c>
+      <c r="H48">
+        <v>38785844.374162</v>
+      </c>
+      <c r="I48">
+        <v>256118797.3389265</v>
+      </c>
+      <c r="J48">
+        <v>100</v>
+      </c>
+      <c r="K48">
+        <v>44.69999999999999</v>
+      </c>
+      <c r="L48">
+        <v>4609062.479962116</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>131</v>
+      </c>
+      <c r="C49">
+        <v>38723</v>
+      </c>
+      <c r="D49">
+        <v>4.938027696133044</v>
+      </c>
+      <c r="E49" t="s">
+        <v>139</v>
+      </c>
+      <c r="F49">
+        <v>230</v>
+      </c>
+      <c r="G49">
+        <v>280634.940059881</v>
+      </c>
+      <c r="H49">
+        <v>38785844.374162</v>
+      </c>
+      <c r="I49">
+        <v>191525573.737518</v>
+      </c>
+      <c r="J49">
+        <v>100</v>
+      </c>
+      <c r="K49">
+        <v>33.04574706496802</v>
+      </c>
+      <c r="L49">
+        <v>4754005.158277944</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
+        <v>132</v>
+      </c>
+      <c r="C50">
+        <v>39596</v>
+      </c>
+      <c r="D50">
+        <v>11.52</v>
+      </c>
+      <c r="E50" t="s">
+        <v>140</v>
+      </c>
+      <c r="F50">
+        <v>230</v>
+      </c>
+      <c r="G50">
+        <v>801035.0141948109</v>
+      </c>
+      <c r="H50">
+        <v>38785844.374162</v>
+      </c>
+      <c r="I50">
+        <v>446812927.1903463</v>
+      </c>
+      <c r="J50">
+        <v>100</v>
+      </c>
+      <c r="K50">
+        <v>155.2000000000001</v>
+      </c>
+      <c r="L50">
+        <v>5573047.833346938</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12">
+      <c r="A51" s="1">
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
+        <v>133</v>
+      </c>
+      <c r="C51">
+        <v>39326</v>
+      </c>
+      <c r="D51">
+        <v>3.767045454545453</v>
+      </c>
+      <c r="E51" t="s">
+        <v>136</v>
+      </c>
+      <c r="F51">
         <v>250</v>
       </c>
-      <c r="G47">
-        <v>768114.7751442149</v>
-      </c>
-      <c r="H47">
+      <c r="G51">
+        <v>260687.6193448816</v>
+      </c>
+      <c r="H51">
         <v>39097761.98338025</v>
       </c>
-      <c r="I47">
-        <v>429339083.9493334</v>
-      </c>
-      <c r="J47">
-        <v>100</v>
-      </c>
-      <c r="K47">
-        <v>74.33405878164058</v>
-      </c>
-      <c r="L47">
-        <v>4573255.840545377</v>
+      <c r="I51">
+        <v>147283046.5623926</v>
+      </c>
+      <c r="J51">
+        <v>100</v>
+      </c>
+      <c r="K51">
+        <v>25.49999999999999</v>
+      </c>
+      <c r="L51">
+        <v>4023656.505734837</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+      <c r="B52" t="s">
+        <v>134</v>
+      </c>
+      <c r="C52">
+        <v>37355</v>
+      </c>
+      <c r="D52">
+        <v>7.571134020618555</v>
+      </c>
+      <c r="E52" t="s">
+        <v>140</v>
+      </c>
+      <c r="F52">
+        <v>290</v>
+      </c>
+      <c r="G52">
+        <v>535696.0892835769</v>
+      </c>
+      <c r="H52">
+        <v>39635749.05499732</v>
+      </c>
+      <c r="I52">
+        <v>300087568.1029899</v>
+      </c>
+      <c r="J52">
+        <v>100</v>
+      </c>
+      <c r="K52">
+        <v>102</v>
+      </c>
+      <c r="L52">
+        <v>4764152.29680264</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12">
+      <c r="A53" s="1">
+        <v>51</v>
+      </c>
+      <c r="B53" t="s">
+        <v>135</v>
+      </c>
+      <c r="C53">
+        <v>58097</v>
+      </c>
+      <c r="D53">
+        <v>0.8204537576519795</v>
+      </c>
+      <c r="E53" t="s">
+        <v>136</v>
+      </c>
+      <c r="F53">
+        <v>290</v>
+      </c>
+      <c r="G53">
+        <v>110591.9127653434</v>
+      </c>
+      <c r="H53">
+        <v>39635749.05499732</v>
+      </c>
+      <c r="I53">
+        <v>32519299.24952344</v>
+      </c>
+      <c r="J53">
+        <v>100</v>
+      </c>
+      <c r="K53">
+        <v>5.553840821028784</v>
+      </c>
+      <c r="L53">
+        <v>3260986.861328017</v>
       </c>
     </row>
   </sheetData>

</xml_diff>